<commit_message>
Update on 2/28/2025 at 11:43pm
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Dropbox/S2P Datasets Shared Folder/MLTC_MMC_NH_data/reports_drafts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5452CC-4E0C-D345-AA76-6E71B7EAA8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F558D929-3845-6344-8333-38F5816C1C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Average Annual Growth Rates</t>
   </si>
   <si>
-    <t>Enter Projected Growth Rate</t>
-  </si>
-  <si>
     <t>Data  Type</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Growth Trends</t>
   </si>
   <si>
-    <t>State Share Spending</t>
-  </si>
-  <si>
     <t>Per Capita Spending</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>Enrollee Months % Growth</t>
   </si>
   <si>
-    <t>State Share Spending Annual Change %</t>
-  </si>
-  <si>
     <t>Average Annual Per Capita Spending % Growth</t>
   </si>
   <si>
@@ -209,9 +200,6 @@
     <t>State Spending Annual Change (Millions)</t>
   </si>
   <si>
-    <t>---</t>
-  </si>
-  <si>
     <t>FY25</t>
   </si>
   <si>
@@ -240,9 +228,6 @@
   </si>
   <si>
     <t>FY26 Growth Assumptions</t>
-  </si>
-  <si>
-    <t>Enter Projected Growth Rates</t>
   </si>
   <si>
     <t>Definitions</t>
@@ -505,29 +490,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>State Share Spending Annual Change %:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> The percentage change in the State’s share of Medicaid managed long term care spending compared to the prior fiscal year.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Average Annual Spending per Enrollee:</t>
     </r>
     <r>
@@ -565,6 +527,44 @@
   </si>
   <si>
     <t>Calculations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>State Spending Annual Change %:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The percentage change in the State’s share of Medicaid managed long term care spending compared to the prior fiscal year.</t>
+    </r>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>FY27 (Forecast)</t>
+  </si>
+  <si>
+    <t>FY28 (Forecast)</t>
+  </si>
+  <si>
+    <t>FY29 (Forecast)</t>
+  </si>
+  <si>
+    <t>You can forecast projected enrollment and State spending by changing the two inputs below:</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1059,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1072,7 +1072,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="7" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="4" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="7" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="3" borderId="18" xfId="7" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1088,11 +1087,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1113,22 +1110,10 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="8" fillId="3" borderId="4" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="8" fillId="3" borderId="22" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1138,11 +1123,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="4" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="14" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1158,6 +1150,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="3" applyFont="1"/>
@@ -3629,10 +3630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92772258-4AC4-6B47-AC5E-CDE7A2651A1C}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3644,1042 +3645,1216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+    </row>
+    <row r="2" spans="1:16" s="12" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+    </row>
+    <row r="3" spans="1:16" s="21" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="25">
+        <f t="shared" ref="C4:C7" si="0">C5*(1+$H$27)</f>
+        <v>687956.48317221063</v>
+      </c>
+      <c r="D4" s="25">
+        <f t="shared" ref="D4:D7" si="1">D5*(1+$H$27)</f>
+        <v>155309.77279023294</v>
+      </c>
+      <c r="E4" s="25">
+        <f t="shared" ref="E4:E6" si="2">E5*(1+$H$27)</f>
+        <v>4567992.0330596119</v>
+      </c>
+      <c r="F4" s="25">
+        <f>G4*12</f>
+        <v>5411252.7154215034</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" ref="G4:G6" si="3">G5*(1+$H$27)</f>
+        <v>450937.7262851253</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="25">
+        <f>F4-F5</f>
+        <v>347381.56118090451</v>
+      </c>
+      <c r="J4" s="27">
+        <f t="shared" ref="J4:J6" si="4">I4/F5</f>
+        <v>6.8599999999999883E-2</v>
+      </c>
+      <c r="K4" s="34">
+        <f t="shared" ref="K4:K6" si="5">N4*G4</f>
+        <v>18842101634.946587</v>
+      </c>
+      <c r="L4" s="34">
+        <f t="shared" ref="L4:L6" si="6">K4-K5</f>
+        <v>1234241283.5088005</v>
+      </c>
+      <c r="M4" s="28">
+        <f t="shared" ref="M4:M6" si="7">L4/K5</f>
+        <v>7.0096040000000193E-2</v>
+      </c>
+      <c r="N4" s="26">
+        <f t="shared" ref="N4:N6" si="8">(1+P4)*N5</f>
+        <v>41784.265402165162</v>
+      </c>
+      <c r="O4" s="26">
+        <f t="shared" ref="O4:O6" si="9">N4-N5</f>
+        <v>58.416188898576365</v>
+      </c>
+      <c r="P4" s="27">
+        <f t="shared" ref="P4:P6" si="10">$H$29</f>
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="25">
+        <f t="shared" si="0"/>
+        <v>643792.32937695179</v>
+      </c>
+      <c r="D5" s="25">
+        <f t="shared" si="1"/>
+        <v>145339.48417577479</v>
+      </c>
+      <c r="E5" s="25">
+        <f t="shared" si="2"/>
+        <v>4274744.5564847579</v>
+      </c>
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F8" si="11">G5*12</f>
+        <v>5063871.1542405989</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="3"/>
+        <v>421989.2628533832</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="25">
+        <f>F5-F6</f>
+        <v>325081.00428682938</v>
+      </c>
+      <c r="J5" s="27">
+        <f t="shared" si="4"/>
+        <v>6.8600000000000161E-2</v>
+      </c>
+      <c r="K5" s="34">
+        <f>N5*G5</f>
+        <v>17607860351.437786</v>
+      </c>
+      <c r="L5" s="34">
+        <f t="shared" si="6"/>
+        <v>1153393001.5373173</v>
+      </c>
+      <c r="M5" s="28">
+        <f t="shared" si="7"/>
+        <v>7.0096039999999998E-2</v>
+      </c>
+      <c r="N5" s="26">
+        <f t="shared" si="8"/>
+        <v>41725.849213266585</v>
+      </c>
+      <c r="O5" s="26">
+        <f t="shared" si="9"/>
+        <v>58.334520569776942</v>
+      </c>
+      <c r="P5" s="27">
+        <f t="shared" si="10"/>
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="25">
+        <f t="shared" si="0"/>
+        <v>602463.34397992864</v>
+      </c>
+      <c r="D6" s="25">
+        <f t="shared" si="1"/>
+        <v>136009.24964979861</v>
+      </c>
+      <c r="E6" s="25">
+        <f t="shared" si="2"/>
+        <v>4000322.437286878</v>
+      </c>
+      <c r="F6" s="25">
+        <f t="shared" si="11"/>
+        <v>4738790.1499537695</v>
+      </c>
+      <c r="G6" s="25">
+        <f t="shared" si="3"/>
+        <v>394899.17916281417</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="25">
+        <f t="shared" ref="I6" si="12">F6-F7</f>
+        <v>304212.0571652893</v>
+      </c>
+      <c r="J6" s="27">
+        <f t="shared" si="4"/>
+        <v>6.8599999999999897E-2</v>
+      </c>
+      <c r="K6" s="34">
+        <f t="shared" si="5"/>
+        <v>16454467349.900469</v>
+      </c>
+      <c r="L6" s="34">
+        <f t="shared" si="6"/>
+        <v>1077840640.8618431</v>
+      </c>
+      <c r="M6" s="28">
+        <f t="shared" si="7"/>
+        <v>7.0096040000000207E-2</v>
+      </c>
+      <c r="N6" s="26">
+        <f t="shared" si="8"/>
+        <v>41667.514692696808</v>
+      </c>
+      <c r="O6" s="26">
+        <f t="shared" si="9"/>
+        <v>58.252966416795971</v>
+      </c>
+      <c r="P6" s="27">
+        <f t="shared" si="10"/>
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25">
+        <f t="shared" si="0"/>
+        <v>563787.52010100009</v>
+      </c>
+      <c r="D7" s="25">
+        <f t="shared" si="1"/>
+        <v>127277.98020756</v>
+      </c>
+      <c r="E7" s="25">
+        <f>E8*(1+$H$27)</f>
+        <v>3743517.1601037602</v>
+      </c>
+      <c r="F7" s="25">
+        <f t="shared" si="11"/>
+        <v>4434578.0927884802</v>
+      </c>
+      <c r="G7" s="25">
+        <f>G8*(1+$H$27)</f>
+        <v>369548.17439904</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="25">
+        <f>F7-F8</f>
+        <v>284682.81598848011</v>
+      </c>
+      <c r="J7" s="27">
+        <f>I7/F8</f>
+        <v>6.8600000000000022E-2</v>
+      </c>
+      <c r="K7" s="34">
+        <f>N7*G7</f>
+        <v>15376626709.038626</v>
+      </c>
+      <c r="L7" s="34">
+        <f>K7-K8</f>
+        <v>1007237295.1327267</v>
+      </c>
+      <c r="M7" s="28">
+        <f>L7/K8</f>
+        <v>7.0096040000000151E-2</v>
+      </c>
+      <c r="N7" s="26">
+        <f>(1+P7)*N8</f>
+        <v>41609.261726280012</v>
+      </c>
+      <c r="O7" s="26">
+        <f>N7-N8</f>
+        <v>58.171526280006219</v>
+      </c>
+      <c r="P7" s="27">
+        <f>$H$29</f>
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25">
+        <f t="shared" ref="C8:D8" si="13">C10*(1+$H$27)</f>
+        <v>527594.53500000003</v>
+      </c>
+      <c r="D8" s="25">
+        <f t="shared" si="13"/>
+        <v>119107.2246</v>
+      </c>
+      <c r="E8" s="25">
+        <f>E10*(1+$H$27)</f>
+        <v>3503197.7916000001</v>
+      </c>
+      <c r="F8" s="25">
+        <f t="shared" si="11"/>
+        <v>4149895.2768000001</v>
+      </c>
+      <c r="G8" s="25">
+        <f>G10*(1+$H$27)</f>
+        <v>345824.60639999999</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="25">
+        <f>F8-F10</f>
+        <v>266403.27680000011</v>
+      </c>
+      <c r="J8" s="28">
+        <f>I8/F10</f>
+        <v>6.8598899341108494E-2</v>
+      </c>
+      <c r="K8" s="34">
+        <f>N8*G8</f>
+        <v>14369389413.905899</v>
+      </c>
+      <c r="L8" s="34">
+        <f>K8-K10</f>
+        <v>941389413.90589905</v>
+      </c>
+      <c r="M8" s="28">
+        <f>L8/K10</f>
+        <v>7.0106450246194454E-2</v>
+      </c>
+      <c r="N8" s="26">
+        <f>(1+P8)*N10</f>
+        <v>41551.090200000006</v>
+      </c>
+      <c r="O8" s="26">
+        <f>N8-N10</f>
+        <v>58.090200000006007</v>
+      </c>
+      <c r="P8" s="27">
+        <f>$H$29</f>
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="24">
+        <v>3</v>
+      </c>
+      <c r="C9" s="25">
+        <v>142671</v>
+      </c>
+      <c r="D9" s="25">
+        <v>28363</v>
+      </c>
+      <c r="E9" s="25">
+        <v>871911</v>
+      </c>
+      <c r="F9" s="25">
+        <v>1042945</v>
+      </c>
+      <c r="G9" s="25">
+        <v>347648</v>
+      </c>
+      <c r="H9" s="25">
+        <v>350874</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="O9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="24">
+        <v>12</v>
+      </c>
+      <c r="C10" s="25">
+        <v>493725</v>
+      </c>
+      <c r="D10" s="25">
+        <v>111461</v>
+      </c>
+      <c r="E10" s="25">
+        <v>3278306</v>
+      </c>
+      <c r="F10" s="25">
+        <v>3883492</v>
+      </c>
+      <c r="G10" s="25">
+        <v>323624</v>
+      </c>
+      <c r="H10" s="25">
+        <v>331699</v>
+      </c>
+      <c r="I10" s="25">
+        <v>358704</v>
+      </c>
+      <c r="J10" s="28">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K10" s="34">
+        <v>13428000000</v>
+      </c>
+      <c r="L10" s="34">
+        <v>1686000000</v>
+      </c>
+      <c r="M10" s="28">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="N10" s="26">
+        <v>41493</v>
+      </c>
+      <c r="O10" s="26">
+        <v>1517</v>
+      </c>
+      <c r="P10" s="28">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="24">
+        <v>12</v>
+      </c>
+      <c r="C11" s="25">
+        <v>416349</v>
+      </c>
+      <c r="D11" s="25">
+        <v>91952</v>
+      </c>
+      <c r="E11" s="25">
+        <v>3016487</v>
+      </c>
+      <c r="F11" s="25">
+        <v>3524788</v>
+      </c>
+      <c r="G11" s="25">
+        <v>293732</v>
+      </c>
+      <c r="H11" s="25">
+        <v>299174</v>
+      </c>
+      <c r="I11" s="25">
+        <v>187451</v>
+      </c>
+      <c r="J11" s="28">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="K11" s="34">
+        <v>11742000000</v>
+      </c>
+      <c r="L11" s="34">
+        <v>115000000</v>
+      </c>
+      <c r="M11" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="N11" s="26">
+        <v>39975</v>
+      </c>
+      <c r="O11" s="26">
+        <v>-1832</v>
+      </c>
+      <c r="P11" s="28">
+        <v>-4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="24">
+        <v>12</v>
+      </c>
+      <c r="C12" s="25">
+        <v>356677</v>
+      </c>
+      <c r="D12" s="25">
+        <v>67089</v>
+      </c>
+      <c r="E12" s="25">
+        <v>2913571</v>
+      </c>
+      <c r="F12" s="25">
+        <v>3337337</v>
+      </c>
+      <c r="G12" s="25">
+        <v>278111</v>
+      </c>
+      <c r="H12" s="25">
+        <v>280507</v>
+      </c>
+      <c r="I12" s="25">
+        <v>84633</v>
+      </c>
+      <c r="J12" s="28">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="K12" s="34">
+        <v>11627000000</v>
+      </c>
+      <c r="L12" s="34">
+        <v>979000000</v>
+      </c>
+      <c r="M12" s="28">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="N12" s="26">
+        <v>41807</v>
+      </c>
+      <c r="O12" s="26">
+        <v>2524</v>
+      </c>
+      <c r="P12" s="28">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="24">
+        <v>12</v>
+      </c>
+      <c r="C13" s="25">
+        <v>271573</v>
+      </c>
+      <c r="D13" s="25">
+        <v>65494</v>
+      </c>
+      <c r="E13" s="25">
+        <v>2915637</v>
+      </c>
+      <c r="F13" s="25">
+        <v>3252704</v>
+      </c>
+      <c r="G13" s="25">
+        <v>271059</v>
+      </c>
+      <c r="H13" s="25">
+        <v>270785</v>
+      </c>
+      <c r="I13" s="25">
+        <v>61573</v>
+      </c>
+      <c r="J13" s="28">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K13" s="34">
+        <v>10648000000</v>
+      </c>
+      <c r="L13" s="34">
+        <v>-539000000</v>
+      </c>
+      <c r="M13" s="28">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="N13" s="26">
+        <v>39283</v>
+      </c>
+      <c r="O13" s="26">
+        <v>-2785</v>
+      </c>
+      <c r="P13" s="28">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="24">
+        <v>12</v>
+      </c>
+      <c r="C14" s="25">
+        <v>211114</v>
+      </c>
+      <c r="D14" s="25">
+        <v>68522</v>
+      </c>
+      <c r="E14" s="25">
+        <v>2911495</v>
+      </c>
+      <c r="F14" s="25">
+        <v>3191131</v>
+      </c>
+      <c r="G14" s="25">
+        <v>265928</v>
+      </c>
+      <c r="H14" s="25">
+        <v>272758</v>
+      </c>
+      <c r="I14" s="25">
+        <v>391265</v>
+      </c>
+      <c r="J14" s="28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K14" s="34">
+        <v>11187000000</v>
+      </c>
+      <c r="L14" s="34">
+        <v>1517000000</v>
+      </c>
+      <c r="M14" s="28">
+        <v>0.157</v>
+      </c>
+      <c r="N14" s="26">
+        <v>42068</v>
+      </c>
+      <c r="O14" s="26">
+        <v>623</v>
+      </c>
+      <c r="P14" s="28">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="24">
+        <v>12</v>
+      </c>
+      <c r="C15" s="25">
+        <v>146837</v>
+      </c>
+      <c r="D15" s="25">
+        <v>68314</v>
+      </c>
+      <c r="E15" s="25">
+        <v>2584715</v>
+      </c>
+      <c r="F15" s="25">
+        <v>2799866</v>
+      </c>
+      <c r="G15" s="25">
+        <v>233322</v>
+      </c>
+      <c r="H15" s="25">
+        <v>240219</v>
+      </c>
+      <c r="I15" s="25">
+        <v>359451</v>
+      </c>
+      <c r="J15" s="28">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="K15" s="34">
+        <v>9670000000</v>
+      </c>
+      <c r="L15" s="34">
+        <v>465000000</v>
+      </c>
+      <c r="M15" s="28">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="N15" s="26">
+        <v>41445</v>
+      </c>
+      <c r="O15" s="26">
+        <v>-3818</v>
+      </c>
+      <c r="P15" s="28">
+        <v>-8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="24">
+        <v>12</v>
+      </c>
+      <c r="C16" s="25">
+        <v>102280</v>
+      </c>
+      <c r="D16" s="25">
+        <v>67591</v>
+      </c>
+      <c r="E16" s="25">
+        <v>2270544</v>
+      </c>
+      <c r="F16" s="25">
+        <v>2440415</v>
+      </c>
+      <c r="G16" s="25">
+        <v>203368</v>
+      </c>
+      <c r="H16" s="25">
+        <v>210264</v>
+      </c>
+      <c r="I16" s="25">
+        <v>352109</v>
+      </c>
+      <c r="J16" s="28">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="K16" s="34">
+        <v>9205000000</v>
+      </c>
+      <c r="L16" s="34">
+        <v>921000000</v>
+      </c>
+      <c r="M16" s="28">
+        <v>0.111</v>
+      </c>
+      <c r="N16" s="26">
+        <v>45263</v>
+      </c>
+      <c r="O16" s="26">
+        <v>-2339</v>
+      </c>
+      <c r="P16" s="28">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="24">
+        <v>12</v>
+      </c>
+      <c r="C17" s="25">
+        <v>74966</v>
+      </c>
+      <c r="D17" s="25">
+        <v>66883</v>
+      </c>
+      <c r="E17" s="25">
+        <v>1946457</v>
+      </c>
+      <c r="F17" s="25">
+        <v>2088306</v>
+      </c>
+      <c r="G17" s="25">
+        <v>174026</v>
+      </c>
+      <c r="H17" s="25">
+        <v>181219</v>
+      </c>
+      <c r="I17" s="25">
+        <v>353466</v>
+      </c>
+      <c r="J17" s="28">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="K17" s="34">
+        <v>8284000000</v>
+      </c>
+      <c r="L17" s="34">
+        <v>436000000</v>
+      </c>
+      <c r="M17" s="28">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="N17" s="26">
+        <v>47602</v>
+      </c>
+      <c r="O17" s="26">
+        <v>-6683</v>
+      </c>
+      <c r="P17" s="28">
+        <v>-0.123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="24">
+        <v>12</v>
+      </c>
+      <c r="C18" s="25">
+        <v>71979</v>
+      </c>
+      <c r="D18" s="25">
+        <v>65736</v>
+      </c>
+      <c r="E18" s="25">
+        <v>1597125</v>
+      </c>
+      <c r="F18" s="25">
+        <v>1734840</v>
+      </c>
+      <c r="G18" s="25">
+        <v>144570</v>
+      </c>
+      <c r="H18" s="25">
+        <v>148887</v>
+      </c>
+      <c r="I18" s="25">
+        <v>121067</v>
+      </c>
+      <c r="J18" s="28">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K18" s="34">
+        <v>7848000000</v>
+      </c>
+      <c r="L18" s="34">
+        <v>371000000</v>
+      </c>
+      <c r="M18" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="N18" s="26">
+        <v>54285</v>
+      </c>
+      <c r="O18" s="26">
+        <v>-1314</v>
+      </c>
+      <c r="P18" s="28">
+        <v>-2.4E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="24">
+        <v>12</v>
+      </c>
+      <c r="C19" s="25">
+        <v>68552</v>
+      </c>
+      <c r="D19" s="25">
+        <v>67476</v>
+      </c>
+      <c r="E19" s="25">
+        <v>1477745</v>
+      </c>
+      <c r="F19" s="25">
+        <v>1613773</v>
+      </c>
+      <c r="G19" s="25">
+        <v>134481</v>
+      </c>
+      <c r="H19" s="25">
+        <v>138251</v>
+      </c>
+      <c r="I19" s="25">
+        <v>243287</v>
+      </c>
+      <c r="J19" s="28">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="K19" s="34">
+        <v>7477000000</v>
+      </c>
+      <c r="L19" s="34">
+        <v>3076000000</v>
+      </c>
+      <c r="M19" s="28">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="N19" s="26">
+        <v>55599</v>
+      </c>
+      <c r="O19" s="26">
+        <v>17064</v>
+      </c>
+      <c r="P19" s="28">
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="24">
+        <v>12</v>
+      </c>
+      <c r="C20" s="25">
+        <v>53408</v>
+      </c>
+      <c r="D20" s="25">
+        <v>62026</v>
+      </c>
+      <c r="E20" s="25">
+        <v>1255052</v>
+      </c>
+      <c r="F20" s="25">
+        <v>1370486</v>
+      </c>
+      <c r="G20" s="25">
+        <v>114207</v>
+      </c>
+      <c r="H20" s="25">
+        <v>122486</v>
+      </c>
+      <c r="I20" s="25">
+        <v>570978</v>
+      </c>
+      <c r="J20" s="28">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K20" s="34">
+        <v>4401000000</v>
+      </c>
+      <c r="L20" s="34">
+        <v>-798000000</v>
+      </c>
+      <c r="M20" s="28">
+        <v>-0.153</v>
+      </c>
+      <c r="N20" s="26">
+        <v>38535</v>
+      </c>
+      <c r="O20" s="26">
+        <v>-39498</v>
+      </c>
+      <c r="P20" s="28">
+        <v>-0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="24">
+        <v>12</v>
+      </c>
+      <c r="C21" s="25">
+        <v>30299</v>
+      </c>
+      <c r="D21" s="25">
+        <v>54215</v>
+      </c>
+      <c r="E21" s="25">
+        <v>714994</v>
+      </c>
+      <c r="F21" s="25">
+        <v>799508</v>
+      </c>
+      <c r="G21" s="25">
+        <v>66626</v>
+      </c>
+      <c r="H21" s="25">
+        <v>74300</v>
+      </c>
+      <c r="I21" s="25">
+        <v>302327</v>
+      </c>
+      <c r="J21" s="28">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="K21" s="34">
+        <v>5199000000</v>
+      </c>
+      <c r="L21" s="34">
+        <v>482621000</v>
+      </c>
+      <c r="M21" s="28">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="N21" s="26">
+        <v>78033</v>
+      </c>
+      <c r="O21" s="26">
+        <v>-35802</v>
+      </c>
+      <c r="P21" s="28">
+        <v>-0.315</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="24">
+        <v>12</v>
+      </c>
+      <c r="C22" s="25">
+        <v>19050</v>
+      </c>
+      <c r="D22" s="25">
+        <v>46774</v>
+      </c>
+      <c r="E22" s="25">
+        <v>431357</v>
+      </c>
+      <c r="F22" s="25">
+        <v>497181</v>
+      </c>
+      <c r="G22" s="25">
+        <v>41432</v>
+      </c>
+      <c r="H22" s="25">
+        <v>45071</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="34">
+        <v>4716379000</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="M22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N22" s="26">
+        <v>113835</v>
+      </c>
+      <c r="O22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P22" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
+        <v>(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = 3.</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f>_xlfn.CONCAT("(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H29*100,2),"%")</f>
+        <v>(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = 0.14%</v>
+      </c>
+      <c r="H27" s="14">
+        <v>6.8599999999999994E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="H29" s="14">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-    </row>
-    <row r="2" spans="1:16" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-    </row>
-    <row r="3" spans="1:16" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28">
-        <f t="shared" ref="C4:E4" si="0">(1+$A$29)*C5</f>
-        <v>609832.92240000004</v>
-      </c>
-      <c r="D4" s="28">
-        <f t="shared" si="0"/>
-        <v>121234.8072</v>
-      </c>
-      <c r="E4" s="28">
-        <f t="shared" si="0"/>
-        <v>3726896.3783999998</v>
-      </c>
-      <c r="F4" s="28">
-        <f>(1+$A$29)*F5</f>
-        <v>4457964.108</v>
-      </c>
-      <c r="G4" s="28">
-        <f>F4/12</f>
-        <v>371497.00900000002</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="28">
-        <f>F4-F5</f>
-        <v>286184.10800000001</v>
-      </c>
-      <c r="J4" s="30">
-        <f>I4/F5</f>
-        <v>6.8600000000000008E-2</v>
-      </c>
-      <c r="K4" s="41">
-        <f>N4*G4</f>
-        <v>15457716278.011202</v>
-      </c>
-      <c r="L4" s="41">
-        <f>K4-K5</f>
-        <v>1012549021.7982006</v>
-      </c>
-      <c r="M4" s="31">
-        <f>L4/K5</f>
-        <v>7.0096040000000262E-2</v>
-      </c>
-      <c r="N4" s="29">
-        <f>(1+P4)*N5</f>
-        <v>41609.261726280012</v>
-      </c>
-      <c r="O4" s="29">
-        <f>N4-N5</f>
-        <v>58.171526280006219</v>
-      </c>
-      <c r="P4" s="30">
-        <f>A31</f>
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28">
-        <f t="shared" ref="C5:E5" si="1">C6*12/$B$6</f>
-        <v>570684</v>
-      </c>
-      <c r="D5" s="28">
-        <f t="shared" si="1"/>
-        <v>113452</v>
-      </c>
-      <c r="E5" s="28">
-        <f t="shared" si="1"/>
-        <v>3487644</v>
-      </c>
-      <c r="F5" s="28">
-        <f>F6*12/$B$6</f>
-        <v>4171780</v>
-      </c>
-      <c r="G5" s="28">
-        <f>F5/12</f>
-        <v>347648.33333333331</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="28">
-        <f>F5-F7</f>
-        <v>288288</v>
-      </c>
-      <c r="J5" s="31">
-        <f>I5/F7</f>
-        <v>7.4234220129718309E-2</v>
-      </c>
-      <c r="K5" s="41">
-        <f>N5*G5</f>
-        <v>14445167256.213001</v>
-      </c>
-      <c r="L5" s="41">
-        <f>K5-K7</f>
-        <v>1017167256.2130013</v>
-      </c>
-      <c r="M5" s="31">
-        <f>L5/K7</f>
-        <v>7.5749721195487132E-2</v>
-      </c>
-      <c r="N5" s="29">
-        <f>(1+P5)*N7</f>
-        <v>41551.090200000006</v>
-      </c>
-      <c r="O5" s="29">
-        <f>N5-N7</f>
-        <v>58.090200000006007</v>
-      </c>
-      <c r="P5" s="30">
-        <f>A31</f>
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="27">
-        <v>3</v>
-      </c>
-      <c r="C6" s="28">
-        <v>142671</v>
-      </c>
-      <c r="D6" s="28">
-        <v>28363</v>
-      </c>
-      <c r="E6" s="28">
-        <v>871911</v>
-      </c>
-      <c r="F6" s="28">
-        <v>1042945</v>
-      </c>
-      <c r="G6" s="28">
-        <v>347648</v>
-      </c>
-      <c r="H6" s="28">
-        <v>350874</v>
-      </c>
-      <c r="I6" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="P6" s="35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="27">
-        <v>12</v>
-      </c>
-      <c r="C7" s="28">
-        <v>493725</v>
-      </c>
-      <c r="D7" s="28">
-        <v>111461</v>
-      </c>
-      <c r="E7" s="28">
-        <v>3278306</v>
-      </c>
-      <c r="F7" s="28">
-        <v>3883492</v>
-      </c>
-      <c r="G7" s="28">
-        <v>323624</v>
-      </c>
-      <c r="H7" s="28">
-        <v>331699</v>
-      </c>
-      <c r="I7" s="28">
-        <v>358704</v>
-      </c>
-      <c r="J7" s="31">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="K7" s="41">
-        <v>13428000000</v>
-      </c>
-      <c r="L7" s="41">
-        <v>1686000000</v>
-      </c>
-      <c r="M7" s="31">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="N7" s="29">
-        <v>41493</v>
-      </c>
-      <c r="O7" s="29">
-        <v>1517</v>
-      </c>
-      <c r="P7" s="31">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="27">
-        <v>12</v>
-      </c>
-      <c r="C8" s="28">
-        <v>416349</v>
-      </c>
-      <c r="D8" s="28">
-        <v>91952</v>
-      </c>
-      <c r="E8" s="28">
-        <v>3016487</v>
-      </c>
-      <c r="F8" s="28">
-        <v>3524788</v>
-      </c>
-      <c r="G8" s="28">
-        <v>293732</v>
-      </c>
-      <c r="H8" s="28">
-        <v>299174</v>
-      </c>
-      <c r="I8" s="28">
-        <v>187451</v>
-      </c>
-      <c r="J8" s="31">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="K8" s="41">
-        <v>11742000000</v>
-      </c>
-      <c r="L8" s="41">
-        <v>115000000</v>
-      </c>
-      <c r="M8" s="31">
-        <v>0.01</v>
-      </c>
-      <c r="N8" s="29">
-        <v>39975</v>
-      </c>
-      <c r="O8" s="29">
-        <v>-1832</v>
-      </c>
-      <c r="P8" s="31">
-        <v>-4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="27">
-        <v>12</v>
-      </c>
-      <c r="C9" s="28">
-        <v>356677</v>
-      </c>
-      <c r="D9" s="28">
-        <v>67089</v>
-      </c>
-      <c r="E9" s="28">
-        <v>2913571</v>
-      </c>
-      <c r="F9" s="28">
-        <v>3337337</v>
-      </c>
-      <c r="G9" s="28">
-        <v>278111</v>
-      </c>
-      <c r="H9" s="28">
-        <v>280507</v>
-      </c>
-      <c r="I9" s="28">
-        <v>84633</v>
-      </c>
-      <c r="J9" s="31">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K9" s="41">
-        <v>11627000000</v>
-      </c>
-      <c r="L9" s="41">
-        <v>979000000</v>
-      </c>
-      <c r="M9" s="31">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="N9" s="29">
-        <v>41807</v>
-      </c>
-      <c r="O9" s="29">
-        <v>2524</v>
-      </c>
-      <c r="P9" s="31">
-        <v>6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="27">
-        <v>12</v>
-      </c>
-      <c r="C10" s="28">
-        <v>271573</v>
-      </c>
-      <c r="D10" s="28">
-        <v>65494</v>
-      </c>
-      <c r="E10" s="28">
-        <v>2915637</v>
-      </c>
-      <c r="F10" s="28">
-        <v>3252704</v>
-      </c>
-      <c r="G10" s="28">
-        <v>271059</v>
-      </c>
-      <c r="H10" s="28">
-        <v>270785</v>
-      </c>
-      <c r="I10" s="28">
-        <v>61573</v>
-      </c>
-      <c r="J10" s="31">
-        <v>1.9E-2</v>
-      </c>
-      <c r="K10" s="41">
-        <v>10648000000</v>
-      </c>
-      <c r="L10" s="41">
-        <v>-539000000</v>
-      </c>
-      <c r="M10" s="31">
-        <v>-4.8000000000000001E-2</v>
-      </c>
-      <c r="N10" s="29">
-        <v>39283</v>
-      </c>
-      <c r="O10" s="29">
-        <v>-2785</v>
-      </c>
-      <c r="P10" s="31">
-        <v>-6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="27">
-        <v>12</v>
-      </c>
-      <c r="C11" s="28">
-        <v>211114</v>
-      </c>
-      <c r="D11" s="28">
-        <v>68522</v>
-      </c>
-      <c r="E11" s="28">
-        <v>2911495</v>
-      </c>
-      <c r="F11" s="28">
-        <v>3191131</v>
-      </c>
-      <c r="G11" s="28">
-        <v>265928</v>
-      </c>
-      <c r="H11" s="28">
-        <v>272758</v>
-      </c>
-      <c r="I11" s="28">
-        <v>391265</v>
-      </c>
-      <c r="J11" s="31">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K11" s="41">
-        <v>11187000000</v>
-      </c>
-      <c r="L11" s="41">
-        <v>1517000000</v>
-      </c>
-      <c r="M11" s="31">
-        <v>0.157</v>
-      </c>
-      <c r="N11" s="29">
-        <v>42068</v>
-      </c>
-      <c r="O11" s="29">
-        <v>623</v>
-      </c>
-      <c r="P11" s="31">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="27">
-        <v>12</v>
-      </c>
-      <c r="C12" s="28">
-        <v>146837</v>
-      </c>
-      <c r="D12" s="28">
-        <v>68314</v>
-      </c>
-      <c r="E12" s="28">
-        <v>2584715</v>
-      </c>
-      <c r="F12" s="28">
-        <v>2799866</v>
-      </c>
-      <c r="G12" s="28">
-        <v>233322</v>
-      </c>
-      <c r="H12" s="28">
-        <v>240219</v>
-      </c>
-      <c r="I12" s="28">
-        <v>359451</v>
-      </c>
-      <c r="J12" s="31">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="K12" s="41">
-        <v>9670000000</v>
-      </c>
-      <c r="L12" s="41">
-        <v>465000000</v>
-      </c>
-      <c r="M12" s="31">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="N12" s="29">
-        <v>41445</v>
-      </c>
-      <c r="O12" s="29">
-        <v>-3818</v>
-      </c>
-      <c r="P12" s="31">
-        <v>-8.4000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="27">
-        <v>12</v>
-      </c>
-      <c r="C13" s="28">
-        <v>102280</v>
-      </c>
-      <c r="D13" s="28">
-        <v>67591</v>
-      </c>
-      <c r="E13" s="28">
-        <v>2270544</v>
-      </c>
-      <c r="F13" s="28">
-        <v>2440415</v>
-      </c>
-      <c r="G13" s="28">
-        <v>203368</v>
-      </c>
-      <c r="H13" s="28">
-        <v>210264</v>
-      </c>
-      <c r="I13" s="28">
-        <v>352109</v>
-      </c>
-      <c r="J13" s="31">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="K13" s="41">
-        <v>9205000000</v>
-      </c>
-      <c r="L13" s="41">
-        <v>921000000</v>
-      </c>
-      <c r="M13" s="31">
-        <v>0.111</v>
-      </c>
-      <c r="N13" s="29">
-        <v>45263</v>
-      </c>
-      <c r="O13" s="29">
-        <v>-2339</v>
-      </c>
-      <c r="P13" s="31">
-        <v>-4.9000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="27">
-        <v>12</v>
-      </c>
-      <c r="C14" s="28">
-        <v>74966</v>
-      </c>
-      <c r="D14" s="28">
-        <v>66883</v>
-      </c>
-      <c r="E14" s="28">
-        <v>1946457</v>
-      </c>
-      <c r="F14" s="28">
-        <v>2088306</v>
-      </c>
-      <c r="G14" s="28">
-        <v>174026</v>
-      </c>
-      <c r="H14" s="28">
-        <v>181219</v>
-      </c>
-      <c r="I14" s="28">
-        <v>353466</v>
-      </c>
-      <c r="J14" s="31">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="K14" s="41">
-        <v>8284000000</v>
-      </c>
-      <c r="L14" s="41">
-        <v>436000000</v>
-      </c>
-      <c r="M14" s="31">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="N14" s="29">
-        <v>47602</v>
-      </c>
-      <c r="O14" s="29">
-        <v>-6683</v>
-      </c>
-      <c r="P14" s="31">
-        <v>-0.123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="27">
-        <v>12</v>
-      </c>
-      <c r="C15" s="28">
-        <v>71979</v>
-      </c>
-      <c r="D15" s="28">
-        <v>65736</v>
-      </c>
-      <c r="E15" s="28">
-        <v>1597125</v>
-      </c>
-      <c r="F15" s="28">
-        <v>1734840</v>
-      </c>
-      <c r="G15" s="28">
-        <v>144570</v>
-      </c>
-      <c r="H15" s="28">
-        <v>148887</v>
-      </c>
-      <c r="I15" s="28">
-        <v>121067</v>
-      </c>
-      <c r="J15" s="31">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="K15" s="41">
-        <v>7848000000</v>
-      </c>
-      <c r="L15" s="41">
-        <v>371000000</v>
-      </c>
-      <c r="M15" s="31">
-        <v>0.05</v>
-      </c>
-      <c r="N15" s="29">
-        <v>54285</v>
-      </c>
-      <c r="O15" s="29">
-        <v>-1314</v>
-      </c>
-      <c r="P15" s="31">
-        <v>-2.4E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="27">
-        <v>12</v>
-      </c>
-      <c r="C16" s="28">
-        <v>68552</v>
-      </c>
-      <c r="D16" s="28">
-        <v>67476</v>
-      </c>
-      <c r="E16" s="28">
-        <v>1477745</v>
-      </c>
-      <c r="F16" s="28">
-        <v>1613773</v>
-      </c>
-      <c r="G16" s="28">
-        <v>134481</v>
-      </c>
-      <c r="H16" s="28">
-        <v>138251</v>
-      </c>
-      <c r="I16" s="28">
-        <v>243287</v>
-      </c>
-      <c r="J16" s="31">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="K16" s="41">
-        <v>7477000000</v>
-      </c>
-      <c r="L16" s="41">
-        <v>3076000000</v>
-      </c>
-      <c r="M16" s="31">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="N16" s="29">
-        <v>55599</v>
-      </c>
-      <c r="O16" s="29">
-        <v>17064</v>
-      </c>
-      <c r="P16" s="31">
-        <v>0.443</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="27">
-        <v>12</v>
-      </c>
-      <c r="C17" s="28">
-        <v>53408</v>
-      </c>
-      <c r="D17" s="28">
-        <v>62026</v>
-      </c>
-      <c r="E17" s="28">
-        <v>1255052</v>
-      </c>
-      <c r="F17" s="28">
-        <v>1370486</v>
-      </c>
-      <c r="G17" s="28">
-        <v>114207</v>
-      </c>
-      <c r="H17" s="28">
-        <v>122486</v>
-      </c>
-      <c r="I17" s="28">
-        <v>570978</v>
-      </c>
-      <c r="J17" s="31">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="K17" s="41">
-        <v>4401000000</v>
-      </c>
-      <c r="L17" s="41">
-        <v>-798000000</v>
-      </c>
-      <c r="M17" s="31">
-        <v>-0.153</v>
-      </c>
-      <c r="N17" s="29">
-        <v>38535</v>
-      </c>
-      <c r="O17" s="29">
-        <v>-39498</v>
-      </c>
-      <c r="P17" s="31">
-        <v>-0.50600000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="27">
-        <v>12</v>
-      </c>
-      <c r="C18" s="28">
-        <v>30299</v>
-      </c>
-      <c r="D18" s="28">
-        <v>54215</v>
-      </c>
-      <c r="E18" s="28">
-        <v>714994</v>
-      </c>
-      <c r="F18" s="28">
-        <v>799508</v>
-      </c>
-      <c r="G18" s="28">
-        <v>66626</v>
-      </c>
-      <c r="H18" s="28">
-        <v>74300</v>
-      </c>
-      <c r="I18" s="28">
-        <v>302327</v>
-      </c>
-      <c r="J18" s="31">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="K18" s="41">
-        <v>5199000000</v>
-      </c>
-      <c r="L18" s="41">
-        <v>482621000</v>
-      </c>
-      <c r="M18" s="31">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="N18" s="29">
-        <v>78033</v>
-      </c>
-      <c r="O18" s="29">
-        <v>-35802</v>
-      </c>
-      <c r="P18" s="31">
-        <v>-0.315</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="27">
-        <v>12</v>
-      </c>
-      <c r="C19" s="28">
-        <v>19050</v>
-      </c>
-      <c r="D19" s="28">
-        <v>46774</v>
-      </c>
-      <c r="E19" s="28">
-        <v>431357</v>
-      </c>
-      <c r="F19" s="28">
-        <v>497181</v>
-      </c>
-      <c r="G19" s="28">
-        <v>41432</v>
-      </c>
-      <c r="H19" s="28">
-        <v>45071</v>
-      </c>
-      <c r="I19" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="J19" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="41">
-        <v>4716379000</v>
-      </c>
-      <c r="L19" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="N19" s="29">
-        <v>113835</v>
-      </c>
-      <c r="O19" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="P19" s="35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" t="str">
-        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = ",B6,".")</f>
-        <v>(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = 3.</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
-        <f>_xlfn.CONCAT("(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(A31*100,2),"%")</f>
-        <v>(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = 0.14%</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="15">
-        <v>6.8599999999999994E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="15">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:P19">
-    <sortCondition descending="1" ref="A6:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:P22">
+    <sortCondition descending="1" ref="A9:A22"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
@@ -4689,6 +4864,9 @@
     <mergeCell ref="C2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F4:F8" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -4697,7 +4875,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4718,273 +4896,270 @@
   <sheetData>
     <row r="1" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P2" s="61" t="s">
+      <c r="P2" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="64"/>
     </row>
     <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P3" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="66"/>
+      <c r="P3" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="67"/>
     </row>
     <row r="4" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P4" s="17"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="19"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="17"/>
     </row>
     <row r="5" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="60"/>
+      <c r="P5" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="61"/>
     </row>
     <row r="6" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="19">
         <f>AVERAGE(projection_data!O14)</f>
         <v>0.10176623588849699</v>
       </c>
-      <c r="R6" s="21"/>
-      <c r="S6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="17"/>
     </row>
     <row r="7" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="19">
         <f>AVERAGE(projection_data!O12:O14)</f>
         <v>6.1316977536269246E-2</v>
       </c>
-      <c r="R7" s="21"/>
-      <c r="S7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="17"/>
     </row>
     <row r="8" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="19">
         <f>AVERAGE(projection_data!O10:O14)</f>
         <v>6.8598483323739995E-2</v>
       </c>
-      <c r="R8" s="21"/>
-      <c r="S8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="17"/>
     </row>
     <row r="9" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P9" s="17"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="19"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="17"/>
     </row>
     <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P10" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="60"/>
+      <c r="P10" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="61"/>
     </row>
     <row r="11" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="44">
         <f>AVERAGE(projection_data!R14)</f>
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="R11" s="22"/>
-      <c r="S11" s="19"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="17"/>
     </row>
     <row r="12" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="Q12" s="44">
         <f>AVERAGE(projection_data!R12:R14)</f>
         <v>1.9333333333333334E-2</v>
       </c>
-      <c r="R12" s="22"/>
-      <c r="S12" s="19"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="17"/>
     </row>
     <row r="13" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="44">
         <f>AVERAGE(projection_data!R10:R14)</f>
         <v>1.3999999999999998E-3</v>
       </c>
-      <c r="R13" s="22"/>
-      <c r="S13" s="19"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="17"/>
     </row>
     <row r="14" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P14" s="17"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="19"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="17"/>
     </row>
     <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="55" t="s">
+      <c r="P15" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="58"/>
     </row>
     <row r="16" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P16" s="46" t="s">
+      <c r="P16" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="19"/>
-    </row>
-    <row r="17" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P17" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="19"/>
-    </row>
-    <row r="18" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P18" s="16">
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="17"/>
+    </row>
+    <row r="17" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P17" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="55"/>
+    </row>
+    <row r="18" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P18" s="53"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="55"/>
+    </row>
+    <row r="19" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" s="17"/>
+    </row>
+    <row r="20" spans="16:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="P20" s="15">
         <v>6.8599999999999994E-2</v>
       </c>
-      <c r="Q18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R18" s="5"/>
-      <c r="S18" s="7"/>
-    </row>
-    <row r="19" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P19" s="6"/>
-      <c r="S19" s="7"/>
-    </row>
-    <row r="20" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P20" s="20" t="s">
-        <v>86</v>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="47">
+        <v>1.4E-3</v>
       </c>
       <c r="S20" s="7"/>
     </row>
-    <row r="21" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P21" s="16">
-        <v>1.4E-3</v>
-      </c>
-      <c r="Q21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R21" s="5"/>
+    <row r="21" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P21" s="6"/>
       <c r="S21" s="7"/>
     </row>
     <row r="22" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P22" s="6"/>
+      <c r="P22" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="S22" s="7"/>
     </row>
-    <row r="23" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P23" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="S23" s="7"/>
-    </row>
-    <row r="24" spans="16:19" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q24" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="R24" s="48" t="s">
+    <row r="23" spans="16:19" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q23" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="S24" s="49" t="s">
+      <c r="R23" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="S23" s="41" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="24" spans="16:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="P24" s="9" t="str" cm="1">
+        <f t="array" ref="P24:P28">projection_data!B15:B19</f>
+        <v>FY25</v>
+      </c>
+      <c r="Q24" s="46" cm="1">
+        <f t="array" ref="Q24:Q28">projection_data!N15:N19</f>
+        <v>345824.60639999999</v>
+      </c>
+      <c r="R24" s="35" cm="1">
+        <f t="array" ref="R24:R28">projection_data!P15:P19</f>
+        <v>41551.090200000006</v>
+      </c>
+      <c r="S24" s="37" cm="1">
+        <f t="array" ref="S24:S28">projection_data!K15:K19</f>
+        <v>14369389413.905899</v>
+      </c>
+    </row>
     <row r="25" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P25" s="9" t="str" cm="1">
-        <f t="array" ref="P25:P29">projection_data!B15:B19</f>
-        <v>FY25</v>
-      </c>
-      <c r="Q25" s="10" cm="1">
-        <f t="array" ref="Q25:Q29">projection_data!N15:N19</f>
-        <v>345824.60639999999</v>
-      </c>
-      <c r="R25" s="42" cm="1">
-        <f t="array" ref="R25:R29">projection_data!P15:P19</f>
-        <v>41551.090200000006</v>
-      </c>
-      <c r="S25" s="44" cm="1">
-        <f t="array" ref="S25:S29">projection_data!K15:K19</f>
-        <v>14369389413.905899</v>
+      <c r="P25" s="9" t="str">
+        <v>FY26</v>
+      </c>
+      <c r="Q25" s="46">
+        <v>369548.17439904</v>
+      </c>
+      <c r="R25" s="35">
+        <v>41609.261726280012</v>
+      </c>
+      <c r="S25" s="37">
+        <v>15376626709.038626</v>
       </c>
     </row>
     <row r="26" spans="16:19" ht="16" x14ac:dyDescent="0.2">
       <c r="P26" s="9" t="str">
-        <v>FY26</v>
-      </c>
-      <c r="Q26" s="10">
-        <v>369548.17439904</v>
-      </c>
-      <c r="R26" s="42">
-        <v>41609.261726280012</v>
-      </c>
-      <c r="S26" s="44">
-        <v>15376626709.038626</v>
+        <v>FY27</v>
+      </c>
+      <c r="Q26" s="46">
+        <v>394899.17916281417</v>
+      </c>
+      <c r="R26" s="35">
+        <v>41667.514692696808</v>
+      </c>
+      <c r="S26" s="37">
+        <v>16454467349.900469</v>
       </c>
     </row>
     <row r="27" spans="16:19" ht="16" x14ac:dyDescent="0.2">
       <c r="P27" s="9" t="str">
-        <v>FY27</v>
-      </c>
-      <c r="Q27" s="10">
-        <v>394899.17916281417</v>
-      </c>
-      <c r="R27" s="42">
-        <v>41667.514692696808</v>
-      </c>
-      <c r="S27" s="44">
-        <v>16454467349.900469</v>
-      </c>
-    </row>
-    <row r="28" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P28" s="9" t="str">
         <v>FY28</v>
       </c>
-      <c r="Q28" s="10">
+      <c r="Q27" s="46">
         <v>421989.2628533832</v>
       </c>
-      <c r="R28" s="42">
+      <c r="R27" s="35">
         <v>41725.849213266585</v>
       </c>
-      <c r="S28" s="44">
+      <c r="S27" s="37">
         <v>17607860351.437786</v>
       </c>
     </row>
-    <row r="29" spans="16:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P29" s="11" t="str">
+    <row r="28" spans="16:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="10" t="str">
         <v>FY29</v>
       </c>
-      <c r="Q29" s="12">
+      <c r="Q28" s="11">
         <v>450937.7262851253</v>
       </c>
-      <c r="R29" s="43">
+      <c r="R28" s="36">
         <v>41784.265402165162</v>
       </c>
-      <c r="S29" s="45">
+      <c r="S28" s="38">
         <v>18842101634.946587</v>
       </c>
     </row>
+    <row r="29" spans="16:19" x14ac:dyDescent="0.2"/>
     <row r="30" spans="16:19" x14ac:dyDescent="0.2"/>
     <row r="31" spans="16:19" x14ac:dyDescent="0.2"/>
     <row r="32" spans="16:19" x14ac:dyDescent="0.2"/>
@@ -5003,7 +5178,8 @@
     <row r="45" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="P17:S18"/>
     <mergeCell ref="P15:S15"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="P2:S2"/>
@@ -5023,8 +5199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EC6393-3785-8B4D-BC33-531ADF13ED6E}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5049,7 +5225,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5058,13 +5234,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -5087,11 +5263,11 @@
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>57</v>
+      <c r="N1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>9</v>
@@ -5105,10 +5281,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -5141,10 +5317,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -5182,7 +5358,7 @@
       <c r="N3" s="2">
         <v>66626</v>
       </c>
-      <c r="O3" s="23">
+      <c r="O3" s="20">
         <f>(N3-N2)/N2</f>
         <v>0.60808071056188451</v>
       </c>
@@ -5198,10 +5374,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -5239,7 +5415,7 @@
       <c r="N4" s="2">
         <v>114207</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="20">
         <f t="shared" ref="O4:O14" si="0">(N4-N3)/N3</f>
         <v>0.71415063188545014</v>
       </c>
@@ -5255,10 +5431,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -5296,7 +5472,7 @@
       <c r="N5" s="2">
         <v>134481</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="20">
         <f t="shared" si="0"/>
         <v>0.17751976673934172</v>
       </c>
@@ -5312,10 +5488,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -5353,7 +5529,7 @@
       <c r="N6" s="2">
         <v>144570</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="20">
         <f t="shared" si="0"/>
         <v>7.50217502844268E-2</v>
       </c>
@@ -5369,10 +5545,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -5410,7 +5586,7 @@
       <c r="N7" s="2">
         <v>174026</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="20">
         <f t="shared" si="0"/>
         <v>0.20374904890364529</v>
       </c>
@@ -5426,10 +5602,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -5467,7 +5643,7 @@
       <c r="N8" s="2">
         <v>203368</v>
       </c>
-      <c r="O8" s="23">
+      <c r="O8" s="20">
         <f t="shared" si="0"/>
         <v>0.16860698976015079</v>
       </c>
@@ -5483,10 +5659,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -5524,7 +5700,7 @@
       <c r="N9" s="2">
         <v>233322</v>
       </c>
-      <c r="O9" s="23">
+      <c r="O9" s="20">
         <f t="shared" si="0"/>
         <v>0.14728964242161993</v>
       </c>
@@ -5540,10 +5716,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -5581,7 +5757,7 @@
       <c r="N10" s="2">
         <v>265928</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="20">
         <f t="shared" si="0"/>
         <v>0.1397467877011169</v>
       </c>
@@ -5597,10 +5773,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -5638,7 +5814,7 @@
       <c r="N11" s="2">
         <v>271059</v>
       </c>
-      <c r="O11" s="23">
+      <c r="O11" s="20">
         <f t="shared" si="0"/>
         <v>1.9294696308775307E-2</v>
       </c>
@@ -5654,10 +5830,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>12</v>
@@ -5695,7 +5871,7 @@
       <c r="N12" s="2">
         <v>278111</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O12" s="20">
         <f t="shared" si="0"/>
         <v>2.6016476117745584E-2</v>
       </c>
@@ -5711,10 +5887,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -5752,7 +5928,7 @@
       <c r="N13" s="2">
         <v>293732</v>
       </c>
-      <c r="O13" s="23">
+      <c r="O13" s="20">
         <f t="shared" si="0"/>
         <v>5.6168220602565162E-2</v>
       </c>
@@ -5768,10 +5944,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -5809,7 +5985,7 @@
       <c r="N14" s="2">
         <v>323624</v>
       </c>
-      <c r="O14" s="23">
+      <c r="O14" s="20">
         <f t="shared" si="0"/>
         <v>0.10176623588849699</v>
       </c>
@@ -5823,132 +5999,133 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="37">
-        <f>(1+Graph!$P$18)*G14</f>
+    <row r="15" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="31">
+        <f>(1+Graph!$P$20)*G14</f>
         <v>4149899.5512000001</v>
       </c>
-      <c r="K15" s="38">
+      <c r="K15" s="32">
         <f>N15*P15</f>
         <v>14369389413.905899</v>
       </c>
-      <c r="N15" s="39">
-        <f>(1+Graph!$P$18)*N14</f>
+      <c r="N15" s="33">
+        <f>(1+Graph!$P$20)*N14</f>
         <v>345824.60639999999</v>
       </c>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38">
-        <f>(1+Graph!$P$21)*P14</f>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32">
+        <f>(1+Graph!$R$20)*P14</f>
         <v>41551.090200000006</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="37">
-        <f>(1+Graph!$P$18)*G15</f>
+    <row r="16" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="31">
+        <f>(1+Graph!$P$20)*G15</f>
         <v>4434582.6604123199</v>
       </c>
-      <c r="K16" s="38">
-        <f t="shared" ref="K16:K19" si="1">N16*P16</f>
+      <c r="K16" s="32">
+        <f>N16*P16</f>
         <v>15376626709.038626</v>
       </c>
-      <c r="N16" s="39">
-        <f>(1+Graph!$P$18)*N15</f>
+      <c r="N16" s="33">
+        <f>(1+Graph!$P$20)*N15</f>
         <v>369548.17439904</v>
       </c>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38">
-        <f>(1+Graph!$P$21)*P15</f>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32">
+        <f>(1+Graph!$R$20)*P15</f>
         <v>41609.261726280012</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="37">
-        <f>(1+Graph!$P$18)*G16</f>
+    <row r="17" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="31">
+        <f>(1+Graph!$P$20)*G16</f>
         <v>4738795.0309166051</v>
       </c>
-      <c r="K17" s="38">
-        <f t="shared" si="1"/>
+      <c r="K17" s="32">
+        <f t="shared" ref="K17:K19" si="1">N17*P17</f>
         <v>16454467349.900469</v>
       </c>
-      <c r="N17" s="39">
-        <f>(1+Graph!$P$18)*N16</f>
+      <c r="N17" s="33">
+        <f>(1+Graph!$P$20)*N16</f>
         <v>394899.17916281417</v>
       </c>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38">
-        <f>(1+Graph!$P$21)*P16</f>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32">
+        <f>(1+Graph!$R$20)*P16</f>
         <v>41667.514692696808</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="37">
-        <f>(1+Graph!$P$18)*G17</f>
+    <row r="18" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="31">
+        <f>(1+Graph!$P$20)*G17</f>
         <v>5063876.370037484</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K18" s="32">
         <f t="shared" si="1"/>
         <v>17607860351.437786</v>
       </c>
-      <c r="N18" s="39">
-        <f>(1+Graph!$P$18)*N17</f>
+      <c r="N18" s="33">
+        <f>(1+Graph!$P$20)*N17</f>
         <v>421989.2628533832</v>
       </c>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38">
-        <f>(1+Graph!$P$21)*P17</f>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32">
+        <f>(1+Graph!$R$20)*P17</f>
         <v>41725.849213266585</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="37">
-        <f>(1+Graph!$P$18)*G18</f>
+    <row r="19" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="31">
+        <f>(1+Graph!$P$20)*G18</f>
         <v>5411258.2890220555</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K19" s="32">
         <f t="shared" si="1"/>
         <v>18842101634.946587</v>
       </c>
-      <c r="N19" s="39">
-        <f>(1+Graph!$P$18)*N18</f>
+      <c r="N19" s="33">
+        <f>(1+Graph!$P$20)*N18</f>
         <v>450937.7262851253</v>
       </c>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38">
-        <f>(1+Graph!$P$21)*P18</f>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32">
+        <f>(1+Graph!$R$20)*P18</f>
         <v>41784.265402165162</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:R15">
     <sortCondition ref="B2:B15"/>
   </sortState>

</xml_diff>

<commit_message>
Update on 3/07/2025 at 9:49am
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F558D929-3845-6344-8333-38F5816C1C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342C446-A9E4-314E-AF3F-35DE71579B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -65,24 +65,12 @@
     <t>Months Reported</t>
   </si>
   <si>
-    <t>Enrollee Months</t>
-  </si>
-  <si>
-    <t>Average Monthly Change %</t>
-  </si>
-  <si>
     <t>Enrollee Months Annual Change</t>
   </si>
   <si>
-    <t>Enrollee Months Annual Change %</t>
-  </si>
-  <si>
     <t>State Spending</t>
   </si>
   <si>
-    <t>State Spending Annual Change</t>
-  </si>
-  <si>
     <t>State Spending Annual Change %</t>
   </si>
   <si>
@@ -177,15 +165,6 @@
   </si>
   <si>
     <t>FY15</t>
-  </si>
-  <si>
-    <t>FY14</t>
-  </si>
-  <si>
-    <t>FY13</t>
-  </si>
-  <si>
-    <t>FY12</t>
   </si>
   <si>
     <t>Average Annual Enrollment:</t>
@@ -375,15 +354,6 @@
   </si>
   <si>
     <t>Medicaid Managed Long Term Care Enrollment and Spending</t>
-  </si>
-  <si>
-    <t>PARTIAL MLTC</t>
-  </si>
-  <si>
-    <t>PACE</t>
-  </si>
-  <si>
-    <t>MAP</t>
   </si>
   <si>
     <t>Total Medicaid Managed Long Term Care Enrollment</t>
@@ -1061,9 +1031,6 @@
   </cellStyleXfs>
   <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1076,9 +1043,6 @@
     <xf numFmtId="165" fontId="8" fillId="3" borderId="18" xfId="7" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1172,6 +1136,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent4" xfId="11" builtinId="42"/>
@@ -1460,61 +1430,52 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>projection_data!$B$2:$B$19</c:f>
+              <c:f>projection_data!$B$2:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>FY12</c:v>
+                  <c:v>FY15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FY13</c:v>
+                  <c:v>FY16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FY14</c:v>
+                  <c:v>FY17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>FY15</c:v>
+                  <c:v>FY18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>FY16</c:v>
+                  <c:v>FY19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FY17</c:v>
+                  <c:v>FY20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>FY18</c:v>
+                  <c:v>FY21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FY19</c:v>
+                  <c:v>FY22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>FY20</c:v>
+                  <c:v>FY23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>FY21</c:v>
+                  <c:v>FY24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>FY22</c:v>
+                  <c:v>FY25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>FY23</c:v>
+                  <c:v>FY26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>FY24</c:v>
+                  <c:v>FY27</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>FY25</c:v>
+                  <c:v>FY28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>FY26</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>FY27</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>FY28</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>FY29</c:v>
                 </c:pt>
               </c:strCache>
@@ -1522,63 +1483,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>projection_data!$N$2:$N$19</c:f>
+              <c:f>projection_data!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>41432</c:v>
+                  <c:v>134481.07999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66626</c:v>
+                  <c:v>144570</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114207</c:v>
+                  <c:v>174025.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>134481</c:v>
+                  <c:v>203367.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>144570</c:v>
+                  <c:v>233322.17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>174026</c:v>
+                  <c:v>265927.58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>203368</c:v>
+                  <c:v>271057.83</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>233322</c:v>
+                  <c:v>278112.42</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>265928</c:v>
+                  <c:v>293737.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>271059</c:v>
+                  <c:v>323615.58</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>278111</c:v>
+                  <c:v>345815.60878800001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>293732</c:v>
+                  <c:v>369538.55955085682</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>323624</c:v>
+                  <c:v>394888.90473604557</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>345824.60639999999</c:v>
+                  <c:v>421978.28360093827</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>369548.17439904</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>394899.17916281417</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>421989.2628533832</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>450937.7262851253</c:v>
+                  <c:v>450925.99385596265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,7 +1561,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>projection_data!$K$1</c:f>
+              <c:f>projection_data!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1848,61 +1800,52 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>projection_data!$B$2:$B$19</c:f>
+              <c:f>projection_data!$B$2:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>FY12</c:v>
+                  <c:v>FY15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FY13</c:v>
+                  <c:v>FY16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FY14</c:v>
+                  <c:v>FY17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>FY15</c:v>
+                  <c:v>FY18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>FY16</c:v>
+                  <c:v>FY19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FY17</c:v>
+                  <c:v>FY20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>FY18</c:v>
+                  <c:v>FY21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FY19</c:v>
+                  <c:v>FY22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>FY20</c:v>
+                  <c:v>FY23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>FY21</c:v>
+                  <c:v>FY24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>FY22</c:v>
+                  <c:v>FY25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>FY23</c:v>
+                  <c:v>FY26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>FY24</c:v>
+                  <c:v>FY27</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>FY25</c:v>
+                  <c:v>FY28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>FY26</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>FY27</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>FY28</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>FY29</c:v>
                 </c:pt>
               </c:strCache>
@@ -1910,63 +1853,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>projection_data!$K$2:$K$19</c:f>
+              <c:f>projection_data!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4716379000</c:v>
+                  <c:v>3471000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5199000000</c:v>
+                  <c:v>3793000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4401000000</c:v>
+                  <c:v>4612000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7477000000</c:v>
+                  <c:v>5812000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7848000000</c:v>
+                  <c:v>6285000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8284000000</c:v>
+                  <c:v>7765000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9205000000</c:v>
+                  <c:v>7215000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9670000000</c:v>
+                  <c:v>7697000000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11187000000</c:v>
+                  <c:v>7614000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10648000000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11627000000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11742000000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13428000000</c:v>
+                  <c:v>8865000000</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
+                  <c:v>9527134805.1896362</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
+                  <c:v>10238726221.466753</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
+                  <c:v>11003467126.448851</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>14369389413.905899</c:v>
+                  <c:v>11825327309.659784</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>15376626709.038626</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>16454467349.900469</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>17607860351.437786</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>18842101634.946587</c:v>
+                  <c:v>12708573068.252131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3630,10 +3564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92772258-4AC4-6B47-AC5E-CDE7A2651A1C}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3645,1216 +3579,1066 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+    </row>
+    <row r="2" spans="1:16" s="11" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+    </row>
+    <row r="3" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-    </row>
-    <row r="2" spans="1:16" s="12" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="48" t="s">
+      <c r="E3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49" t="s">
+      <c r="K3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50" t="s">
+      <c r="P3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-    </row>
-    <row r="3" spans="1:16" s="21" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+    </row>
+    <row r="4" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="23">
+        <f t="shared" ref="C4:C7" si="0">C5*(1+$H$24)</f>
+        <v>687858.94516254519</v>
+      </c>
+      <c r="D4" s="23">
+        <f>D5*(1+$H$24)</f>
+        <v>155302.80578954259</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E6" si="1">E5*(1+$H$24)</f>
+        <v>4567950.2310554693</v>
+      </c>
+      <c r="F4" s="23">
+        <f>G4*12</f>
+        <v>5411111.9262715522</v>
+      </c>
+      <c r="G4" s="23">
+        <f t="shared" ref="G4:G6" si="2">G5*(1+$H$24)</f>
+        <v>450925.99385596265</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="23">
+        <f>F4-F5</f>
+        <v>347372.52306029294</v>
+      </c>
+      <c r="J4" s="25">
+        <f t="shared" ref="J4:J6" si="3">I4/F5</f>
+        <v>6.8600000000000105E-2</v>
+      </c>
+      <c r="K4" s="32">
+        <f t="shared" ref="K4:K6" si="4">N4*G4</f>
+        <v>12708573068.252131</v>
+      </c>
+      <c r="L4" s="32">
+        <f t="shared" ref="L4:L6" si="5">K4-K5</f>
+        <v>883245758.59234619</v>
+      </c>
+      <c r="M4" s="26">
+        <f t="shared" ref="M4:M6" si="6">L4/K5</f>
+        <v>7.4691020000000094E-2</v>
+      </c>
+      <c r="N4" s="24">
+        <f t="shared" ref="N4:N6" si="7">(1+P4)*N5</f>
+        <v>28183.278944685488</v>
+      </c>
+      <c r="O4" s="24">
+        <f t="shared" ref="O4:O6" si="8">N4-N5</f>
+        <v>159.7342050161169</v>
+      </c>
+      <c r="P4" s="25">
+        <f>$H$26</f>
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="23">
+        <f t="shared" si="0"/>
+        <v>643701.05293144786</v>
+      </c>
+      <c r="D5" s="23">
+        <f>D6*(1+$H$24)</f>
+        <v>145332.96442966739</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="1"/>
+        <v>4274705.4380081128</v>
+      </c>
+      <c r="F5" s="23">
+        <f t="shared" ref="F5:F8" si="9">G5*12</f>
+        <v>5063739.4032112593</v>
+      </c>
+      <c r="G5" s="23">
+        <f t="shared" si="2"/>
+        <v>421978.28360093827</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="23">
+        <f>F5-F6</f>
+        <v>325072.54637871217</v>
+      </c>
+      <c r="J5" s="25">
+        <f t="shared" si="3"/>
+        <v>6.8599999999999883E-2</v>
+      </c>
+      <c r="K5" s="32">
+        <f>N5*G5</f>
+        <v>11825327309.659784</v>
+      </c>
+      <c r="L5" s="32">
+        <f t="shared" si="5"/>
+        <v>821860183.21093369</v>
+      </c>
+      <c r="M5" s="26">
+        <f t="shared" si="6"/>
+        <v>7.4691020000000011E-2</v>
+      </c>
+      <c r="N5" s="24">
+        <f t="shared" si="7"/>
+        <v>28023.544739669371</v>
+      </c>
+      <c r="O5" s="24">
+        <f t="shared" si="8"/>
+        <v>158.8288803978503</v>
+      </c>
+      <c r="P5" s="25">
+        <f>$H$26</f>
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="23">
+        <f t="shared" si="0"/>
+        <v>602377.9271303087</v>
+      </c>
+      <c r="D6" s="23">
+        <f>D7*(1+$H$24)</f>
+        <v>136003.14844625434</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="1"/>
+        <v>4000285.8300656122</v>
+      </c>
+      <c r="F6" s="23">
+        <f t="shared" si="9"/>
+        <v>4738666.8568325471</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" si="2"/>
+        <v>394888.90473604557</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="23">
+        <f t="shared" ref="I6" si="10">F6-F7</f>
+        <v>304204.14222226478</v>
+      </c>
+      <c r="J6" s="25">
+        <f t="shared" si="3"/>
+        <v>6.8599999999999869E-2</v>
+      </c>
+      <c r="K6" s="32">
+        <f t="shared" si="4"/>
+        <v>11003467126.448851</v>
+      </c>
+      <c r="L6" s="32">
+        <f t="shared" si="5"/>
+        <v>764740904.98209763</v>
+      </c>
+      <c r="M6" s="26">
+        <f t="shared" si="6"/>
+        <v>7.4691019999999997E-2</v>
+      </c>
+      <c r="N6" s="24">
+        <f t="shared" si="7"/>
+        <v>27864.71585927152</v>
+      </c>
+      <c r="O6" s="24">
+        <f t="shared" si="8"/>
+        <v>157.9286868826166</v>
+      </c>
+      <c r="P6" s="25">
+        <f>$H$26</f>
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="22" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="23">
+        <f t="shared" si="0"/>
+        <v>563707.58668379998</v>
+      </c>
+      <c r="D7" s="23">
+        <f>D8*(1+$H$24)</f>
+        <v>127272.27067776</v>
+      </c>
+      <c r="E7" s="23">
+        <f>E8*(1+$H$24)</f>
+        <v>3743482.90292496</v>
+      </c>
+      <c r="F7" s="23">
+        <f t="shared" si="9"/>
+        <v>4434462.7146102823</v>
+      </c>
+      <c r="G7" s="23">
+        <f>G8*(1+$H$24)</f>
+        <v>369538.55955085682</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="23">
+        <f>F7-F8</f>
+        <v>284675.40915428195</v>
+      </c>
+      <c r="J7" s="25">
+        <f>I7/F8</f>
+        <v>6.8600000000000078E-2</v>
+      </c>
+      <c r="K7" s="32">
+        <f>N7*G7</f>
+        <v>10238726221.466753</v>
+      </c>
+      <c r="L7" s="32">
+        <f>K7-K8</f>
+        <v>711591416.27711678</v>
+      </c>
+      <c r="M7" s="26">
+        <f>L7/K8</f>
+        <v>7.4691020000000163E-2</v>
+      </c>
+      <c r="N7" s="24">
+        <f>(1+P7)*N8</f>
+        <v>27706.787172388904</v>
+      </c>
+      <c r="O7" s="24">
+        <f>N7-N8</f>
+        <v>157.03359538890072</v>
+      </c>
+      <c r="P7" s="25">
+        <f>$H$26</f>
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23">
+        <f t="shared" ref="C8:D8" si="11">C10*(1+$H$24)</f>
+        <v>527519.73300000001</v>
+      </c>
+      <c r="D8" s="23">
+        <f t="shared" si="11"/>
+        <v>119101.88159999999</v>
+      </c>
+      <c r="E8" s="23">
+        <f>E10*(1+$H$24)</f>
+        <v>3503165.7335999999</v>
+      </c>
+      <c r="F8" s="23">
+        <f t="shared" si="9"/>
+        <v>4149787.3054560004</v>
+      </c>
+      <c r="G8" s="23">
+        <f>G10*(1+$H$24)</f>
+        <v>345815.60878800001</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="23">
+        <f>F8-F10</f>
+        <v>266400.30545600038</v>
+      </c>
+      <c r="J8" s="26">
+        <f>I8/F10</f>
+        <v>6.8599988993113578E-2</v>
+      </c>
+      <c r="K8" s="32">
+        <f>N8*G8</f>
+        <v>9527134805.1896362</v>
+      </c>
+      <c r="L8" s="32">
+        <f>K8-K10</f>
+        <v>662134805.18963623</v>
+      </c>
+      <c r="M8" s="26">
+        <f>L8/K10</f>
+        <v>7.4690897370517345E-2</v>
+      </c>
+      <c r="N8" s="24">
+        <f>(1+P8)*N10</f>
+        <v>27549.753577000003</v>
+      </c>
+      <c r="O8" s="24">
+        <f>N8-N10</f>
+        <v>156.14357700000255</v>
+      </c>
+      <c r="P8" s="25">
+        <f>$H$26</f>
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="22">
+        <v>5</v>
+      </c>
+      <c r="C9" s="23">
+        <v>242846</v>
+      </c>
+      <c r="D9" s="23">
+        <v>47389</v>
+      </c>
+      <c r="E9" s="23">
+        <v>1465713</v>
+      </c>
+      <c r="F9" s="23">
+        <v>1755948</v>
+      </c>
+      <c r="G9" s="23">
+        <v>351189.6</v>
+      </c>
+      <c r="H9" s="23">
+        <v>358404</v>
+      </c>
+      <c r="I9" s="27">
+        <v>-2127439</v>
+      </c>
+      <c r="J9" s="27">
+        <v>-0.54783079999999995</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="N9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P9" s="27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="22">
+        <v>12</v>
+      </c>
+      <c r="C10" s="23">
+        <v>493655</v>
+      </c>
+      <c r="D10" s="23">
+        <v>111456</v>
+      </c>
+      <c r="E10" s="23">
+        <v>3278276</v>
+      </c>
+      <c r="F10" s="23">
+        <v>3883387</v>
+      </c>
+      <c r="G10" s="23">
+        <v>323615.58</v>
+      </c>
+      <c r="H10" s="23">
+        <v>331687</v>
+      </c>
+      <c r="I10" s="23">
+        <v>358537</v>
+      </c>
+      <c r="J10" s="26">
+        <v>0.10171695</v>
+      </c>
+      <c r="K10" s="32">
+        <v>8865000000</v>
+      </c>
+      <c r="L10" s="32">
+        <v>1251000000</v>
+      </c>
+      <c r="M10" s="26">
+        <v>0.16430259999999999</v>
+      </c>
+      <c r="N10" s="24">
+        <v>27393.61</v>
+      </c>
+      <c r="O10" s="24">
+        <v>1472.5098</v>
+      </c>
+      <c r="P10" s="26">
+        <v>5.6807370000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="22">
+        <v>12</v>
+      </c>
+      <c r="C11" s="23">
+        <v>416312</v>
+      </c>
+      <c r="D11" s="23">
+        <v>91950</v>
+      </c>
+      <c r="E11" s="23">
+        <v>3016588</v>
+      </c>
+      <c r="F11" s="23">
+        <v>3524850</v>
+      </c>
+      <c r="G11" s="23">
+        <v>293737.5</v>
+      </c>
+      <c r="H11" s="23">
+        <v>299176</v>
+      </c>
+      <c r="I11" s="23">
+        <v>187501</v>
+      </c>
+      <c r="J11" s="26">
+        <v>5.6182620000000003E-2</v>
+      </c>
+      <c r="K11" s="32">
+        <v>7614000000</v>
+      </c>
+      <c r="L11" s="32">
+        <v>-83000000</v>
+      </c>
+      <c r="M11" s="26">
+        <v>-1.078342E-2</v>
+      </c>
+      <c r="N11" s="24">
+        <v>25921.1</v>
+      </c>
+      <c r="O11" s="24">
+        <v>-1754.7559000000001</v>
+      </c>
+      <c r="P11" s="26">
+        <v>-6.3403840000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="22">
+        <v>12</v>
+      </c>
+      <c r="C12" s="23">
+        <v>356653</v>
+      </c>
+      <c r="D12" s="23">
+        <v>67089</v>
+      </c>
+      <c r="E12" s="23">
+        <v>2913607</v>
+      </c>
+      <c r="F12" s="23">
+        <v>3337349</v>
+      </c>
+      <c r="G12" s="23">
+        <v>278112.42</v>
+      </c>
+      <c r="H12" s="23">
+        <v>280508</v>
+      </c>
+      <c r="I12" s="23">
+        <v>84655</v>
+      </c>
+      <c r="J12" s="26">
+        <v>2.602612E-2</v>
+      </c>
+      <c r="K12" s="32">
+        <v>7697000000</v>
+      </c>
+      <c r="L12" s="32">
+        <v>482000000</v>
+      </c>
+      <c r="M12" s="26">
+        <v>6.680527E-2</v>
+      </c>
+      <c r="N12" s="24">
+        <v>27675.86</v>
+      </c>
+      <c r="O12" s="24">
+        <v>1057.9231</v>
+      </c>
+      <c r="P12" s="26">
+        <v>3.9744750000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="22">
+        <v>12</v>
+      </c>
+      <c r="C13" s="23">
+        <v>271565</v>
+      </c>
+      <c r="D13" s="23">
+        <v>65494</v>
+      </c>
+      <c r="E13" s="23">
+        <v>2915635</v>
+      </c>
+      <c r="F13" s="23">
+        <v>3252694</v>
+      </c>
+      <c r="G13" s="23">
+        <v>271057.83</v>
+      </c>
+      <c r="H13" s="23">
+        <v>270784</v>
+      </c>
+      <c r="I13" s="23">
+        <v>61563</v>
+      </c>
+      <c r="J13" s="26">
+        <v>1.9291909999999999E-2</v>
+      </c>
+      <c r="K13" s="32">
+        <v>7215000000</v>
+      </c>
+      <c r="L13" s="32">
+        <v>-550000000</v>
+      </c>
+      <c r="M13" s="26">
+        <v>-7.0830649999999995E-2</v>
+      </c>
+      <c r="N13" s="24">
+        <v>26617.94</v>
+      </c>
+      <c r="O13" s="24">
+        <v>-2581.7429999999999</v>
+      </c>
+      <c r="P13" s="26">
+        <v>-8.8416830000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="22">
+        <v>12</v>
+      </c>
+      <c r="C14" s="23">
+        <v>211114</v>
+      </c>
+      <c r="D14" s="23">
+        <v>68522</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2911495</v>
+      </c>
+      <c r="F14" s="23">
+        <v>3191131</v>
+      </c>
+      <c r="G14" s="23">
+        <v>265927.58</v>
+      </c>
+      <c r="H14" s="23">
+        <v>272758</v>
+      </c>
+      <c r="I14" s="23">
+        <v>391265</v>
+      </c>
+      <c r="J14" s="26">
+        <v>0.13974418999999999</v>
+      </c>
+      <c r="K14" s="32">
+        <v>7765000000</v>
+      </c>
+      <c r="L14" s="32">
+        <v>1480000000</v>
+      </c>
+      <c r="M14" s="26">
+        <v>0.2354813</v>
+      </c>
+      <c r="N14" s="24">
+        <v>29199.68</v>
+      </c>
+      <c r="O14" s="24">
+        <v>2262.6752999999999</v>
+      </c>
+      <c r="P14" s="26">
+        <v>8.3998779999999995E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="22">
+        <v>12</v>
+      </c>
+      <c r="C15" s="23">
+        <v>146837</v>
+      </c>
+      <c r="D15" s="23">
+        <v>68314</v>
+      </c>
+      <c r="E15" s="23">
+        <v>2584715</v>
+      </c>
+      <c r="F15" s="23">
+        <v>2799866</v>
+      </c>
+      <c r="G15" s="23">
+        <v>233322.17</v>
+      </c>
+      <c r="H15" s="23">
+        <v>240219</v>
+      </c>
+      <c r="I15" s="23">
+        <v>359451</v>
+      </c>
+      <c r="J15" s="26">
+        <v>0.14729092999999999</v>
+      </c>
+      <c r="K15" s="32">
+        <v>6285000000</v>
+      </c>
+      <c r="L15" s="32">
+        <v>473000000</v>
+      </c>
+      <c r="M15" s="26">
+        <v>8.1383339999999998E-2</v>
+      </c>
+      <c r="N15" s="24">
+        <v>26937</v>
+      </c>
+      <c r="O15" s="24">
+        <v>-1641.7424000000001</v>
+      </c>
+      <c r="P15" s="26">
+        <v>-5.7446270000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="22">
+        <v>12</v>
+      </c>
+      <c r="C16" s="23">
+        <v>102280</v>
+      </c>
+      <c r="D16" s="23">
+        <v>67591</v>
+      </c>
+      <c r="E16" s="23">
+        <v>2270544</v>
+      </c>
+      <c r="F16" s="23">
+        <v>2440415</v>
+      </c>
+      <c r="G16" s="23">
+        <v>203367.92</v>
+      </c>
+      <c r="H16" s="23">
+        <v>210264</v>
+      </c>
+      <c r="I16" s="23">
+        <v>352109</v>
+      </c>
+      <c r="J16" s="26">
+        <v>0.16860987</v>
+      </c>
+      <c r="K16" s="32">
+        <v>5812000000</v>
+      </c>
+      <c r="L16" s="32">
+        <v>1200000000</v>
+      </c>
+      <c r="M16" s="26">
+        <v>0.26019080999999999</v>
+      </c>
+      <c r="N16" s="24">
+        <v>28578.75</v>
+      </c>
+      <c r="O16" s="24">
+        <v>2076.8825999999999</v>
+      </c>
+      <c r="P16" s="26">
+        <v>7.8367419999999993E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="22">
+        <v>12</v>
+      </c>
+      <c r="C17" s="23">
+        <v>74966</v>
+      </c>
+      <c r="D17" s="23">
+        <v>66883</v>
+      </c>
+      <c r="E17" s="23">
+        <v>1946457</v>
+      </c>
+      <c r="F17" s="23">
+        <v>2088306</v>
+      </c>
+      <c r="G17" s="23">
+        <v>174025.5</v>
+      </c>
+      <c r="H17" s="23">
+        <v>181219</v>
+      </c>
+      <c r="I17" s="23">
+        <v>353466</v>
+      </c>
+      <c r="J17" s="26">
+        <v>0.20374559</v>
+      </c>
+      <c r="K17" s="32">
+        <v>4612000000</v>
+      </c>
+      <c r="L17" s="32">
+        <v>819000000</v>
+      </c>
+      <c r="M17" s="26">
+        <v>0.21592407</v>
+      </c>
+      <c r="N17" s="24">
+        <v>26501.86</v>
+      </c>
+      <c r="O17" s="24">
+        <v>265.43799999999999</v>
+      </c>
+      <c r="P17" s="26">
+        <v>1.011715E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="22">
+        <v>12</v>
+      </c>
+      <c r="C18" s="23">
+        <v>71979</v>
+      </c>
+      <c r="D18" s="23">
+        <v>65736</v>
+      </c>
+      <c r="E18" s="23">
+        <v>1597125</v>
+      </c>
+      <c r="F18" s="23">
+        <v>1734840</v>
+      </c>
+      <c r="G18" s="23">
+        <v>144570</v>
+      </c>
+      <c r="H18" s="23">
+        <v>148887</v>
+      </c>
+      <c r="I18" s="23">
+        <v>121067</v>
+      </c>
+      <c r="J18" s="26">
+        <v>7.5021080000000004E-2</v>
+      </c>
+      <c r="K18" s="32">
+        <v>3793000000</v>
+      </c>
+      <c r="L18" s="32">
+        <v>322000000</v>
+      </c>
+      <c r="M18" s="26">
+        <v>9.2768649999999994E-2</v>
+      </c>
+      <c r="N18" s="24">
+        <v>26236.43</v>
+      </c>
+      <c r="O18" s="24">
+        <v>426.1037</v>
+      </c>
+      <c r="P18" s="26">
+        <v>1.6509039999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="22">
+        <v>12</v>
+      </c>
+      <c r="C19" s="23">
+        <v>68552</v>
+      </c>
+      <c r="D19" s="23">
+        <v>67476</v>
+      </c>
+      <c r="E19" s="23">
+        <v>1477745</v>
+      </c>
+      <c r="F19" s="23">
+        <v>1613773</v>
+      </c>
+      <c r="G19" s="23">
+        <v>134481.07999999999</v>
+      </c>
+      <c r="H19" s="23">
+        <v>138251</v>
+      </c>
+      <c r="I19" s="23">
+        <v>243287</v>
+      </c>
+      <c r="J19" s="26">
+        <v>0.17751877999999999</v>
+      </c>
+      <c r="K19" s="32">
+        <v>3471000000</v>
+      </c>
+      <c r="L19" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="N19" s="24">
+        <v>25810.32</v>
+      </c>
+      <c r="O19" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="P19" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="25">
-        <f t="shared" ref="C4:C7" si="0">C5*(1+$H$27)</f>
-        <v>687956.48317221063</v>
-      </c>
-      <c r="D4" s="25">
-        <f t="shared" ref="D4:D7" si="1">D5*(1+$H$27)</f>
-        <v>155309.77279023294</v>
-      </c>
-      <c r="E4" s="25">
-        <f t="shared" ref="E4:E6" si="2">E5*(1+$H$27)</f>
-        <v>4567992.0330596119</v>
-      </c>
-      <c r="F4" s="25">
-        <f>G4*12</f>
-        <v>5411252.7154215034</v>
-      </c>
-      <c r="G4" s="25">
-        <f t="shared" ref="G4:G6" si="3">G5*(1+$H$27)</f>
-        <v>450937.7262851253</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" s="25">
-        <f>F4-F5</f>
-        <v>347381.56118090451</v>
-      </c>
-      <c r="J4" s="27">
-        <f t="shared" ref="J4:J6" si="4">I4/F5</f>
-        <v>6.8599999999999883E-2</v>
-      </c>
-      <c r="K4" s="34">
-        <f t="shared" ref="K4:K6" si="5">N4*G4</f>
-        <v>18842101634.946587</v>
-      </c>
-      <c r="L4" s="34">
-        <f t="shared" ref="L4:L6" si="6">K4-K5</f>
-        <v>1234241283.5088005</v>
-      </c>
-      <c r="M4" s="28">
-        <f t="shared" ref="M4:M6" si="7">L4/K5</f>
-        <v>7.0096040000000193E-2</v>
-      </c>
-      <c r="N4" s="26">
-        <f t="shared" ref="N4:N6" si="8">(1+P4)*N5</f>
-        <v>41784.265402165162</v>
-      </c>
-      <c r="O4" s="26">
-        <f t="shared" ref="O4:O6" si="9">N4-N5</f>
-        <v>58.416188898576365</v>
-      </c>
-      <c r="P4" s="27">
-        <f t="shared" ref="P4:P6" si="10">$H$29</f>
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="25">
-        <f t="shared" si="0"/>
-        <v>643792.32937695179</v>
-      </c>
-      <c r="D5" s="25">
-        <f t="shared" si="1"/>
-        <v>145339.48417577479</v>
-      </c>
-      <c r="E5" s="25">
-        <f t="shared" si="2"/>
-        <v>4274744.5564847579</v>
-      </c>
-      <c r="F5" s="25">
-        <f t="shared" ref="F5:F8" si="11">G5*12</f>
-        <v>5063871.1542405989</v>
-      </c>
-      <c r="G5" s="25">
-        <f t="shared" si="3"/>
-        <v>421989.2628533832</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" s="25">
-        <f>F5-F6</f>
-        <v>325081.00428682938</v>
-      </c>
-      <c r="J5" s="27">
-        <f t="shared" si="4"/>
-        <v>6.8600000000000161E-2</v>
-      </c>
-      <c r="K5" s="34">
-        <f>N5*G5</f>
-        <v>17607860351.437786</v>
-      </c>
-      <c r="L5" s="34">
-        <f t="shared" si="6"/>
-        <v>1153393001.5373173</v>
-      </c>
-      <c r="M5" s="28">
-        <f t="shared" si="7"/>
-        <v>7.0096039999999998E-2</v>
-      </c>
-      <c r="N5" s="26">
-        <f t="shared" si="8"/>
-        <v>41725.849213266585</v>
-      </c>
-      <c r="O5" s="26">
-        <f t="shared" si="9"/>
-        <v>58.334520569776942</v>
-      </c>
-      <c r="P5" s="27">
-        <f t="shared" si="10"/>
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="25">
-        <f t="shared" si="0"/>
-        <v>602463.34397992864</v>
-      </c>
-      <c r="D6" s="25">
-        <f t="shared" si="1"/>
-        <v>136009.24964979861</v>
-      </c>
-      <c r="E6" s="25">
-        <f t="shared" si="2"/>
-        <v>4000322.437286878</v>
-      </c>
-      <c r="F6" s="25">
-        <f t="shared" si="11"/>
-        <v>4738790.1499537695</v>
-      </c>
-      <c r="G6" s="25">
-        <f t="shared" si="3"/>
-        <v>394899.17916281417</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="I6" s="25">
-        <f t="shared" ref="I6" si="12">F6-F7</f>
-        <v>304212.0571652893</v>
-      </c>
-      <c r="J6" s="27">
-        <f t="shared" si="4"/>
-        <v>6.8599999999999897E-2</v>
-      </c>
-      <c r="K6" s="34">
-        <f t="shared" si="5"/>
-        <v>16454467349.900469</v>
-      </c>
-      <c r="L6" s="34">
-        <f t="shared" si="6"/>
-        <v>1077840640.8618431</v>
-      </c>
-      <c r="M6" s="28">
-        <f t="shared" si="7"/>
-        <v>7.0096040000000207E-2</v>
-      </c>
-      <c r="N6" s="26">
-        <f t="shared" si="8"/>
-        <v>41667.514692696808</v>
-      </c>
-      <c r="O6" s="26">
-        <f t="shared" si="9"/>
-        <v>58.252966416795971</v>
-      </c>
-      <c r="P6" s="27">
-        <f t="shared" si="10"/>
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25">
-        <f t="shared" si="0"/>
-        <v>563787.52010100009</v>
-      </c>
-      <c r="D7" s="25">
-        <f t="shared" si="1"/>
-        <v>127277.98020756</v>
-      </c>
-      <c r="E7" s="25">
-        <f>E8*(1+$H$27)</f>
-        <v>3743517.1601037602</v>
-      </c>
-      <c r="F7" s="25">
-        <f t="shared" si="11"/>
-        <v>4434578.0927884802</v>
-      </c>
-      <c r="G7" s="25">
-        <f>G8*(1+$H$27)</f>
-        <v>369548.17439904</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="25">
-        <f>F7-F8</f>
-        <v>284682.81598848011</v>
-      </c>
-      <c r="J7" s="27">
-        <f>I7/F8</f>
-        <v>6.8600000000000022E-2</v>
-      </c>
-      <c r="K7" s="34">
-        <f>N7*G7</f>
-        <v>15376626709.038626</v>
-      </c>
-      <c r="L7" s="34">
-        <f>K7-K8</f>
-        <v>1007237295.1327267</v>
-      </c>
-      <c r="M7" s="28">
-        <f>L7/K8</f>
-        <v>7.0096040000000151E-2</v>
-      </c>
-      <c r="N7" s="26">
-        <f>(1+P7)*N8</f>
-        <v>41609.261726280012</v>
-      </c>
-      <c r="O7" s="26">
-        <f>N7-N8</f>
-        <v>58.171526280006219</v>
-      </c>
-      <c r="P7" s="27">
-        <f>$H$29</f>
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25">
-        <f t="shared" ref="C8:D8" si="13">C10*(1+$H$27)</f>
-        <v>527594.53500000003</v>
-      </c>
-      <c r="D8" s="25">
-        <f t="shared" si="13"/>
-        <v>119107.2246</v>
-      </c>
-      <c r="E8" s="25">
-        <f>E10*(1+$H$27)</f>
-        <v>3503197.7916000001</v>
-      </c>
-      <c r="F8" s="25">
-        <f t="shared" si="11"/>
-        <v>4149895.2768000001</v>
-      </c>
-      <c r="G8" s="25">
-        <f>G10*(1+$H$27)</f>
-        <v>345824.60639999999</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" s="25">
-        <f>F8-F10</f>
-        <v>266403.27680000011</v>
-      </c>
-      <c r="J8" s="28">
-        <f>I8/F10</f>
-        <v>6.8598899341108494E-2</v>
-      </c>
-      <c r="K8" s="34">
-        <f>N8*G8</f>
-        <v>14369389413.905899</v>
-      </c>
-      <c r="L8" s="34">
-        <f>K8-K10</f>
-        <v>941389413.90589905</v>
-      </c>
-      <c r="M8" s="28">
-        <f>L8/K10</f>
-        <v>7.0106450246194454E-2</v>
-      </c>
-      <c r="N8" s="26">
-        <f>(1+P8)*N10</f>
-        <v>41551.090200000006</v>
-      </c>
-      <c r="O8" s="26">
-        <f>N8-N10</f>
-        <v>58.090200000006007</v>
-      </c>
-      <c r="P8" s="27">
-        <f>$H$29</f>
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="24">
-        <v>3</v>
-      </c>
-      <c r="C9" s="25">
-        <v>142671</v>
-      </c>
-      <c r="D9" s="25">
-        <v>28363</v>
-      </c>
-      <c r="E9" s="25">
-        <v>871911</v>
-      </c>
-      <c r="F9" s="25">
-        <v>1042945</v>
-      </c>
-      <c r="G9" s="25">
-        <v>347648</v>
-      </c>
-      <c r="H9" s="25">
-        <v>350874</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="M9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="N9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="O9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P9" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="24">
-        <v>12</v>
-      </c>
-      <c r="C10" s="25">
-        <v>493725</v>
-      </c>
-      <c r="D10" s="25">
-        <v>111461</v>
-      </c>
-      <c r="E10" s="25">
-        <v>3278306</v>
-      </c>
-      <c r="F10" s="25">
-        <v>3883492</v>
-      </c>
-      <c r="G10" s="25">
-        <v>323624</v>
-      </c>
-      <c r="H10" s="25">
-        <v>331699</v>
-      </c>
-      <c r="I10" s="25">
-        <v>358704</v>
-      </c>
-      <c r="J10" s="28">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="K10" s="34">
-        <v>13428000000</v>
-      </c>
-      <c r="L10" s="34">
-        <v>1686000000</v>
-      </c>
-      <c r="M10" s="28">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="N10" s="26">
-        <v>41493</v>
-      </c>
-      <c r="O10" s="26">
-        <v>1517</v>
-      </c>
-      <c r="P10" s="28">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="24">
-        <v>12</v>
-      </c>
-      <c r="C11" s="25">
-        <v>416349</v>
-      </c>
-      <c r="D11" s="25">
-        <v>91952</v>
-      </c>
-      <c r="E11" s="25">
-        <v>3016487</v>
-      </c>
-      <c r="F11" s="25">
-        <v>3524788</v>
-      </c>
-      <c r="G11" s="25">
-        <v>293732</v>
-      </c>
-      <c r="H11" s="25">
-        <v>299174</v>
-      </c>
-      <c r="I11" s="25">
-        <v>187451</v>
-      </c>
-      <c r="J11" s="28">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="K11" s="34">
-        <v>11742000000</v>
-      </c>
-      <c r="L11" s="34">
-        <v>115000000</v>
-      </c>
-      <c r="M11" s="28">
-        <v>0.01</v>
-      </c>
-      <c r="N11" s="26">
-        <v>39975</v>
-      </c>
-      <c r="O11" s="26">
-        <v>-1832</v>
-      </c>
-      <c r="P11" s="28">
-        <v>-4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="24">
-        <v>12</v>
-      </c>
-      <c r="C12" s="25">
-        <v>356677</v>
-      </c>
-      <c r="D12" s="25">
-        <v>67089</v>
-      </c>
-      <c r="E12" s="25">
-        <v>2913571</v>
-      </c>
-      <c r="F12" s="25">
-        <v>3337337</v>
-      </c>
-      <c r="G12" s="25">
-        <v>278111</v>
-      </c>
-      <c r="H12" s="25">
-        <v>280507</v>
-      </c>
-      <c r="I12" s="25">
-        <v>84633</v>
-      </c>
-      <c r="J12" s="28">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K12" s="34">
-        <v>11627000000</v>
-      </c>
-      <c r="L12" s="34">
-        <v>979000000</v>
-      </c>
-      <c r="M12" s="28">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="N12" s="26">
-        <v>41807</v>
-      </c>
-      <c r="O12" s="26">
-        <v>2524</v>
-      </c>
-      <c r="P12" s="28">
-        <v>6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="24">
-        <v>12</v>
-      </c>
-      <c r="C13" s="25">
-        <v>271573</v>
-      </c>
-      <c r="D13" s="25">
-        <v>65494</v>
-      </c>
-      <c r="E13" s="25">
-        <v>2915637</v>
-      </c>
-      <c r="F13" s="25">
-        <v>3252704</v>
-      </c>
-      <c r="G13" s="25">
-        <v>271059</v>
-      </c>
-      <c r="H13" s="25">
-        <v>270785</v>
-      </c>
-      <c r="I13" s="25">
-        <v>61573</v>
-      </c>
-      <c r="J13" s="28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="K13" s="34">
-        <v>10648000000</v>
-      </c>
-      <c r="L13" s="34">
-        <v>-539000000</v>
-      </c>
-      <c r="M13" s="28">
-        <v>-4.8000000000000001E-2</v>
-      </c>
-      <c r="N13" s="26">
-        <v>39283</v>
-      </c>
-      <c r="O13" s="26">
-        <v>-2785</v>
-      </c>
-      <c r="P13" s="28">
-        <v>-6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="24">
-        <v>12</v>
-      </c>
-      <c r="C14" s="25">
-        <v>211114</v>
-      </c>
-      <c r="D14" s="25">
-        <v>68522</v>
-      </c>
-      <c r="E14" s="25">
-        <v>2911495</v>
-      </c>
-      <c r="F14" s="25">
-        <v>3191131</v>
-      </c>
-      <c r="G14" s="25">
-        <v>265928</v>
-      </c>
-      <c r="H14" s="25">
-        <v>272758</v>
-      </c>
-      <c r="I14" s="25">
-        <v>391265</v>
-      </c>
-      <c r="J14" s="28">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K14" s="34">
-        <v>11187000000</v>
-      </c>
-      <c r="L14" s="34">
-        <v>1517000000</v>
-      </c>
-      <c r="M14" s="28">
-        <v>0.157</v>
-      </c>
-      <c r="N14" s="26">
-        <v>42068</v>
-      </c>
-      <c r="O14" s="26">
-        <v>623</v>
-      </c>
-      <c r="P14" s="28">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="24">
-        <v>12</v>
-      </c>
-      <c r="C15" s="25">
-        <v>146837</v>
-      </c>
-      <c r="D15" s="25">
-        <v>68314</v>
-      </c>
-      <c r="E15" s="25">
-        <v>2584715</v>
-      </c>
-      <c r="F15" s="25">
-        <v>2799866</v>
-      </c>
-      <c r="G15" s="25">
-        <v>233322</v>
-      </c>
-      <c r="H15" s="25">
-        <v>240219</v>
-      </c>
-      <c r="I15" s="25">
-        <v>359451</v>
-      </c>
-      <c r="J15" s="28">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="K15" s="34">
-        <v>9670000000</v>
-      </c>
-      <c r="L15" s="34">
-        <v>465000000</v>
-      </c>
-      <c r="M15" s="28">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="N15" s="26">
-        <v>41445</v>
-      </c>
-      <c r="O15" s="26">
-        <v>-3818</v>
-      </c>
-      <c r="P15" s="28">
-        <v>-8.4000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
+        <v>(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = 5.</v>
+      </c>
+      <c r="H23" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="24">
-        <v>12</v>
-      </c>
-      <c r="C16" s="25">
-        <v>102280</v>
-      </c>
-      <c r="D16" s="25">
-        <v>67591</v>
-      </c>
-      <c r="E16" s="25">
-        <v>2270544</v>
-      </c>
-      <c r="F16" s="25">
-        <v>2440415</v>
-      </c>
-      <c r="G16" s="25">
-        <v>203368</v>
-      </c>
-      <c r="H16" s="25">
-        <v>210264</v>
-      </c>
-      <c r="I16" s="25">
-        <v>352109</v>
-      </c>
-      <c r="J16" s="28">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="K16" s="34">
-        <v>9205000000</v>
-      </c>
-      <c r="L16" s="34">
-        <v>921000000</v>
-      </c>
-      <c r="M16" s="28">
-        <v>0.111</v>
-      </c>
-      <c r="N16" s="26">
-        <v>45263</v>
-      </c>
-      <c r="O16" s="26">
-        <v>-2339</v>
-      </c>
-      <c r="P16" s="28">
-        <v>-4.9000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+    </row>
+    <row r="24" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>_xlfn.CONCAT("(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H26*100,2),"%")</f>
+        <v>(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = 0.57%</v>
+      </c>
+      <c r="H24" s="12">
+        <v>6.8599999999999994E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="24">
-        <v>12</v>
-      </c>
-      <c r="C17" s="25">
-        <v>74966</v>
-      </c>
-      <c r="D17" s="25">
-        <v>66883</v>
-      </c>
-      <c r="E17" s="25">
-        <v>1946457</v>
-      </c>
-      <c r="F17" s="25">
-        <v>2088306</v>
-      </c>
-      <c r="G17" s="25">
-        <v>174026</v>
-      </c>
-      <c r="H17" s="25">
-        <v>181219</v>
-      </c>
-      <c r="I17" s="25">
-        <v>353466</v>
-      </c>
-      <c r="J17" s="28">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="K17" s="34">
-        <v>8284000000</v>
-      </c>
-      <c r="L17" s="34">
-        <v>436000000</v>
-      </c>
-      <c r="M17" s="28">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="N17" s="26">
-        <v>47602</v>
-      </c>
-      <c r="O17" s="26">
-        <v>-6683</v>
-      </c>
-      <c r="P17" s="28">
-        <v>-0.123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="24">
-        <v>12</v>
-      </c>
-      <c r="C18" s="25">
-        <v>71979</v>
-      </c>
-      <c r="D18" s="25">
-        <v>65736</v>
-      </c>
-      <c r="E18" s="25">
-        <v>1597125</v>
-      </c>
-      <c r="F18" s="25">
-        <v>1734840</v>
-      </c>
-      <c r="G18" s="25">
-        <v>144570</v>
-      </c>
-      <c r="H18" s="25">
-        <v>148887</v>
-      </c>
-      <c r="I18" s="25">
-        <v>121067</v>
-      </c>
-      <c r="J18" s="28">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="K18" s="34">
-        <v>7848000000</v>
-      </c>
-      <c r="L18" s="34">
-        <v>371000000</v>
-      </c>
-      <c r="M18" s="28">
-        <v>0.05</v>
-      </c>
-      <c r="N18" s="26">
-        <v>54285</v>
-      </c>
-      <c r="O18" s="26">
-        <v>-1314</v>
-      </c>
-      <c r="P18" s="28">
-        <v>-2.4E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="24">
-        <v>12</v>
-      </c>
-      <c r="C19" s="25">
-        <v>68552</v>
-      </c>
-      <c r="D19" s="25">
-        <v>67476</v>
-      </c>
-      <c r="E19" s="25">
-        <v>1477745</v>
-      </c>
-      <c r="F19" s="25">
-        <v>1613773</v>
-      </c>
-      <c r="G19" s="25">
-        <v>134481</v>
-      </c>
-      <c r="H19" s="25">
-        <v>138251</v>
-      </c>
-      <c r="I19" s="25">
-        <v>243287</v>
-      </c>
-      <c r="J19" s="28">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="K19" s="34">
-        <v>7477000000</v>
-      </c>
-      <c r="L19" s="34">
-        <v>3076000000</v>
-      </c>
-      <c r="M19" s="28">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="N19" s="26">
-        <v>55599</v>
-      </c>
-      <c r="O19" s="26">
-        <v>17064</v>
-      </c>
-      <c r="P19" s="28">
-        <v>0.443</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="24">
-        <v>12</v>
-      </c>
-      <c r="C20" s="25">
-        <v>53408</v>
-      </c>
-      <c r="D20" s="25">
-        <v>62026</v>
-      </c>
-      <c r="E20" s="25">
-        <v>1255052</v>
-      </c>
-      <c r="F20" s="25">
-        <v>1370486</v>
-      </c>
-      <c r="G20" s="25">
-        <v>114207</v>
-      </c>
-      <c r="H20" s="25">
-        <v>122486</v>
-      </c>
-      <c r="I20" s="25">
-        <v>570978</v>
-      </c>
-      <c r="J20" s="28">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="K20" s="34">
-        <v>4401000000</v>
-      </c>
-      <c r="L20" s="34">
-        <v>-798000000</v>
-      </c>
-      <c r="M20" s="28">
-        <v>-0.153</v>
-      </c>
-      <c r="N20" s="26">
-        <v>38535</v>
-      </c>
-      <c r="O20" s="26">
-        <v>-39498</v>
-      </c>
-      <c r="P20" s="28">
-        <v>-0.50600000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="24">
-        <v>12</v>
-      </c>
-      <c r="C21" s="25">
-        <v>30299</v>
-      </c>
-      <c r="D21" s="25">
-        <v>54215</v>
-      </c>
-      <c r="E21" s="25">
-        <v>714994</v>
-      </c>
-      <c r="F21" s="25">
-        <v>799508</v>
-      </c>
-      <c r="G21" s="25">
-        <v>66626</v>
-      </c>
-      <c r="H21" s="25">
-        <v>74300</v>
-      </c>
-      <c r="I21" s="25">
-        <v>302327</v>
-      </c>
-      <c r="J21" s="28">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="K21" s="34">
-        <v>5199000000</v>
-      </c>
-      <c r="L21" s="34">
-        <v>482621000</v>
-      </c>
-      <c r="M21" s="28">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="N21" s="26">
-        <v>78033</v>
-      </c>
-      <c r="O21" s="26">
-        <v>-35802</v>
-      </c>
-      <c r="P21" s="28">
-        <v>-0.315</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="24">
-        <v>12</v>
-      </c>
-      <c r="C22" s="25">
-        <v>19050</v>
-      </c>
-      <c r="D22" s="25">
-        <v>46774</v>
-      </c>
-      <c r="E22" s="25">
-        <v>431357</v>
-      </c>
-      <c r="F22" s="25">
-        <v>497181</v>
-      </c>
-      <c r="G22" s="25">
-        <v>41432</v>
-      </c>
-      <c r="H22" s="25">
-        <v>45071</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="K22" s="34">
-        <v>4716379000</v>
-      </c>
-      <c r="L22" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="M22" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="N22" s="26">
-        <v>113835</v>
-      </c>
-      <c r="O22" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P22" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
-        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
-        <v>(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = 3.</v>
-      </c>
-      <c r="H26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
-        <f>_xlfn.CONCAT("(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H29*100,2),"%")</f>
-        <v>(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = 0.14%</v>
-      </c>
-      <c r="H27" s="14">
-        <v>6.8599999999999994E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="H29" s="14">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>57</v>
+    </row>
+    <row r="26" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="H26" s="12">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:P22">
-    <sortCondition descending="1" ref="A9:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:P19">
+    <sortCondition descending="1" ref="A9:A19"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
@@ -4875,7 +4659,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4896,267 +4680,267 @@
   <sheetData>
     <row r="1" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P2" s="62" t="s">
+      <c r="P2" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="62"/>
+    </row>
+    <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="65"/>
+    </row>
+    <row r="4" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P4" s="14"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="15"/>
+    </row>
+    <row r="5" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="59"/>
+    </row>
+    <row r="6" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="17">
+        <f>AVERAGE(projection_data!E11)</f>
+        <v>0.10171695</v>
+      </c>
+      <c r="R6" s="17"/>
+      <c r="S6" s="15"/>
+    </row>
+    <row r="7" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="17">
+        <f>AVERAGE(projection_data!E9:E11)</f>
+        <v>6.1308563333333337E-2</v>
+      </c>
+      <c r="R7" s="17"/>
+      <c r="S7" s="15"/>
+    </row>
+    <row r="8" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="17">
+        <f>AVERAGE(projection_data!E7:E11)</f>
+        <v>6.8592358000000006E-2</v>
+      </c>
+      <c r="R8" s="17"/>
+      <c r="S8" s="15"/>
+    </row>
+    <row r="9" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P9" s="14"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="15"/>
+    </row>
+    <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="59"/>
+    </row>
+    <row r="11" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="42">
+        <f>AVERAGE(projection_data!G11)</f>
+        <v>5.6807370000000003E-2</v>
+      </c>
+      <c r="R11" s="42"/>
+      <c r="S11" s="15"/>
+    </row>
+    <row r="12" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="42">
+        <f>AVERAGE(projection_data!G9:G11)</f>
+        <v>1.1049426666666667E-2</v>
+      </c>
+      <c r="R12" s="42"/>
+      <c r="S12" s="15"/>
+    </row>
+    <row r="13" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="42">
+        <f>AVERAGE(projection_data!G7:G11)</f>
+        <v>5.7460459999999994E-3</v>
+      </c>
+      <c r="R13" s="42"/>
+      <c r="S13" s="15"/>
+    </row>
+    <row r="14" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P14" s="14"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="15"/>
+    </row>
+    <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="56"/>
+    </row>
+    <row r="16" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="P16" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="64"/>
-    </row>
-    <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P3" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="67"/>
-    </row>
-    <row r="4" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P4" s="16"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="17"/>
-    </row>
-    <row r="5" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="61"/>
-    </row>
-    <row r="6" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="19">
-        <f>AVERAGE(projection_data!O14)</f>
-        <v>0.10176623588849699</v>
-      </c>
-      <c r="R6" s="19"/>
-      <c r="S6" s="17"/>
-    </row>
-    <row r="7" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="19">
-        <f>AVERAGE(projection_data!O12:O14)</f>
-        <v>6.1316977536269246E-2</v>
-      </c>
-      <c r="R7" s="19"/>
-      <c r="S7" s="17"/>
-    </row>
-    <row r="8" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="19">
-        <f>AVERAGE(projection_data!O10:O14)</f>
-        <v>6.8598483323739995E-2</v>
-      </c>
-      <c r="R8" s="19"/>
-      <c r="S8" s="17"/>
-    </row>
-    <row r="9" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P9" s="16"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="17"/>
-    </row>
-    <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P10" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="61"/>
-    </row>
-    <row r="11" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q11" s="44">
-        <f>AVERAGE(projection_data!R14)</f>
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="R11" s="44"/>
-      <c r="S11" s="17"/>
-    </row>
-    <row r="12" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q12" s="44">
-        <f>AVERAGE(projection_data!R12:R14)</f>
-        <v>1.9333333333333334E-2</v>
-      </c>
-      <c r="R12" s="44"/>
-      <c r="S12" s="17"/>
-    </row>
-    <row r="13" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q13" s="44">
-        <f>AVERAGE(projection_data!R10:R14)</f>
-        <v>1.3999999999999998E-3</v>
-      </c>
-      <c r="R13" s="44"/>
-      <c r="S13" s="17"/>
-    </row>
-    <row r="14" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P14" s="16"/>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="17"/>
-    </row>
-    <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="58"/>
-    </row>
-    <row r="16" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P16" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="17"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="15"/>
     </row>
     <row r="17" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P17" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="55"/>
+      <c r="P17" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="53"/>
     </row>
     <row r="18" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P18" s="53"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="55"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="53"/>
     </row>
     <row r="19" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P19" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q19" s="43"/>
-      <c r="R19" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="S19" s="17"/>
+      <c r="P19" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="S19" s="15"/>
     </row>
     <row r="20" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P20" s="15">
+      <c r="P20" s="13">
         <v>6.8599999999999994E-2</v>
       </c>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="47">
-        <v>1.4E-3</v>
-      </c>
-      <c r="S20" s="7"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="45">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="S20" s="6"/>
     </row>
     <row r="21" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P21" s="6"/>
-      <c r="S21" s="7"/>
+      <c r="P21" s="5"/>
+      <c r="S21" s="6"/>
     </row>
     <row r="22" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P22" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="S22" s="7"/>
+      <c r="P22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="S22" s="6"/>
     </row>
     <row r="23" spans="16:19" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q23" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="R23" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="S23" s="41" t="s">
-        <v>6</v>
+      <c r="P23" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="R23" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="S23" s="39" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P24" s="9" t="str" cm="1">
-        <f t="array" ref="P24:P28">projection_data!B15:B19</f>
+      <c r="P24" s="8" t="str" cm="1">
+        <f t="array" ref="P24:P28">projection_data!B12:B16</f>
         <v>FY25</v>
       </c>
-      <c r="Q24" s="46" cm="1">
-        <f t="array" ref="Q24:Q28">projection_data!N15:N19</f>
-        <v>345824.60639999999</v>
-      </c>
-      <c r="R24" s="35" cm="1">
-        <f t="array" ref="R24:R28">projection_data!P15:P19</f>
-        <v>41551.090200000006</v>
-      </c>
-      <c r="S24" s="37" cm="1">
-        <f t="array" ref="S24:S28">projection_data!K15:K19</f>
-        <v>14369389413.905899</v>
+      <c r="Q24" s="44" cm="1">
+        <f t="array" ref="Q24:Q28">projection_data!D12:D16</f>
+        <v>345815.60878800001</v>
+      </c>
+      <c r="R24" s="33" cm="1">
+        <f t="array" ref="R24:R28">projection_data!F12:F16</f>
+        <v>27549.753577000003</v>
+      </c>
+      <c r="S24" s="35" cm="1">
+        <f t="array" ref="S24:S28">projection_data!C12:C16</f>
+        <v>9527134805.1896362</v>
       </c>
     </row>
     <row r="25" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P25" s="9" t="str">
+      <c r="P25" s="8" t="str">
         <v>FY26</v>
       </c>
-      <c r="Q25" s="46">
-        <v>369548.17439904</v>
-      </c>
-      <c r="R25" s="35">
-        <v>41609.261726280012</v>
-      </c>
-      <c r="S25" s="37">
-        <v>15376626709.038626</v>
+      <c r="Q25" s="44">
+        <v>369538.55955085682</v>
+      </c>
+      <c r="R25" s="33">
+        <v>27706.787172388904</v>
+      </c>
+      <c r="S25" s="35">
+        <v>10238726221.466753</v>
       </c>
     </row>
     <row r="26" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P26" s="9" t="str">
+      <c r="P26" s="8" t="str">
         <v>FY27</v>
       </c>
-      <c r="Q26" s="46">
-        <v>394899.17916281417</v>
-      </c>
-      <c r="R26" s="35">
-        <v>41667.514692696808</v>
-      </c>
-      <c r="S26" s="37">
-        <v>16454467349.900469</v>
+      <c r="Q26" s="44">
+        <v>394888.90473604557</v>
+      </c>
+      <c r="R26" s="33">
+        <v>27864.71585927152</v>
+      </c>
+      <c r="S26" s="35">
+        <v>11003467126.448851</v>
       </c>
     </row>
     <row r="27" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P27" s="9" t="str">
+      <c r="P27" s="8" t="str">
         <v>FY28</v>
       </c>
-      <c r="Q27" s="46">
-        <v>421989.2628533832</v>
-      </c>
-      <c r="R27" s="35">
-        <v>41725.849213266585</v>
-      </c>
-      <c r="S27" s="37">
-        <v>17607860351.437786</v>
+      <c r="Q27" s="44">
+        <v>421978.28360093827</v>
+      </c>
+      <c r="R27" s="33">
+        <v>28023.544739669371</v>
+      </c>
+      <c r="S27" s="35">
+        <v>11825327309.659784</v>
       </c>
     </row>
     <row r="28" spans="16:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P28" s="10" t="str">
+      <c r="P28" s="9" t="str">
         <v>FY29</v>
       </c>
-      <c r="Q28" s="11">
-        <v>450937.7262851253</v>
-      </c>
-      <c r="R28" s="36">
-        <v>41784.265402165162</v>
-      </c>
-      <c r="S28" s="38">
-        <v>18842101634.946587</v>
+      <c r="Q28" s="10">
+        <v>450925.99385596265</v>
+      </c>
+      <c r="R28" s="34">
+        <v>28183.278944685488</v>
+      </c>
+      <c r="S28" s="36">
+        <v>12708573068.252131</v>
       </c>
     </row>
     <row r="29" spans="16:19" x14ac:dyDescent="0.2"/>
@@ -5197,937 +4981,384 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EC6393-3785-8B4D-BC33-531ADF13ED6E}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31" customWidth="1"/>
-    <col min="16" max="16" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="66" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="C1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="D1" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="G1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3471000000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>134481.07999999999</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0.17751877999999999</v>
+      </c>
+      <c r="F2" s="3">
+        <v>25810.32</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3793000000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>144570</v>
+      </c>
+      <c r="E3" s="18">
+        <v>7.5021080000000004E-2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>26236.43</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.6509039999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4612000000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>174025.5</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.20374559</v>
+      </c>
+      <c r="F4" s="3">
+        <v>26501.86</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.011715E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5812000000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>203367.92</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.16860987</v>
+      </c>
+      <c r="F5" s="3">
+        <v>28578.75</v>
+      </c>
+      <c r="G5" s="2">
+        <v>7.8367419999999993E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6285000000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>233322.17</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.14729092999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>26937</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-5.7446270000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7765000000</v>
+      </c>
+      <c r="D7" s="1">
+        <v>265927.58</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.13974418999999999</v>
+      </c>
+      <c r="F7" s="3">
+        <v>29199.68</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8.3998779999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7215000000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>271057.83</v>
+      </c>
+      <c r="E8" s="18">
+        <v>1.9291909999999999E-2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>26617.94</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-8.8416830000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7697000000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>278112.42</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2.602612E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>27675.86</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3.9744750000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7614000000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>293737.5</v>
+      </c>
+      <c r="E10" s="18">
+        <v>5.6182620000000003E-2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>25921.1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-6.3403840000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8865000000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>323615.58</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.10171695</v>
+      </c>
+      <c r="F11" s="3">
+        <v>27393.61</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5.6807370000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="30">
+        <f>D12*F12</f>
+        <v>9527134805.1896362</v>
+      </c>
+      <c r="D12" s="31">
+        <f>(1+Graph!$P$20)*D11</f>
+        <v>345815.60878800001</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30">
+        <f>(1+Graph!$R$20)*F11</f>
+        <v>27549.753577000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="30">
+        <f>D13*F13</f>
+        <v>10238726221.466753</v>
+      </c>
+      <c r="D13" s="31">
+        <f>(1+Graph!$P$20)*D12</f>
+        <v>369538.55955085682</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30">
+        <f>(1+Graph!$R$20)*F12</f>
+        <v>27706.787172388904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
-        <v>19050</v>
-      </c>
-      <c r="E2" s="2">
-        <v>46774</v>
-      </c>
-      <c r="F2" s="2">
-        <v>431357</v>
-      </c>
-      <c r="G2" s="2">
-        <v>497181</v>
-      </c>
-      <c r="H2" s="3">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="K2" s="4">
-        <v>4716379000</v>
-      </c>
-      <c r="N2" s="2">
-        <v>41432</v>
-      </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="4">
-        <v>113835</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2">
-        <v>30299</v>
-      </c>
-      <c r="E3" s="2">
-        <v>54215</v>
-      </c>
-      <c r="F3" s="2">
-        <v>714994</v>
-      </c>
-      <c r="G3" s="2">
-        <v>799508</v>
-      </c>
-      <c r="H3" s="3">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="I3" s="2">
-        <v>302327</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="K3" s="4">
-        <v>5199000000</v>
-      </c>
-      <c r="L3" s="4">
-        <v>482621000</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="N3" s="2">
-        <v>66626</v>
-      </c>
-      <c r="O3" s="20">
-        <f>(N3-N2)/N2</f>
-        <v>0.60808071056188451</v>
-      </c>
-      <c r="P3" s="4">
-        <v>78033</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>-35802</v>
-      </c>
-      <c r="R3" s="3">
-        <v>-0.315</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
-        <v>53408</v>
-      </c>
-      <c r="E4" s="2">
-        <v>62026</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1255052</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1370486</v>
-      </c>
-      <c r="H4" s="3">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>570978</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="K4" s="4">
-        <v>4401000000</v>
-      </c>
-      <c r="L4" s="4">
-        <v>-798000000</v>
-      </c>
-      <c r="M4" s="3">
-        <v>-0.153</v>
-      </c>
-      <c r="N4" s="2">
-        <v>114207</v>
-      </c>
-      <c r="O4" s="20">
-        <f t="shared" ref="O4:O14" si="0">(N4-N3)/N3</f>
-        <v>0.71415063188545014</v>
-      </c>
-      <c r="P4" s="4">
-        <v>38535</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>-39498</v>
-      </c>
-      <c r="R4" s="3">
-        <v>-0.50600000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2">
-        <v>68552</v>
-      </c>
-      <c r="E5" s="2">
-        <v>67476</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1477745</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1613773</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>243287</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="K5" s="4">
-        <v>7477000000</v>
-      </c>
-      <c r="L5" s="4">
-        <v>3076000000</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="N5" s="2">
-        <v>134481</v>
-      </c>
-      <c r="O5" s="20">
-        <f t="shared" si="0"/>
-        <v>0.17751976673934172</v>
-      </c>
-      <c r="P5" s="4">
-        <v>55599</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>17064</v>
-      </c>
-      <c r="R5" s="3">
-        <v>0.443</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2">
-        <v>71979</v>
-      </c>
-      <c r="E6" s="2">
-        <v>65736</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1597125</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1734840</v>
-      </c>
-      <c r="H6" s="3">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="I6" s="2">
-        <v>121067</v>
-      </c>
-      <c r="J6" s="3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="K6" s="4">
-        <v>7848000000</v>
-      </c>
-      <c r="L6" s="4">
-        <v>371000000</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="N6" s="2">
-        <v>144570</v>
-      </c>
-      <c r="O6" s="20">
-        <f t="shared" si="0"/>
-        <v>7.50217502844268E-2</v>
-      </c>
-      <c r="P6" s="4">
-        <v>54285</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>-1314</v>
-      </c>
-      <c r="R6" s="3">
-        <v>-2.4E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2">
-        <v>74966</v>
-      </c>
-      <c r="E7" s="2">
-        <v>66883</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1946457</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2088306</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1.9E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>353466</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="K7" s="4">
-        <v>8284000000</v>
-      </c>
-      <c r="L7" s="4">
-        <v>436000000</v>
-      </c>
-      <c r="M7" s="3">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="N7" s="2">
-        <v>174026</v>
-      </c>
-      <c r="O7" s="20">
-        <f t="shared" si="0"/>
-        <v>0.20374904890364529</v>
-      </c>
-      <c r="P7" s="4">
-        <v>47602</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>-6683</v>
-      </c>
-      <c r="R7" s="3">
-        <v>-0.123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2">
-        <v>102280</v>
-      </c>
-      <c r="E8" s="2">
-        <v>67591</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2270544</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2440415</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1.4E-2</v>
-      </c>
-      <c r="I8" s="2">
-        <v>352109</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="K8" s="4">
-        <v>9205000000</v>
-      </c>
-      <c r="L8" s="4">
-        <v>921000000</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0.111</v>
-      </c>
-      <c r="N8" s="2">
-        <v>203368</v>
-      </c>
-      <c r="O8" s="20">
-        <f t="shared" si="0"/>
-        <v>0.16860698976015079</v>
-      </c>
-      <c r="P8" s="4">
-        <v>45263</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>-2339</v>
-      </c>
-      <c r="R8" s="3">
-        <v>-4.9000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2">
-        <v>146837</v>
-      </c>
-      <c r="E9" s="2">
-        <v>68314</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2584715</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2799866</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I9" s="2">
-        <v>359451</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="K9" s="4">
-        <v>9670000000</v>
-      </c>
-      <c r="L9" s="4">
-        <v>465000000</v>
-      </c>
-      <c r="M9" s="3">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="N9" s="2">
-        <v>233322</v>
-      </c>
-      <c r="O9" s="20">
-        <f t="shared" si="0"/>
-        <v>0.14728964242161993</v>
-      </c>
-      <c r="P9" s="4">
-        <v>41445</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>-3818</v>
-      </c>
-      <c r="R9" s="3">
-        <v>-8.4000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2">
-        <v>211114</v>
-      </c>
-      <c r="E10" s="2">
-        <v>68522</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2911495</v>
-      </c>
-      <c r="G10" s="2">
-        <v>3191131</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1.2E-2</v>
-      </c>
-      <c r="I10" s="2">
-        <v>391265</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K10" s="4">
-        <v>11187000000</v>
-      </c>
-      <c r="L10" s="4">
-        <v>1517000000</v>
-      </c>
-      <c r="M10" s="3">
-        <v>0.157</v>
-      </c>
-      <c r="N10" s="2">
-        <v>265928</v>
-      </c>
-      <c r="O10" s="20">
-        <f t="shared" si="0"/>
-        <v>0.1397467877011169</v>
-      </c>
-      <c r="P10" s="4">
-        <v>42068</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>623</v>
-      </c>
-      <c r="R10" s="3">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2">
-        <v>271573</v>
-      </c>
-      <c r="E11" s="2">
-        <v>65494</v>
-      </c>
-      <c r="F11" s="2">
-        <v>2915637</v>
-      </c>
-      <c r="G11" s="2">
-        <v>3252704</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>61573</v>
-      </c>
-      <c r="J11" s="3">
-        <v>1.9E-2</v>
-      </c>
-      <c r="K11" s="4">
-        <v>10648000000</v>
-      </c>
-      <c r="L11" s="4">
-        <v>-539000000</v>
-      </c>
-      <c r="M11" s="3">
-        <v>-4.8000000000000001E-2</v>
-      </c>
-      <c r="N11" s="2">
-        <v>271059</v>
-      </c>
-      <c r="O11" s="20">
-        <f t="shared" si="0"/>
-        <v>1.9294696308775307E-2</v>
-      </c>
-      <c r="P11" s="4">
-        <v>39283</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>-2785</v>
-      </c>
-      <c r="R11" s="3">
-        <v>-6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>356677</v>
-      </c>
-      <c r="E12" s="2">
-        <v>67089</v>
-      </c>
-      <c r="F12" s="2">
-        <v>2913571</v>
-      </c>
-      <c r="G12" s="2">
-        <v>3337337</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I12" s="2">
-        <v>84633</v>
-      </c>
-      <c r="J12" s="3">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K12" s="4">
-        <v>11627000000</v>
-      </c>
-      <c r="L12" s="4">
-        <v>979000000</v>
-      </c>
-      <c r="M12" s="3">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="N12" s="2">
-        <v>278111</v>
-      </c>
-      <c r="O12" s="20">
-        <f t="shared" si="0"/>
-        <v>2.6016476117745584E-2</v>
-      </c>
-      <c r="P12" s="4">
-        <v>41807</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>2524</v>
-      </c>
-      <c r="R12" s="3">
-        <v>6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2">
-        <v>416349</v>
-      </c>
-      <c r="E13" s="2">
-        <v>91952</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3016487</v>
-      </c>
-      <c r="G13" s="2">
-        <v>3524788</v>
-      </c>
-      <c r="H13" s="3">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="I13" s="2">
-        <v>187451</v>
-      </c>
-      <c r="J13" s="3">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="K13" s="4">
-        <v>11742000000</v>
-      </c>
-      <c r="L13" s="4">
-        <v>115000000</v>
-      </c>
-      <c r="M13" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="N13" s="2">
-        <v>293732</v>
-      </c>
-      <c r="O13" s="20">
-        <f t="shared" si="0"/>
-        <v>5.6168220602565162E-2</v>
-      </c>
-      <c r="P13" s="4">
-        <v>39975</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>-1832</v>
-      </c>
-      <c r="R13" s="3">
-        <v>-4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14" s="2">
-        <v>493725</v>
-      </c>
-      <c r="E14" s="2">
-        <v>111461</v>
-      </c>
-      <c r="F14" s="2">
-        <v>3278306</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3883492</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="I14" s="2">
-        <v>358704</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="K14" s="4">
-        <v>13428000000</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1686000000</v>
-      </c>
-      <c r="M14" s="3">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="N14" s="2">
-        <v>323624</v>
-      </c>
-      <c r="O14" s="20">
-        <f t="shared" si="0"/>
-        <v>0.10176623588849699</v>
-      </c>
-      <c r="P14" s="4">
-        <v>41493</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>1517</v>
-      </c>
-      <c r="R14" s="3">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="31">
-        <f>(1+Graph!$P$20)*G14</f>
-        <v>4149899.5512000001</v>
-      </c>
-      <c r="K15" s="32">
-        <f>N15*P15</f>
-        <v>14369389413.905899</v>
-      </c>
-      <c r="N15" s="33">
-        <f>(1+Graph!$P$20)*N14</f>
-        <v>345824.60639999999</v>
-      </c>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32">
-        <f>(1+Graph!$R$20)*P14</f>
-        <v>41551.090200000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="31">
-        <f>(1+Graph!$P$20)*G15</f>
-        <v>4434582.6604123199</v>
-      </c>
-      <c r="K16" s="32">
-        <f>N16*P16</f>
-        <v>15376626709.038626</v>
-      </c>
-      <c r="N16" s="33">
-        <f>(1+Graph!$P$20)*N15</f>
-        <v>369548.17439904</v>
-      </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32">
-        <f>(1+Graph!$R$20)*P15</f>
-        <v>41609.261726280012</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="31">
-        <f>(1+Graph!$P$20)*G16</f>
-        <v>4738795.0309166051</v>
-      </c>
-      <c r="K17" s="32">
-        <f t="shared" ref="K17:K19" si="1">N17*P17</f>
-        <v>16454467349.900469</v>
-      </c>
-      <c r="N17" s="33">
-        <f>(1+Graph!$P$20)*N16</f>
-        <v>394899.17916281417</v>
-      </c>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32">
-        <f>(1+Graph!$R$20)*P16</f>
-        <v>41667.514692696808</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="31">
-        <f>(1+Graph!$P$20)*G17</f>
-        <v>5063876.370037484</v>
-      </c>
-      <c r="K18" s="32">
-        <f t="shared" si="1"/>
-        <v>17607860351.437786</v>
-      </c>
-      <c r="N18" s="33">
-        <f>(1+Graph!$P$20)*N17</f>
-        <v>421989.2628533832</v>
-      </c>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32">
-        <f>(1+Graph!$R$20)*P17</f>
-        <v>41725.849213266585</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="31">
-        <f>(1+Graph!$P$20)*G18</f>
-        <v>5411258.2890220555</v>
-      </c>
-      <c r="K19" s="32">
-        <f t="shared" si="1"/>
-        <v>18842101634.946587</v>
-      </c>
-      <c r="N19" s="33">
-        <f>(1+Graph!$P$20)*N18</f>
-        <v>450937.7262851253</v>
-      </c>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32">
-        <f>(1+Graph!$R$20)*P18</f>
-        <v>41784.265402165162</v>
+      <c r="C14" s="30">
+        <f>D14*F14</f>
+        <v>11003467126.448851</v>
+      </c>
+      <c r="D14" s="31">
+        <f>(1+Graph!$P$20)*D13</f>
+        <v>394888.90473604557</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30">
+        <f>(1+Graph!$R$20)*F13</f>
+        <v>27864.71585927152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="30">
+        <f>D15*F15</f>
+        <v>11825327309.659784</v>
+      </c>
+      <c r="D15" s="31">
+        <f>(1+Graph!$P$20)*D14</f>
+        <v>421978.28360093827</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30">
+        <f>(1+Graph!$R$20)*F14</f>
+        <v>28023.544739669371</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="30">
+        <f>D16*F16</f>
+        <v>12708573068.252131</v>
+      </c>
+      <c r="D16" s="31">
+        <f>(1+Graph!$P$20)*D15</f>
+        <v>450925.99385596265</v>
+      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30">
+        <f>(1+Graph!$R$20)*F15</f>
+        <v>28183.278944685488</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:R15">
-    <sortCondition ref="B2:B15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G12">
+    <sortCondition ref="B2:B12"/>
   </sortState>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 4/05/2025 at 3:11pm
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342C446-A9E4-314E-AF3F-35DE71579B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3568D740-3573-8B47-A215-BFE41A7319EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -177,21 +177,6 @@
   </si>
   <si>
     <t>State Spending Annual Change (Millions)</t>
-  </si>
-  <si>
-    <t>FY25</t>
-  </si>
-  <si>
-    <t>FY26</t>
-  </si>
-  <si>
-    <t>FY27</t>
-  </si>
-  <si>
-    <t>FY28</t>
-  </si>
-  <si>
-    <t>FY29</t>
   </si>
   <si>
     <t>Average Annual Growth Rates (as of FY24)</t>
@@ -1029,7 +1014,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1100,6 +1085,12 @@
     <xf numFmtId="10" fontId="14" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1136,11 +1127,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1157,7 +1151,57 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1295,6 +1339,75 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001A-EC81-CF44-920D-19D254A97AA7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-EC81-CF44-920D-19D254A97AA7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-EC81-CF44-920D-19D254A97AA7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
             <c:invertIfNegative val="0"/>
@@ -1488,7 +1601,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>134481.07999999999</c:v>
+                  <c:v>134481.08333333299</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>144570</c:v>
@@ -1497,40 +1610,40 @@
                   <c:v>174025.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>203367.92</c:v>
+                  <c:v>203367.91666666599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>233322.17</c:v>
+                  <c:v>233322.16666666599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>265927.58</c:v>
+                  <c:v>265927.58333333302</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>271057.83</c:v>
+                  <c:v>271057.83333333302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>278112.42</c:v>
+                  <c:v>278112.41666666599</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>293737.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>323615.58</c:v>
+                  <c:v>323615.58333333302</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>345815.60878800001</c:v>
+                  <c:v>345815.61234999966</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>369538.55955085682</c:v>
+                  <c:v>369538.56335720961</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>394888.90473604557</c:v>
+                  <c:v>394888.9088035142</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>421978.28360093827</c:v>
+                  <c:v>421978.28794743528</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>450925.99385596265</c:v>
+                  <c:v>450925.99850062933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1888,19 +2001,19 @@
                   <c:v>8865000000</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>9527134805.1896362</c:v>
+                  <c:v>9527135892.2999687</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>10238726221.466753</c:v>
+                  <c:v>10238727389.774464</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>11003467126.448851</c:v>
+                  <c:v>11003468382.018658</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>11825327309.659784</c:v>
+                  <c:v>11825328659.00938</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>12708573068.252131</c:v>
+                  <c:v>12708574518.386024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3277,6 +3390,22 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}" name="Table1" displayName="Table1" ref="A1:G11" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:G11" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{5930A738-8B59-6A4E-919B-090BCB11A0AA}" name="Data  Type"/>
+    <tableColumn id="2" xr3:uid="{BC5DD464-CE62-C145-9541-0E916FE9BF25}" name="Fiscal Year"/>
+    <tableColumn id="3" xr3:uid="{1858EE94-CA04-2649-B52D-6343C025BC1C}" name="State Spending" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{2A994CA5-E802-1241-A0A7-341CFD69AFD6}" name="Average Annual Enrollment" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{410693AE-0DD9-F340-BB48-7F49D2049665}" name="Average Annual Enrollment Change %" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{4B0D0AC8-F08E-7544-9AF6-BC3DA742F6F2}" name="Average Annual Spending per Enrollee" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{F8434FAD-6E36-6344-9152-D139B9351C1D}" name="Average Annual Spending per Enrollee Annual Change %" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -3579,48 +3708,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
+      <c r="A1" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
     </row>
     <row r="2" spans="1:16" s="11" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="46" t="s">
+      <c r="C2" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="47" t="s">
+      <c r="J2" s="48"/>
+      <c r="K2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="48" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
     </row>
     <row r="3" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
@@ -3630,22 +3759,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>2</v>
@@ -3674,7 +3803,7 @@
     </row>
     <row r="4" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="23">
@@ -3691,42 +3820,42 @@
       </c>
       <c r="F4" s="23">
         <f>G4*12</f>
-        <v>5411111.9262715522</v>
+        <v>5411111.9820075519</v>
       </c>
       <c r="G4" s="23">
         <f t="shared" ref="G4:G6" si="2">G5*(1+$H$24)</f>
-        <v>450925.99385596265</v>
+        <v>450925.99850062933</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I4" s="23">
         <f>F4-F5</f>
-        <v>347372.52306029294</v>
+        <v>347372.52663832903</v>
       </c>
       <c r="J4" s="25">
         <f t="shared" ref="J4:J6" si="3">I4/F5</f>
-        <v>6.8600000000000105E-2</v>
+        <v>6.8600000000000064E-2</v>
       </c>
       <c r="K4" s="32">
         <f t="shared" ref="K4:K6" si="4">N4*G4</f>
-        <v>12708573068.252131</v>
+        <v>12708574518.386024</v>
       </c>
       <c r="L4" s="32">
         <f t="shared" ref="L4:L6" si="5">K4-K5</f>
-        <v>883245758.59234619</v>
+        <v>883245859.37664413</v>
       </c>
       <c r="M4" s="26">
         <f t="shared" ref="M4:M6" si="6">L4/K5</f>
-        <v>7.4691020000000094E-2</v>
+        <v>7.4691020000000108E-2</v>
       </c>
       <c r="N4" s="24">
         <f t="shared" ref="N4:N6" si="7">(1+P4)*N5</f>
-        <v>28183.278944685488</v>
+        <v>28183.281870291823</v>
       </c>
       <c r="O4" s="24">
         <f t="shared" ref="O4:O6" si="8">N4-N5</f>
-        <v>159.7342050161169</v>
+        <v>159.73422159755864</v>
       </c>
       <c r="P4" s="25">
         <f>$H$26</f>
@@ -3735,7 +3864,7 @@
     </row>
     <row r="5" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="23">
@@ -3752,42 +3881,42 @@
       </c>
       <c r="F5" s="23">
         <f t="shared" ref="F5:F8" si="9">G5*12</f>
-        <v>5063739.4032112593</v>
+        <v>5063739.4553692229</v>
       </c>
       <c r="G5" s="23">
         <f t="shared" si="2"/>
-        <v>421978.28360093827</v>
+        <v>421978.28794743528</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I5" s="23">
         <f>F5-F6</f>
-        <v>325072.54637871217</v>
+        <v>325072.54972705245</v>
       </c>
       <c r="J5" s="25">
         <f t="shared" si="3"/>
-        <v>6.8599999999999883E-2</v>
+        <v>6.8599999999999911E-2</v>
       </c>
       <c r="K5" s="32">
         <f>N5*G5</f>
-        <v>11825327309.659784</v>
+        <v>11825328659.00938</v>
       </c>
       <c r="L5" s="32">
         <f t="shared" si="5"/>
-        <v>821860183.21093369</v>
+        <v>821860276.99072266</v>
       </c>
       <c r="M5" s="26">
         <f t="shared" si="6"/>
-        <v>7.4691020000000011E-2</v>
+        <v>7.4691019999999955E-2</v>
       </c>
       <c r="N5" s="24">
         <f t="shared" si="7"/>
-        <v>28023.544739669371</v>
+        <v>28023.547648694264</v>
       </c>
       <c r="O5" s="24">
         <f t="shared" si="8"/>
-        <v>158.8288803978503</v>
+        <v>158.82889688531213</v>
       </c>
       <c r="P5" s="25">
         <f>$H$26</f>
@@ -3796,7 +3925,7 @@
     </row>
     <row r="6" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="23">
@@ -3813,42 +3942,42 @@
       </c>
       <c r="F6" s="23">
         <f t="shared" si="9"/>
-        <v>4738666.8568325471</v>
+        <v>4738666.9056421705</v>
       </c>
       <c r="G6" s="23">
         <f t="shared" si="2"/>
-        <v>394888.90473604557</v>
+        <v>394888.9088035142</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I6" s="23">
         <f t="shared" ref="I6" si="10">F6-F7</f>
-        <v>304204.14222226478</v>
+        <v>304204.14535565488</v>
       </c>
       <c r="J6" s="25">
         <f t="shared" si="3"/>
-        <v>6.8599999999999869E-2</v>
+        <v>6.859999999999998E-2</v>
       </c>
       <c r="K6" s="32">
         <f t="shared" si="4"/>
-        <v>11003467126.448851</v>
+        <v>11003468382.018658</v>
       </c>
       <c r="L6" s="32">
         <f t="shared" si="5"/>
-        <v>764740904.98209763</v>
+        <v>764740992.24419403</v>
       </c>
       <c r="M6" s="26">
         <f t="shared" si="6"/>
-        <v>7.4691019999999997E-2</v>
+        <v>7.4691020000000177E-2</v>
       </c>
       <c r="N6" s="24">
         <f t="shared" si="7"/>
-        <v>27864.71585927152</v>
+        <v>27864.718751808952</v>
       </c>
       <c r="O6" s="24">
         <f t="shared" si="8"/>
-        <v>157.9286868826166</v>
+        <v>157.92870327663695</v>
       </c>
       <c r="P6" s="25">
         <f>$H$26</f>
@@ -3874,42 +4003,42 @@
       </c>
       <c r="F7" s="23">
         <f t="shared" si="9"/>
-        <v>4434462.7146102823</v>
+        <v>4434462.7602865156</v>
       </c>
       <c r="G7" s="23">
         <f>G8*(1+$H$24)</f>
-        <v>369538.55955085682</v>
+        <v>369538.56335720961</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I7" s="23">
         <f>F7-F8</f>
-        <v>284675.40915428195</v>
+        <v>284675.41208651941</v>
       </c>
       <c r="J7" s="25">
         <f>I7/F8</f>
-        <v>6.8600000000000078E-2</v>
+        <v>6.8599999999999925E-2</v>
       </c>
       <c r="K7" s="32">
         <f>N7*G7</f>
-        <v>10238726221.466753</v>
+        <v>10238727389.774464</v>
       </c>
       <c r="L7" s="32">
         <f>K7-K8</f>
-        <v>711591416.27711678</v>
+        <v>711591497.47449493</v>
       </c>
       <c r="M7" s="26">
         <f>L7/K8</f>
-        <v>7.4691020000000163E-2</v>
+        <v>7.4691020000000011E-2</v>
       </c>
       <c r="N7" s="24">
         <f>(1+P7)*N8</f>
-        <v>27706.787172388904</v>
+        <v>27706.790048532315</v>
       </c>
       <c r="O7" s="24">
         <f>N7-N8</f>
-        <v>157.03359538890072</v>
+        <v>157.03361169000345</v>
       </c>
       <c r="P7" s="25">
         <f>$H$26</f>
@@ -3935,42 +4064,42 @@
       </c>
       <c r="F8" s="23">
         <f t="shared" si="9"/>
-        <v>4149787.3054560004</v>
+        <v>4149787.3481999962</v>
       </c>
       <c r="G8" s="23">
         <f>G10*(1+$H$24)</f>
-        <v>345815.60878800001</v>
+        <v>345815.61234999966</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I8" s="23">
         <f>F8-F10</f>
-        <v>266400.30545600038</v>
+        <v>266400.34819999617</v>
       </c>
       <c r="J8" s="26">
         <f>I8/F10</f>
-        <v>6.8599988993113578E-2</v>
+        <v>6.8599999999999009E-2</v>
       </c>
       <c r="K8" s="32">
         <f>N8*G8</f>
-        <v>9527134805.1896362</v>
+        <v>9527135892.2999687</v>
       </c>
       <c r="L8" s="32">
         <f>K8-K10</f>
-        <v>662134805.18963623</v>
+        <v>662135892.29996872</v>
       </c>
       <c r="M8" s="26">
         <f>L8/K10</f>
-        <v>7.4690897370517345E-2</v>
+        <v>7.4691019999996472E-2</v>
       </c>
       <c r="N8" s="24">
         <f>(1+P8)*N10</f>
-        <v>27549.753577000003</v>
+        <v>27549.756436842312</v>
       </c>
       <c r="O8" s="24">
         <f>N8-N10</f>
-        <v>156.14357700000255</v>
+        <v>156.14359320871154</v>
       </c>
       <c r="P8" s="25">
         <f>$H$26</f>
@@ -4002,29 +4131,29 @@
       <c r="H9" s="23">
         <v>358404</v>
       </c>
-      <c r="I9" s="27">
-        <v>-2127439</v>
-      </c>
-      <c r="J9" s="27">
-        <v>-0.54783079999999995</v>
+      <c r="I9" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="L9" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="M9" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="O9" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="P9" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -4047,7 +4176,7 @@
         <v>3883387</v>
       </c>
       <c r="G10" s="23">
-        <v>323615.58</v>
+        <v>323615.58333333302</v>
       </c>
       <c r="H10" s="23">
         <v>331687</v>
@@ -4056,7 +4185,7 @@
         <v>358537</v>
       </c>
       <c r="J10" s="26">
-        <v>0.10171695</v>
+        <v>0.10171695249443199</v>
       </c>
       <c r="K10" s="32">
         <v>8865000000</v>
@@ -4065,16 +4194,16 @@
         <v>1251000000</v>
       </c>
       <c r="M10" s="26">
-        <v>0.16430259999999999</v>
+        <v>0.164302600472813</v>
       </c>
       <c r="N10" s="24">
-        <v>27393.61</v>
+        <v>27393.6128436336</v>
       </c>
       <c r="O10" s="24">
-        <v>1472.5098</v>
+        <v>1472.50981797299</v>
       </c>
       <c r="P10" s="26">
-        <v>5.6807370000000003E-2</v>
+        <v>5.6807374922096497E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -4106,7 +4235,7 @@
         <v>187501</v>
       </c>
       <c r="J11" s="26">
-        <v>5.6182620000000003E-2</v>
+        <v>5.6182616801539097E-2</v>
       </c>
       <c r="K11" s="32">
         <v>7614000000</v>
@@ -4115,16 +4244,16 @@
         <v>-83000000</v>
       </c>
       <c r="M11" s="26">
-        <v>-1.078342E-2</v>
+        <v>-1.07834221125113E-2</v>
       </c>
       <c r="N11" s="24">
-        <v>25921.1</v>
+        <v>25921.103025660599</v>
       </c>
       <c r="O11" s="24">
-        <v>-1754.7559000000001</v>
+        <v>-1754.7558671311799</v>
       </c>
       <c r="P11" s="26">
-        <v>-6.3403840000000003E-2</v>
+        <v>-6.3403844987380095E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -4147,7 +4276,7 @@
         <v>3337349</v>
       </c>
       <c r="G12" s="23">
-        <v>278112.42</v>
+        <v>278112.41666666599</v>
       </c>
       <c r="H12" s="23">
         <v>280508</v>
@@ -4156,7 +4285,7 @@
         <v>84655</v>
       </c>
       <c r="J12" s="26">
-        <v>2.602612E-2</v>
+        <v>2.60261186573345E-2</v>
       </c>
       <c r="K12" s="32">
         <v>7697000000</v>
@@ -4165,16 +4294,16 @@
         <v>482000000</v>
       </c>
       <c r="M12" s="26">
-        <v>6.680527E-2</v>
+        <v>6.68052668052668E-2</v>
       </c>
       <c r="N12" s="24">
-        <v>27675.86</v>
+        <v>27675.858892791799</v>
       </c>
       <c r="O12" s="24">
-        <v>1057.9231</v>
+        <v>1057.9231140189199</v>
       </c>
       <c r="P12" s="26">
-        <v>3.9744750000000002E-2</v>
+        <v>3.9744746655471098E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -4197,7 +4326,7 @@
         <v>3252694</v>
       </c>
       <c r="G13" s="23">
-        <v>271057.83</v>
+        <v>271057.83333333302</v>
       </c>
       <c r="H13" s="23">
         <v>270784</v>
@@ -4206,7 +4335,7 @@
         <v>61563</v>
       </c>
       <c r="J13" s="26">
-        <v>1.9291909999999999E-2</v>
+        <v>1.92919062238435E-2</v>
       </c>
       <c r="K13" s="32">
         <v>7215000000</v>
@@ -4215,16 +4344,16 @@
         <v>-550000000</v>
       </c>
       <c r="M13" s="26">
-        <v>-7.0830649999999995E-2</v>
+        <v>-7.0830650354153202E-2</v>
       </c>
       <c r="N13" s="24">
-        <v>26617.94</v>
+        <v>26617.935778772899</v>
       </c>
       <c r="O13" s="24">
-        <v>-2581.7429999999999</v>
+        <v>-2581.7429558199201</v>
       </c>
       <c r="P13" s="26">
-        <v>-8.8416830000000002E-2</v>
+        <v>-8.8416827434520201E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -4247,7 +4376,7 @@
         <v>3191131</v>
       </c>
       <c r="G14" s="23">
-        <v>265927.58</v>
+        <v>265927.58333333302</v>
       </c>
       <c r="H14" s="23">
         <v>272758</v>
@@ -4256,7 +4385,7 @@
         <v>391265</v>
       </c>
       <c r="J14" s="26">
-        <v>0.13974418999999999</v>
+        <v>0.13974418775755601</v>
       </c>
       <c r="K14" s="32">
         <v>7765000000</v>
@@ -4265,16 +4394,16 @@
         <v>1480000000</v>
       </c>
       <c r="M14" s="26">
-        <v>0.2354813</v>
+        <v>0.235481304693715</v>
       </c>
       <c r="N14" s="24">
-        <v>29199.68</v>
+        <v>29199.678734592799</v>
       </c>
       <c r="O14" s="24">
-        <v>2262.6752999999999</v>
+        <v>2262.6753208580399</v>
       </c>
       <c r="P14" s="26">
-        <v>8.3998779999999995E-2</v>
+        <v>8.3998776185488302E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -4297,7 +4426,7 @@
         <v>2799866</v>
       </c>
       <c r="G15" s="23">
-        <v>233322.17</v>
+        <v>233322.16666666599</v>
       </c>
       <c r="H15" s="23">
         <v>240219</v>
@@ -4306,7 +4435,7 @@
         <v>359451</v>
       </c>
       <c r="J15" s="26">
-        <v>0.14729092999999999</v>
+        <v>0.14729093207507701</v>
       </c>
       <c r="K15" s="32">
         <v>6285000000</v>
@@ -4315,16 +4444,16 @@
         <v>473000000</v>
       </c>
       <c r="M15" s="26">
-        <v>8.1383339999999998E-2</v>
+        <v>8.1383344803853994E-2</v>
       </c>
       <c r="N15" s="24">
-        <v>26937</v>
+        <v>26937.003413734801</v>
       </c>
       <c r="O15" s="24">
-        <v>-1641.7424000000001</v>
+        <v>-1641.7424143313201</v>
       </c>
       <c r="P15" s="26">
-        <v>-5.7446270000000001E-2</v>
+        <v>-5.7446272282495797E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -4347,7 +4476,7 @@
         <v>2440415</v>
       </c>
       <c r="G16" s="23">
-        <v>203367.92</v>
+        <v>203367.91666666599</v>
       </c>
       <c r="H16" s="23">
         <v>210264</v>
@@ -4356,7 +4485,7 @@
         <v>352109</v>
       </c>
       <c r="J16" s="26">
-        <v>0.16860987</v>
+        <v>0.168609868477129</v>
       </c>
       <c r="K16" s="32">
         <v>5812000000</v>
@@ -4365,16 +4494,16 @@
         <v>1200000000</v>
       </c>
       <c r="M16" s="26">
-        <v>0.26019080999999999</v>
+        <v>0.26019080659150001</v>
       </c>
       <c r="N16" s="24">
-        <v>28578.75</v>
+        <v>28578.745828066101</v>
       </c>
       <c r="O16" s="24">
-        <v>2076.8825999999999</v>
+        <v>2076.8825953789601</v>
       </c>
       <c r="P16" s="26">
-        <v>7.8367419999999993E-2</v>
+        <v>7.8367418062038702E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -4406,7 +4535,7 @@
         <v>353466</v>
       </c>
       <c r="J17" s="26">
-        <v>0.20374559</v>
+        <v>0.20374559037144599</v>
       </c>
       <c r="K17" s="32">
         <v>4612000000</v>
@@ -4415,16 +4544,16 @@
         <v>819000000</v>
       </c>
       <c r="M17" s="26">
-        <v>0.21592407</v>
+        <v>0.21592407065647201</v>
       </c>
       <c r="N17" s="24">
-        <v>26501.86</v>
+        <v>26501.863232687101</v>
       </c>
       <c r="O17" s="24">
-        <v>265.43799999999999</v>
+        <v>265.437971567982</v>
       </c>
       <c r="P17" s="26">
-        <v>1.011715E-2</v>
+        <v>1.01171546400166E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -4456,7 +4585,7 @@
         <v>121067</v>
       </c>
       <c r="J18" s="26">
-        <v>7.5021080000000004E-2</v>
+        <v>7.5021084130171903E-2</v>
       </c>
       <c r="K18" s="32">
         <v>3793000000</v>
@@ -4465,16 +4594,16 @@
         <v>322000000</v>
       </c>
       <c r="M18" s="26">
-        <v>9.2768649999999994E-2</v>
+        <v>9.2768654566407302E-2</v>
       </c>
       <c r="N18" s="24">
-        <v>26236.43</v>
+        <v>26236.4252611191</v>
       </c>
       <c r="O18" s="24">
-        <v>426.1037</v>
+        <v>426.10373510530098</v>
       </c>
       <c r="P18" s="26">
-        <v>1.6509039999999999E-2</v>
+        <v>1.6509044053396899E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -4497,50 +4626,50 @@
         <v>1613773</v>
       </c>
       <c r="G19" s="23">
-        <v>134481.07999999999</v>
+        <v>134481.08333333299</v>
       </c>
       <c r="H19" s="23">
         <v>138251</v>
       </c>
-      <c r="I19" s="23">
-        <v>243287</v>
-      </c>
-      <c r="J19" s="26">
-        <v>0.17751877999999999</v>
+      <c r="I19" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="69" t="s">
+        <v>68</v>
       </c>
       <c r="K19" s="32">
         <v>3471000000</v>
       </c>
-      <c r="L19" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="M19" s="26" t="s">
-        <v>73</v>
+      <c r="L19" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="69" t="s">
+        <v>68</v>
       </c>
       <c r="N19" s="24">
-        <v>25810.32</v>
-      </c>
-      <c r="O19" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="P19" s="26" t="s">
-        <v>73</v>
+        <v>25810.321526013799</v>
+      </c>
+      <c r="O19" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" s="69" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
@@ -4573,67 +4702,67 @@
     </row>
     <row r="28" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -4659,7 +4788,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4680,20 +4809,20 @@
   <sheetData>
     <row r="1" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P2" s="60" t="s">
+      <c r="P2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="62"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="64"/>
     </row>
     <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P3" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="65"/>
+      <c r="P3" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="67"/>
     </row>
     <row r="4" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P4" s="14"/>
@@ -4702,12 +4831,12 @@
       <c r="S4" s="15"/>
     </row>
     <row r="5" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="57" t="s">
+      <c r="P5" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="59"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="61"/>
     </row>
     <row r="6" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P6" s="7" t="s">
@@ -4715,7 +4844,7 @@
       </c>
       <c r="Q6" s="17">
         <f>AVERAGE(projection_data!E11)</f>
-        <v>0.10171695</v>
+        <v>0.10171695249443199</v>
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="15"/>
@@ -4726,7 +4855,7 @@
       </c>
       <c r="Q7" s="17">
         <f>AVERAGE(projection_data!E9:E11)</f>
-        <v>6.1308563333333337E-2</v>
+        <v>6.1308562651101899E-2</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="15"/>
@@ -4737,7 +4866,7 @@
       </c>
       <c r="Q8" s="17">
         <f>AVERAGE(projection_data!E7:E11)</f>
-        <v>6.8592358000000006E-2</v>
+        <v>6.8592356386941028E-2</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="15"/>
@@ -4749,12 +4878,12 @@
       <c r="S9" s="15"/>
     </row>
     <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P10" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="59"/>
+      <c r="P10" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="61"/>
     </row>
     <row r="11" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P11" s="7" t="s">
@@ -4762,7 +4891,7 @@
       </c>
       <c r="Q11" s="42">
         <f>AVERAGE(projection_data!G11)</f>
-        <v>5.6807370000000003E-2</v>
+        <v>5.6807374922096497E-2</v>
       </c>
       <c r="R11" s="42"/>
       <c r="S11" s="15"/>
@@ -4773,7 +4902,7 @@
       </c>
       <c r="Q12" s="42">
         <f>AVERAGE(projection_data!G9:G11)</f>
-        <v>1.1049426666666667E-2</v>
+        <v>1.1049425530062501E-2</v>
       </c>
       <c r="R12" s="42"/>
       <c r="S12" s="15"/>
@@ -4784,7 +4913,7 @@
       </c>
       <c r="Q13" s="42">
         <f>AVERAGE(projection_data!G7:G11)</f>
-        <v>5.7460459999999994E-3</v>
+        <v>5.7460450682311204E-3</v>
       </c>
       <c r="R13" s="42"/>
       <c r="S13" s="15"/>
@@ -4796,12 +4925,12 @@
       <c r="S14" s="15"/>
     </row>
     <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="54" t="s">
+      <c r="P15" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="55"/>
-      <c r="S15" s="56"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="58"/>
     </row>
     <row r="16" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="P16" s="37" t="s">
@@ -4812,18 +4941,18 @@
       <c r="S16" s="15"/>
     </row>
     <row r="17" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P17" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="53"/>
+      <c r="P17" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="55"/>
     </row>
     <row r="18" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P18" s="51"/>
-      <c r="Q18" s="52"/>
-      <c r="R18" s="52"/>
-      <c r="S18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="55"/>
     </row>
     <row r="19" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P19" s="16" t="s">
@@ -4831,7 +4960,7 @@
       </c>
       <c r="Q19" s="41"/>
       <c r="R19" s="40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="S19" s="15"/>
     </row>
@@ -4851,7 +4980,7 @@
     </row>
     <row r="22" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P22" s="37" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="S22" s="6"/>
     </row>
@@ -4876,15 +5005,15 @@
       </c>
       <c r="Q24" s="44" cm="1">
         <f t="array" ref="Q24:Q28">projection_data!D12:D16</f>
-        <v>345815.60878800001</v>
+        <v>345815.61234999966</v>
       </c>
       <c r="R24" s="33" cm="1">
         <f t="array" ref="R24:R28">projection_data!F12:F16</f>
-        <v>27549.753577000003</v>
+        <v>27549.756436842312</v>
       </c>
       <c r="S24" s="35" cm="1">
         <f t="array" ref="S24:S28">projection_data!C12:C16</f>
-        <v>9527134805.1896362</v>
+        <v>9527135892.2999687</v>
       </c>
     </row>
     <row r="25" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4892,13 +5021,13 @@
         <v>FY26</v>
       </c>
       <c r="Q25" s="44">
-        <v>369538.55955085682</v>
+        <v>369538.56335720961</v>
       </c>
       <c r="R25" s="33">
-        <v>27706.787172388904</v>
+        <v>27706.790048532315</v>
       </c>
       <c r="S25" s="35">
-        <v>10238726221.466753</v>
+        <v>10238727389.774464</v>
       </c>
     </row>
     <row r="26" spans="16:19" ht="16" x14ac:dyDescent="0.2">
@@ -4906,13 +5035,13 @@
         <v>FY27</v>
       </c>
       <c r="Q26" s="44">
-        <v>394888.90473604557</v>
+        <v>394888.9088035142</v>
       </c>
       <c r="R26" s="33">
-        <v>27864.71585927152</v>
+        <v>27864.718751808952</v>
       </c>
       <c r="S26" s="35">
-        <v>11003467126.448851</v>
+        <v>11003468382.018658</v>
       </c>
     </row>
     <row r="27" spans="16:19" ht="16" x14ac:dyDescent="0.2">
@@ -4920,13 +5049,13 @@
         <v>FY28</v>
       </c>
       <c r="Q27" s="44">
-        <v>421978.28360093827</v>
+        <v>421978.28794743528</v>
       </c>
       <c r="R27" s="33">
-        <v>28023.544739669371</v>
+        <v>28023.547648694264</v>
       </c>
       <c r="S27" s="35">
-        <v>11825327309.659784</v>
+        <v>11825328659.00938</v>
       </c>
     </row>
     <row r="28" spans="16:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4934,13 +5063,13 @@
         <v>FY29</v>
       </c>
       <c r="Q28" s="10">
-        <v>450925.99385596265</v>
+        <v>450925.99850062933</v>
       </c>
       <c r="R28" s="34">
-        <v>28183.278944685488</v>
+        <v>28183.281870291823</v>
       </c>
       <c r="S28" s="36">
-        <v>12708573068.252131</v>
+        <v>12708574518.386024</v>
       </c>
     </row>
     <row r="29" spans="16:19" x14ac:dyDescent="0.2"/>
@@ -4973,7 +5102,7 @@
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="Q12:Q13" formulaRange="1"/>
+    <ignoredError sqref="Q12:Q13 Q7:Q8" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4984,39 +5113,40 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="66" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="66" t="s">
+      <c r="E1" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="46" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5031,16 +5161,16 @@
         <v>3471000000</v>
       </c>
       <c r="D2" s="1">
-        <v>134481.07999999999</v>
-      </c>
-      <c r="E2" s="18">
-        <v>0.17751877999999999</v>
+        <v>134481.08333333299</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="F2" s="3">
-        <v>25810.32</v>
+        <v>25810.321526013799</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -5057,13 +5187,13 @@
         <v>144570</v>
       </c>
       <c r="E3" s="18">
-        <v>7.5021080000000004E-2</v>
+        <v>7.5021084130171806E-2</v>
       </c>
       <c r="F3" s="3">
-        <v>26236.43</v>
+        <v>26236.4252611191</v>
       </c>
       <c r="G3" s="2">
-        <v>1.6509039999999999E-2</v>
+        <v>1.6509044053396899E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -5080,13 +5210,13 @@
         <v>174025.5</v>
       </c>
       <c r="E4" s="18">
-        <v>0.20374559</v>
+        <v>0.20374559037144599</v>
       </c>
       <c r="F4" s="3">
-        <v>26501.86</v>
+        <v>26501.863232687101</v>
       </c>
       <c r="G4" s="2">
-        <v>1.011715E-2</v>
+        <v>1.01171546400166E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -5100,16 +5230,16 @@
         <v>5812000000</v>
       </c>
       <c r="D5" s="1">
-        <v>203367.92</v>
+        <v>203367.91666666599</v>
       </c>
       <c r="E5" s="18">
-        <v>0.16860987</v>
+        <v>0.168609868477129</v>
       </c>
       <c r="F5" s="3">
-        <v>28578.75</v>
+        <v>28578.745828066101</v>
       </c>
       <c r="G5" s="2">
-        <v>7.8367419999999993E-2</v>
+        <v>7.8367418062038702E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -5123,16 +5253,16 @@
         <v>6285000000</v>
       </c>
       <c r="D6" s="1">
-        <v>233322.17</v>
+        <v>233322.16666666599</v>
       </c>
       <c r="E6" s="18">
-        <v>0.14729092999999999</v>
+        <v>0.14729093207507701</v>
       </c>
       <c r="F6" s="3">
-        <v>26937</v>
+        <v>26937.003413734801</v>
       </c>
       <c r="G6" s="2">
-        <v>-5.7446270000000001E-2</v>
+        <v>-5.7446272282495797E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5146,16 +5276,16 @@
         <v>7765000000</v>
       </c>
       <c r="D7" s="1">
-        <v>265927.58</v>
+        <v>265927.58333333302</v>
       </c>
       <c r="E7" s="18">
-        <v>0.13974418999999999</v>
+        <v>0.13974418775755601</v>
       </c>
       <c r="F7" s="3">
-        <v>29199.68</v>
+        <v>29199.678734592799</v>
       </c>
       <c r="G7" s="2">
-        <v>8.3998779999999995E-2</v>
+        <v>8.3998776185488302E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5169,16 +5299,16 @@
         <v>7215000000</v>
       </c>
       <c r="D8" s="1">
-        <v>271057.83</v>
+        <v>271057.83333333302</v>
       </c>
       <c r="E8" s="18">
-        <v>1.9291909999999999E-2</v>
+        <v>1.92919062238435E-2</v>
       </c>
       <c r="F8" s="3">
-        <v>26617.94</v>
+        <v>26617.935778772899</v>
       </c>
       <c r="G8" s="2">
-        <v>-8.8416830000000002E-2</v>
+        <v>-8.8416827434520201E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -5192,16 +5322,16 @@
         <v>7697000000</v>
       </c>
       <c r="D9" s="1">
-        <v>278112.42</v>
+        <v>278112.41666666599</v>
       </c>
       <c r="E9" s="18">
-        <v>2.602612E-2</v>
+        <v>2.6026118657334601E-2</v>
       </c>
       <c r="F9" s="3">
-        <v>27675.86</v>
+        <v>27675.858892791799</v>
       </c>
       <c r="G9" s="2">
-        <v>3.9744750000000002E-2</v>
+        <v>3.9744746655471098E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -5218,13 +5348,13 @@
         <v>293737.5</v>
       </c>
       <c r="E10" s="18">
-        <v>5.6182620000000003E-2</v>
+        <v>5.6182616801539097E-2</v>
       </c>
       <c r="F10" s="3">
-        <v>25921.1</v>
+        <v>25921.103025660599</v>
       </c>
       <c r="G10" s="2">
-        <v>-6.3403840000000003E-2</v>
+        <v>-6.3403844987380095E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -5238,121 +5368,126 @@
         <v>8865000000</v>
       </c>
       <c r="D11" s="1">
-        <v>323615.58</v>
+        <v>323615.58333333302</v>
       </c>
       <c r="E11" s="18">
-        <v>0.10171695</v>
+        <v>0.10171695249443199</v>
       </c>
       <c r="F11" s="3">
-        <v>27393.61</v>
+        <v>27393.6128436336</v>
       </c>
       <c r="G11" s="2">
-        <v>5.6807370000000003E-2</v>
+        <v>5.6807374922096497E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>40</v>
+      <c r="B12" s="29" t="str" cm="1">
+        <f t="array" ref="B12">CONCATENATE("FY",RIGHT(INDEX(Table1[],ROWS(Table1[]),2),2)+1)</f>
+        <v>FY25</v>
       </c>
       <c r="C12" s="30">
         <f>D12*F12</f>
-        <v>9527134805.1896362</v>
-      </c>
-      <c r="D12" s="31">
-        <f>(1+Graph!$P$20)*D11</f>
-        <v>345815.60878800001</v>
+        <v>9527135892.2999687</v>
+      </c>
+      <c r="D12" s="31" cm="1">
+        <f t="array" ref="D12">(1+Graph!$P$20)*INDEX(Table1[],ROWS(Table1[]),4)</f>
+        <v>345815.61234999966</v>
       </c>
       <c r="E12" s="30"/>
-      <c r="F12" s="30">
-        <f>(1+Graph!$R$20)*F11</f>
-        <v>27549.753577000003</v>
+      <c r="F12" s="30" cm="1">
+        <f t="array" ref="F12">(1+Graph!$R$20)*INDEX(Table1[],ROWS(Table1[]),6)</f>
+        <v>27549.756436842312</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>41</v>
+      <c r="B13" s="29" t="str">
+        <f>CONCATENATE("FY",RIGHT(B12,2)+1)</f>
+        <v>FY26</v>
       </c>
       <c r="C13" s="30">
         <f>D13*F13</f>
-        <v>10238726221.466753</v>
+        <v>10238727389.774464</v>
       </c>
       <c r="D13" s="31">
         <f>(1+Graph!$P$20)*D12</f>
-        <v>369538.55955085682</v>
+        <v>369538.56335720961</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30">
         <f>(1+Graph!$R$20)*F12</f>
-        <v>27706.787172388904</v>
+        <v>27706.790048532315</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>42</v>
+      <c r="B14" s="29" t="str">
+        <f t="shared" ref="B14:B16" si="0">CONCATENATE("FY",RIGHT(B13,2)+1)</f>
+        <v>FY27</v>
       </c>
       <c r="C14" s="30">
         <f>D14*F14</f>
-        <v>11003467126.448851</v>
+        <v>11003468382.018658</v>
       </c>
       <c r="D14" s="31">
         <f>(1+Graph!$P$20)*D13</f>
-        <v>394888.90473604557</v>
+        <v>394888.9088035142</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30">
         <f>(1+Graph!$R$20)*F13</f>
-        <v>27864.71585927152</v>
+        <v>27864.718751808952</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>43</v>
+      <c r="B15" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>FY28</v>
       </c>
       <c r="C15" s="30">
         <f>D15*F15</f>
-        <v>11825327309.659784</v>
+        <v>11825328659.00938</v>
       </c>
       <c r="D15" s="31">
         <f>(1+Graph!$P$20)*D14</f>
-        <v>421978.28360093827</v>
+        <v>421978.28794743528</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30">
         <f>(1+Graph!$R$20)*F14</f>
-        <v>28023.544739669371</v>
+        <v>28023.547648694264</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="29" t="s">
-        <v>44</v>
+      <c r="B16" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>FY29</v>
       </c>
       <c r="C16" s="30">
         <f>D16*F16</f>
-        <v>12708573068.252131</v>
+        <v>12708574518.386024</v>
       </c>
       <c r="D16" s="31">
         <f>(1+Graph!$P$20)*D15</f>
-        <v>450925.99385596265</v>
+        <v>450925.99850062933</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30">
         <f>(1+Graph!$R$20)*F15</f>
-        <v>28183.278944685488</v>
+        <v>28183.281870291823</v>
       </c>
     </row>
   </sheetData>
@@ -5362,5 +5497,8 @@
   </sortState>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 7/16/2025 at 2:46am
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3568D740-3573-8B47-A215-BFE41A7319EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116FCDC-A708-604F-8F56-4372C577A83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>FY25 (Estimate)(1)(2)</t>
-  </si>
-  <si>
-    <t>FY25 (YTD)</t>
   </si>
   <si>
     <t>FY24</t>
@@ -521,12 +518,18 @@
   <si>
     <t>You can forecast projected enrollment and State spending by changing the two inputs below:</t>
   </si>
+  <si>
+    <t>FY26 (YTD)</t>
+  </si>
+  <si>
+    <t>FY25</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -534,6 +537,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0,,_);[Red]\(&quot;$&quot;#,##0,,\)"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1014,10 +1018,9 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1091,6 +1094,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1127,13 +1139,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1153,10 +1163,10 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -1177,12 +1187,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1201,10 +1205,17 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC7D8EA"/>
       <color rgb="FFF2DCDB"/>
       <color rgb="FFE4DFEC"/>
       <color rgb="FFEBF1DE"/>
@@ -1345,11 +1356,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                  <a:alpha val="80000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C7D8EA"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1543,9 +1550,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>projection_data!$B$2:$B$16</c:f>
+              <c:f>projection_data!$B$2:$B$17</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>FY15</c:v>
                 </c:pt>
@@ -1590,60 +1597,66 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>FY29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>FY30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>projection_data!$D$2:$D$16</c:f>
+              <c:f>projection_data!$D$2:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>134481.08333333299</c:v>
+                  <c:v>135152.91666666599</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>144570</c:v>
+                  <c:v>144672</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174025.5</c:v>
+                  <c:v>175045.33333333299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>203367.91666666599</c:v>
+                  <c:v>204796.83333333299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>233322.16666666599</c:v>
+                  <c:v>234696.41666666599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>265927.58333333302</c:v>
+                  <c:v>267329.33333333302</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>271057.83333333302</c:v>
+                  <c:v>274331.91666666599</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>278112.41666666599</c:v>
+                  <c:v>279188.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>293737.5</c:v>
+                  <c:v>294392.41666666599</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>323615.58333333302</c:v>
+                  <c:v>324988.41666666599</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>345815.61234999966</c:v>
+                  <c:v>363780</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>369538.56335720961</c:v>
+                  <c:v>391718.304</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>394888.9088035142</c:v>
+                  <c:v>421802.26974720001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>421978.28794743528</c:v>
+                  <c:v>454196.68406378495</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>450925.99850062933</c:v>
+                  <c:v>489078.98939988361</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>526640.2557857947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,9 +1926,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>projection_data!$B$2:$B$16</c:f>
+              <c:f>projection_data!$B$2:$B$17</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>FY15</c:v>
                 </c:pt>
@@ -1960,16 +1973,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>FY29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>FY30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>projection_data!$C$2:$C$16</c:f>
+              <c:f>projection_data!$C$2:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>3471000000</c:v>
                 </c:pt>
@@ -2000,20 +2016,23 @@
                 <c:pt idx="9">
                   <c:v>8865000000</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>9527135892.2999687</c:v>
+                <c:pt idx="10">
+                  <c:v>9728000000</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>10238727389.774464</c:v>
+                  <c:v>10495013109.759989</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>11003468382.018658</c:v>
+                  <c:v>11322502073.811075</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>11825328659.00938</c:v>
+                  <c:v>12215235166.522617</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
-                  <c:v>12708574518.386024</c:v>
+                  <c:v>13178356621.243446</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
+                  <c:v>14217416273.133478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3391,16 +3410,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}" name="Table1" displayName="Table1" ref="A1:G11" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:G11" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:G12" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5930A738-8B59-6A4E-919B-090BCB11A0AA}" name="Data  Type"/>
     <tableColumn id="2" xr3:uid="{BC5DD464-CE62-C145-9541-0E916FE9BF25}" name="Fiscal Year"/>
-    <tableColumn id="3" xr3:uid="{1858EE94-CA04-2649-B52D-6343C025BC1C}" name="State Spending" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{2A994CA5-E802-1241-A0A7-341CFD69AFD6}" name="Average Annual Enrollment" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{1858EE94-CA04-2649-B52D-6343C025BC1C}" name="State Spending" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{2A994CA5-E802-1241-A0A7-341CFD69AFD6}" name="Average Annual Enrollment" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{410693AE-0DD9-F340-BB48-7F49D2049665}" name="Average Annual Enrollment Change %" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{4B0D0AC8-F08E-7544-9AF6-BC3DA742F6F2}" name="Average Annual Spending per Enrollee" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F8434FAD-6E36-6344-9152-D139B9351C1D}" name="Average Annual Spending per Enrollee Annual Change %" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{4B0D0AC8-F08E-7544-9AF6-BC3DA742F6F2}" name="Average Annual Spending per Enrollee" dataDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{F8434FAD-6E36-6344-9152-D139B9351C1D}" name="Average Annual Spending per Enrollee Annual Change %" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3693,10 +3712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92772258-4AC4-6B47-AC5E-CDE7A2651A1C}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3708,1066 +3727,1116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+    </row>
+    <row r="2" spans="1:16" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-    </row>
-    <row r="2" spans="1:16" s="11" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="48" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50" t="s">
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-    </row>
-    <row r="3" spans="1:16" s="19" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+    </row>
+    <row r="3" spans="1:16" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="20" t="s">
+      <c r="H3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="P3" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="22">
+        <f>C5*(1+$H$25)</f>
+        <v>907844.24037334672</v>
+      </c>
+      <c r="D4" s="22">
+        <f>D5*(1+$H$25)</f>
+        <v>169210.21776076485</v>
+      </c>
+      <c r="E4" s="22">
+        <f>E5*(1+$H$25)</f>
+        <v>5242628.6112954253</v>
+      </c>
+      <c r="F4" s="22">
+        <f>G4*12</f>
+        <v>6319683.0694295364</v>
+      </c>
+      <c r="G4" s="22">
+        <f>G5*(1+$H$25)</f>
+        <v>526640.2557857947</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="22">
+        <f>F4-F5</f>
+        <v>450735.19663093332</v>
+      </c>
+      <c r="J4" s="24">
+        <f t="shared" ref="J4:J6" si="0">I4/F5</f>
+        <v>7.6800000000000104E-2</v>
+      </c>
+      <c r="K4" s="31">
+        <f t="shared" ref="K4:K6" si="1">N4*G4</f>
+        <v>14217416273.133478</v>
+      </c>
+      <c r="L4" s="31">
+        <f t="shared" ref="L4:L6" si="2">K4-K5</f>
+        <v>1039059651.8900318</v>
+      </c>
+      <c r="M4" s="25">
+        <f t="shared" ref="M4:M6" si="3">L4/K5</f>
+        <v>7.8845920000000055E-2</v>
+      </c>
+      <c r="N4" s="23">
+        <f t="shared" ref="N4:N6" si="4">(1+P4)*N5</f>
+        <v>26996.447986908657</v>
+      </c>
+      <c r="O4" s="23">
+        <f t="shared" ref="O4:O6" si="5">N4-N5</f>
+        <v>51.195978815376293</v>
+      </c>
+      <c r="P4" s="24">
+        <f>$H$27</f>
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="22">
+        <f>C6*(1+$H$25)</f>
+        <v>843094.57686974993</v>
+      </c>
+      <c r="D5" s="22">
+        <f>D6*(1+$H$25)</f>
+        <v>157141.73269016051</v>
+      </c>
+      <c r="E5" s="22">
+        <f>E6*(1+$H$25)</f>
+        <v>4868711.5632386934</v>
+      </c>
+      <c r="F5" s="22">
+        <f t="shared" ref="F5:F8" si="6">G5*12</f>
+        <v>5868947.872798603</v>
+      </c>
+      <c r="G5" s="22">
+        <f>G6*(1+$H$25)</f>
+        <v>489078.98939988361</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="22">
+        <f>F5-F6</f>
+        <v>418587.66403318383</v>
+      </c>
+      <c r="J5" s="24">
+        <f t="shared" si="0"/>
+        <v>7.6799999999999938E-2</v>
+      </c>
+      <c r="K5" s="31">
+        <f>N5*G5</f>
+        <v>13178356621.243446</v>
+      </c>
+      <c r="L5" s="31">
+        <f t="shared" si="2"/>
+        <v>963121454.72082901</v>
+      </c>
+      <c r="M5" s="25">
+        <f t="shared" si="3"/>
+        <v>7.884592E-2</v>
+      </c>
+      <c r="N5" s="23">
+        <f t="shared" si="4"/>
+        <v>26945.252008093281</v>
+      </c>
+      <c r="O5" s="23">
+        <f t="shared" si="5"/>
+        <v>51.098890922625287</v>
+      </c>
+      <c r="P5" s="24">
+        <f>$H$27</f>
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="22">
+        <f>C7*(1+$H$25)</f>
+        <v>782963.01715244236</v>
+      </c>
+      <c r="D6" s="22">
+        <f>D7*(1+$H$25)</f>
+        <v>145934.00138387864</v>
+      </c>
+      <c r="E6" s="22">
+        <f>E7*(1+$H$25)</f>
+        <v>4521463.1902290983</v>
+      </c>
+      <c r="F6" s="22">
+        <f t="shared" si="6"/>
+        <v>5450360.2087654192</v>
+      </c>
+      <c r="G6" s="22">
+        <f>G7*(1+$H$25)</f>
+        <v>454196.68406378495</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="22">
+        <f t="shared" ref="I6" si="7">F6-F7</f>
+        <v>388732.97179901879</v>
+      </c>
+      <c r="J6" s="24">
+        <f t="shared" si="0"/>
+        <v>7.6799999999999854E-2</v>
+      </c>
+      <c r="K6" s="31">
+        <f t="shared" si="1"/>
+        <v>12215235166.522617</v>
+      </c>
+      <c r="L6" s="31">
+        <f t="shared" si="2"/>
+        <v>892733092.71154213</v>
+      </c>
+      <c r="M6" s="25">
+        <f t="shared" si="3"/>
+        <v>7.884592E-2</v>
+      </c>
+      <c r="N6" s="23">
+        <f t="shared" si="4"/>
+        <v>26894.153117170656</v>
+      </c>
+      <c r="O6" s="23">
+        <f t="shared" si="5"/>
+        <v>51.001987147046748</v>
+      </c>
+      <c r="P6" s="24">
+        <f>$H$27</f>
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22">
+        <f>C8*(1+$H$25)</f>
+        <v>727120.18680576002</v>
+      </c>
+      <c r="D7" s="22">
+        <f>D8*(1+$H$25)</f>
+        <v>135525.63278592</v>
+      </c>
+      <c r="E7" s="22">
+        <f>E8*(1+$H$25)</f>
+        <v>4198981.4173747199</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" si="6"/>
+        <v>5061627.2369664004</v>
+      </c>
+      <c r="G7" s="22">
+        <f>G8*(1+$H$25)</f>
+        <v>421802.26974720001</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="22">
+        <f>F7-F8</f>
+        <v>361007.58896640036</v>
+      </c>
+      <c r="J7" s="24">
+        <f>I7/F8</f>
+        <v>7.6800000000000077E-2</v>
+      </c>
+      <c r="K7" s="31">
+        <f>N7*G7</f>
+        <v>11322502073.811075</v>
+      </c>
+      <c r="L7" s="31">
+        <f>K7-K8</f>
+        <v>827488964.05108643</v>
+      </c>
+      <c r="M7" s="25">
+        <f>L7/K8</f>
+        <v>7.8845919999999917E-2</v>
+      </c>
+      <c r="N7" s="23">
+        <f>(1+P7)*N8</f>
+        <v>26843.151130023609</v>
+      </c>
+      <c r="O7" s="23">
+        <f>N7-N8</f>
+        <v>50.905267139478383</v>
+      </c>
+      <c r="P7" s="24">
+        <f>$H$27</f>
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22">
+        <f>C10*(1+$H$25)</f>
+        <v>675260.20319999999</v>
+      </c>
+      <c r="D8" s="22">
+        <f t="shared" ref="C8:D8" si="8">D10*(1+$H$25)</f>
+        <v>125859.61439999999</v>
+      </c>
+      <c r="E8" s="22">
+        <f>E10*(1+$H$25)</f>
+        <v>3899499.8303999999</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="6"/>
+        <v>4700619.648</v>
+      </c>
+      <c r="G8" s="22">
+        <f>G10*(1+$H$25)</f>
+        <v>391718.304</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="22">
+        <f>F8-F10</f>
+        <v>335259.64800000004</v>
+      </c>
+      <c r="J8" s="24">
+        <f>I8/F10</f>
+        <v>7.6800000000000007E-2</v>
+      </c>
+      <c r="K8" s="31">
+        <f>N8*G8</f>
+        <v>10495013109.759989</v>
+      </c>
+      <c r="L8" s="31">
+        <f>K8-K10</f>
+        <v>767013109.75998878</v>
+      </c>
+      <c r="M8" s="25">
+        <f>L8/K10</f>
+        <v>7.8845919999998848E-2</v>
+      </c>
+      <c r="N8" s="23">
+        <f>(1+P8)*N10</f>
+        <v>26792.24586288413</v>
+      </c>
+      <c r="O8" s="23">
+        <f>N8-N10</f>
+        <v>50.808730551430926</v>
+      </c>
+      <c r="P8" s="24">
+        <f>$H$27</f>
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="21">
+        <v>2</v>
+      </c>
+      <c r="C9" s="22">
+        <v>124444</v>
+      </c>
+      <c r="D9" s="22">
+        <v>19567</v>
+      </c>
+      <c r="E9" s="22">
+        <v>611997</v>
+      </c>
+      <c r="F9" s="22">
+        <v>756008</v>
+      </c>
+      <c r="G9" s="22">
+        <v>378004</v>
+      </c>
+      <c r="H9" s="26">
+        <v>378065</v>
+      </c>
+      <c r="I9" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="O9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="P9" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="21">
+        <v>12</v>
+      </c>
+      <c r="C10" s="22">
+        <v>627099</v>
+      </c>
+      <c r="D10" s="22">
+        <v>116883</v>
+      </c>
+      <c r="E10" s="22">
+        <v>3621378</v>
+      </c>
+      <c r="F10" s="22">
+        <v>4365360</v>
+      </c>
+      <c r="G10" s="22">
+        <v>363780</v>
+      </c>
+      <c r="H10" s="26">
+        <v>373961</v>
+      </c>
+      <c r="I10" s="22">
+        <v>465499</v>
+      </c>
+      <c r="J10" s="48">
+        <v>0.11936297216746899</v>
+      </c>
+      <c r="K10" s="31">
+        <v>9728000000</v>
+      </c>
+      <c r="L10" s="31">
+        <v>863000000</v>
+      </c>
+      <c r="M10" s="25">
+        <v>9.7349125775521697E-2</v>
+      </c>
+      <c r="N10" s="23">
+        <v>26741.4371323327</v>
+      </c>
+      <c r="O10" s="23">
+        <v>-536.45815675577899</v>
+      </c>
+      <c r="P10" s="25">
+        <v>-1.9666405749800199E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="21">
+        <v>12</v>
+      </c>
+      <c r="C11" s="22">
+        <v>495854</v>
+      </c>
+      <c r="D11" s="22">
+        <v>111731</v>
+      </c>
+      <c r="E11" s="22">
+        <v>3292276</v>
+      </c>
+      <c r="F11" s="22">
+        <v>3899861</v>
+      </c>
+      <c r="G11" s="22">
+        <v>324988.41666666599</v>
+      </c>
+      <c r="H11" s="26">
+        <v>333060</v>
+      </c>
+      <c r="I11" s="22">
+        <v>367152</v>
+      </c>
+      <c r="J11" s="48">
+        <v>0.10392930750877</v>
+      </c>
+      <c r="K11" s="31">
+        <v>8865000000</v>
+      </c>
+      <c r="L11" s="31">
+        <v>1251000000</v>
+      </c>
+      <c r="M11" s="25">
+        <v>0.164302600472813</v>
+      </c>
+      <c r="N11" s="23">
+        <v>27277.895289088501</v>
+      </c>
+      <c r="O11" s="23">
+        <v>1414.45734387423</v>
+      </c>
+      <c r="P11" s="25">
+        <v>5.4689455704629499E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="21">
+        <v>12</v>
+      </c>
+      <c r="C12" s="22">
+        <v>417691</v>
+      </c>
+      <c r="D12" s="22">
+        <v>92371</v>
+      </c>
+      <c r="E12" s="22">
+        <v>3022647</v>
+      </c>
+      <c r="F12" s="22">
+        <v>3532709</v>
+      </c>
+      <c r="G12" s="22">
+        <v>294392.41666666599</v>
+      </c>
+      <c r="H12" s="26">
+        <v>300026</v>
+      </c>
+      <c r="I12" s="22">
+        <v>182444</v>
+      </c>
+      <c r="J12" s="48">
+        <v>5.4456587762460498E-2</v>
+      </c>
+      <c r="K12" s="31">
+        <v>7614000000</v>
+      </c>
+      <c r="L12" s="31">
+        <v>-83000000</v>
+      </c>
+      <c r="M12" s="25">
+        <v>-1.07834221125113E-2</v>
+      </c>
+      <c r="N12" s="23">
+        <v>25863.437945214198</v>
+      </c>
+      <c r="O12" s="23">
+        <v>-1705.7244941748399</v>
+      </c>
+      <c r="P12" s="25">
+        <v>-6.1870740466812603E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="21">
+        <v>12</v>
+      </c>
+      <c r="C13" s="22">
+        <v>359128</v>
+      </c>
+      <c r="D13" s="22">
+        <v>67561</v>
+      </c>
+      <c r="E13" s="22">
+        <v>2923576</v>
+      </c>
+      <c r="F13" s="22">
+        <v>3350265</v>
+      </c>
+      <c r="G13" s="22">
+        <v>279188.75</v>
+      </c>
+      <c r="H13" s="26">
+        <v>281667</v>
+      </c>
+      <c r="I13" s="22">
+        <v>58282</v>
+      </c>
+      <c r="J13" s="48">
+        <v>1.7704222652425598E-2</v>
+      </c>
+      <c r="K13" s="31">
+        <v>7697000000</v>
+      </c>
+      <c r="L13" s="31">
+        <v>482000000</v>
+      </c>
+      <c r="M13" s="25">
+        <v>6.68052668052668E-2</v>
+      </c>
+      <c r="N13" s="23">
+        <v>27569.1624393891</v>
+      </c>
+      <c r="O13" s="23">
+        <v>1268.9051172826601</v>
+      </c>
+      <c r="P13" s="25">
+        <v>4.8246870809742701E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="21">
+        <v>12</v>
+      </c>
+      <c r="C14" s="22">
+        <v>274950</v>
+      </c>
+      <c r="D14" s="22">
+        <v>66683</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2950350</v>
+      </c>
+      <c r="F14" s="22">
+        <v>3291983</v>
+      </c>
+      <c r="G14" s="22">
+        <v>274331.91666666599</v>
+      </c>
+      <c r="H14" s="26">
+        <v>272732</v>
+      </c>
+      <c r="I14" s="22">
+        <v>84031</v>
+      </c>
+      <c r="J14" s="48">
+        <v>2.61945939340738E-2</v>
+      </c>
+      <c r="K14" s="31">
+        <v>7215000000</v>
+      </c>
+      <c r="L14" s="31">
+        <v>-550000000</v>
+      </c>
+      <c r="M14" s="25">
+        <v>-7.0830650354153202E-2</v>
+      </c>
+      <c r="N14" s="23">
+        <v>26300.257322106401</v>
+      </c>
+      <c r="O14" s="23">
+        <v>-2746.3119532442902</v>
+      </c>
+      <c r="P14" s="25">
+        <v>-9.4548582560999503E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="21">
+        <v>12</v>
+      </c>
+      <c r="C15" s="22">
+        <v>212188</v>
+      </c>
+      <c r="D15" s="22">
+        <v>69079</v>
+      </c>
+      <c r="E15" s="22">
+        <v>2926685</v>
+      </c>
+      <c r="F15" s="22">
+        <v>3207952</v>
+      </c>
+      <c r="G15" s="22">
+        <v>267329.33333333302</v>
+      </c>
+      <c r="H15" s="26">
+        <v>274097</v>
+      </c>
+      <c r="I15" s="22">
+        <v>391595</v>
+      </c>
+      <c r="J15" s="48">
+        <v>0.13904309716417301</v>
+      </c>
+      <c r="K15" s="31">
+        <v>7765000000</v>
+      </c>
+      <c r="L15" s="31">
+        <v>1480000000</v>
+      </c>
+      <c r="M15" s="25">
+        <v>0.235481304693715</v>
+      </c>
+      <c r="N15" s="23">
+        <v>29046.569275350699</v>
+      </c>
+      <c r="O15" s="23">
+        <v>2267.2937786718799</v>
+      </c>
+      <c r="P15" s="25">
+        <v>8.4665986536979806E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="21">
+        <v>12</v>
+      </c>
+      <c r="C16" s="22">
+        <v>147375</v>
+      </c>
+      <c r="D16" s="22">
+        <v>68798</v>
+      </c>
+      <c r="E16" s="22">
+        <v>2600184</v>
+      </c>
+      <c r="F16" s="22">
+        <v>2816357</v>
+      </c>
+      <c r="G16" s="22">
+        <v>234696.41666666599</v>
+      </c>
+      <c r="H16" s="26">
+        <v>242484</v>
+      </c>
+      <c r="I16" s="22">
+        <v>358795</v>
+      </c>
+      <c r="J16" s="48">
+        <v>0.14599631667481799</v>
+      </c>
+      <c r="K16" s="31">
+        <v>6285000000</v>
+      </c>
+      <c r="L16" s="31">
+        <v>473000000</v>
+      </c>
+      <c r="M16" s="25">
+        <v>8.1383344803853994E-2</v>
+      </c>
+      <c r="N16" s="23">
+        <v>26779.275496678802</v>
+      </c>
+      <c r="O16" s="23">
+        <v>-1600.0695615536299</v>
+      </c>
+      <c r="P16" s="25">
+        <v>-5.6381483021204402E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="21">
+        <v>12</v>
+      </c>
+      <c r="C17" s="22">
+        <v>102662</v>
+      </c>
+      <c r="D17" s="22">
+        <v>68264</v>
+      </c>
+      <c r="E17" s="22">
+        <v>2286636</v>
+      </c>
+      <c r="F17" s="22">
+        <v>2457562</v>
+      </c>
+      <c r="G17" s="22">
+        <v>204796.83333333299</v>
+      </c>
+      <c r="H17" s="26">
+        <v>211642</v>
+      </c>
+      <c r="I17" s="22">
+        <v>357018</v>
+      </c>
+      <c r="J17" s="48">
+        <v>0.16996454251850901</v>
+      </c>
+      <c r="K17" s="31">
+        <v>5812000000</v>
+      </c>
+      <c r="L17" s="31">
+        <v>1200000000</v>
+      </c>
+      <c r="M17" s="25">
+        <v>0.26019080659150001</v>
+      </c>
+      <c r="N17" s="23">
+        <v>28379.345058232499</v>
+      </c>
+      <c r="O17" s="23">
+        <v>2031.8845908488099</v>
+      </c>
+      <c r="P17" s="25">
+        <v>7.7118802146573004E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="21">
+        <v>12</v>
+      </c>
+      <c r="C18" s="22">
+        <v>75216</v>
+      </c>
+      <c r="D18" s="22">
+        <v>67232</v>
+      </c>
+      <c r="E18" s="22">
+        <v>1958096</v>
+      </c>
+      <c r="F18" s="22">
+        <v>2100544</v>
+      </c>
+      <c r="G18" s="22">
+        <v>175045.33333333299</v>
+      </c>
+      <c r="H18" s="26">
+        <v>182251</v>
+      </c>
+      <c r="I18" s="22">
+        <v>364480</v>
+      </c>
+      <c r="J18" s="48">
+        <v>0.20994617709946101</v>
+      </c>
+      <c r="K18" s="31">
+        <v>4612000000</v>
+      </c>
+      <c r="L18" s="31">
+        <v>819000000</v>
+      </c>
+      <c r="M18" s="25">
+        <v>0.21592407065647201</v>
+      </c>
+      <c r="N18" s="23">
+        <v>26347.4604673836</v>
+      </c>
+      <c r="O18" s="23">
+        <v>129.533017704412</v>
+      </c>
+      <c r="P18" s="25">
+        <v>4.9406276660513403E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="21">
+        <v>12</v>
+      </c>
+      <c r="C19" s="22">
+        <v>72207</v>
+      </c>
+      <c r="D19" s="22">
+        <v>65801</v>
+      </c>
+      <c r="E19" s="22">
+        <v>1598056</v>
+      </c>
+      <c r="F19" s="22">
+        <v>1736064</v>
+      </c>
+      <c r="G19" s="22">
+        <v>144672</v>
+      </c>
+      <c r="H19" s="26">
+        <v>149436</v>
+      </c>
+      <c r="I19" s="22">
+        <v>114229</v>
+      </c>
+      <c r="J19" s="48">
+        <v>7.0431948996044602E-2</v>
+      </c>
+      <c r="K19" s="31">
+        <v>3793000000</v>
+      </c>
+      <c r="L19" s="49">
+        <v>322000000</v>
+      </c>
+      <c r="M19" s="25">
+        <v>9.2768654566407302E-2</v>
+      </c>
+      <c r="N19" s="23">
+        <v>26217.927449679199</v>
+      </c>
+      <c r="O19" s="23">
+        <v>535.90677556630897</v>
+      </c>
+      <c r="P19" s="25">
+        <v>2.08670019531015E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="21">
+        <v>12</v>
+      </c>
+      <c r="C20" s="22">
+        <v>68842</v>
+      </c>
+      <c r="D20" s="22">
+        <v>67387</v>
+      </c>
+      <c r="E20" s="22">
+        <v>1485606</v>
+      </c>
+      <c r="F20" s="22">
+        <v>1621835</v>
+      </c>
+      <c r="G20" s="22">
+        <v>135152.91666666599</v>
+      </c>
+      <c r="H20" s="26">
+        <v>139204</v>
+      </c>
+      <c r="I20" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="31">
+        <v>3471000000</v>
+      </c>
+      <c r="L20" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="23">
+        <v>25682.0206741129</v>
+      </c>
+      <c r="O20" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="P20" s="48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="23">
-        <f t="shared" ref="C4:C7" si="0">C5*(1+$H$24)</f>
-        <v>687858.94516254519</v>
-      </c>
-      <c r="D4" s="23">
-        <f>D5*(1+$H$24)</f>
-        <v>155302.80578954259</v>
-      </c>
-      <c r="E4" s="23">
-        <f t="shared" ref="E4:E6" si="1">E5*(1+$H$24)</f>
-        <v>4567950.2310554693</v>
-      </c>
-      <c r="F4" s="23">
-        <f>G4*12</f>
-        <v>5411111.9820075519</v>
-      </c>
-      <c r="G4" s="23">
-        <f t="shared" ref="G4:G6" si="2">G5*(1+$H$24)</f>
-        <v>450925.99850062933</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" s="23">
-        <f>F4-F5</f>
-        <v>347372.52663832903</v>
-      </c>
-      <c r="J4" s="25">
-        <f t="shared" ref="J4:J6" si="3">I4/F5</f>
-        <v>6.8600000000000064E-2</v>
-      </c>
-      <c r="K4" s="32">
-        <f t="shared" ref="K4:K6" si="4">N4*G4</f>
-        <v>12708574518.386024</v>
-      </c>
-      <c r="L4" s="32">
-        <f t="shared" ref="L4:L6" si="5">K4-K5</f>
-        <v>883245859.37664413</v>
-      </c>
-      <c r="M4" s="26">
-        <f t="shared" ref="M4:M6" si="6">L4/K5</f>
-        <v>7.4691020000000108E-2</v>
-      </c>
-      <c r="N4" s="24">
-        <f t="shared" ref="N4:N6" si="7">(1+P4)*N5</f>
-        <v>28183.281870291823</v>
-      </c>
-      <c r="O4" s="24">
-        <f t="shared" ref="O4:O6" si="8">N4-N5</f>
-        <v>159.73422159755864</v>
-      </c>
-      <c r="P4" s="25">
-        <f>$H$26</f>
-        <v>5.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="23">
-        <f t="shared" si="0"/>
-        <v>643701.05293144786</v>
-      </c>
-      <c r="D5" s="23">
-        <f>D6*(1+$H$24)</f>
-        <v>145332.96442966739</v>
-      </c>
-      <c r="E5" s="23">
-        <f t="shared" si="1"/>
-        <v>4274705.4380081128</v>
-      </c>
-      <c r="F5" s="23">
-        <f t="shared" ref="F5:F8" si="9">G5*12</f>
-        <v>5063739.4553692229</v>
-      </c>
-      <c r="G5" s="23">
-        <f t="shared" si="2"/>
-        <v>421978.28794743528</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="23">
-        <f>F5-F6</f>
-        <v>325072.54972705245</v>
-      </c>
-      <c r="J5" s="25">
-        <f t="shared" si="3"/>
-        <v>6.8599999999999911E-2</v>
-      </c>
-      <c r="K5" s="32">
-        <f>N5*G5</f>
-        <v>11825328659.00938</v>
-      </c>
-      <c r="L5" s="32">
-        <f t="shared" si="5"/>
-        <v>821860276.99072266</v>
-      </c>
-      <c r="M5" s="26">
-        <f t="shared" si="6"/>
-        <v>7.4691019999999955E-2</v>
-      </c>
-      <c r="N5" s="24">
-        <f t="shared" si="7"/>
-        <v>28023.547648694264</v>
-      </c>
-      <c r="O5" s="24">
-        <f t="shared" si="8"/>
-        <v>158.82889688531213</v>
-      </c>
-      <c r="P5" s="25">
-        <f>$H$26</f>
-        <v>5.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="23">
-        <f t="shared" si="0"/>
-        <v>602377.9271303087</v>
-      </c>
-      <c r="D6" s="23">
-        <f>D7*(1+$H$24)</f>
-        <v>136003.14844625434</v>
-      </c>
-      <c r="E6" s="23">
-        <f t="shared" si="1"/>
-        <v>4000285.8300656122</v>
-      </c>
-      <c r="F6" s="23">
-        <f t="shared" si="9"/>
-        <v>4738666.9056421705</v>
-      </c>
-      <c r="G6" s="23">
-        <f t="shared" si="2"/>
-        <v>394888.9088035142</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="23">
-        <f t="shared" ref="I6" si="10">F6-F7</f>
-        <v>304204.14535565488</v>
-      </c>
-      <c r="J6" s="25">
-        <f t="shared" si="3"/>
-        <v>6.859999999999998E-2</v>
-      </c>
-      <c r="K6" s="32">
-        <f t="shared" si="4"/>
-        <v>11003468382.018658</v>
-      </c>
-      <c r="L6" s="32">
-        <f t="shared" si="5"/>
-        <v>764740992.24419403</v>
-      </c>
-      <c r="M6" s="26">
-        <f t="shared" si="6"/>
-        <v>7.4691020000000177E-2</v>
-      </c>
-      <c r="N6" s="24">
-        <f t="shared" si="7"/>
-        <v>27864.718751808952</v>
-      </c>
-      <c r="O6" s="24">
-        <f t="shared" si="8"/>
-        <v>157.92870327663695</v>
-      </c>
-      <c r="P6" s="25">
-        <f>$H$26</f>
-        <v>5.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23">
-        <f t="shared" si="0"/>
-        <v>563707.58668379998</v>
-      </c>
-      <c r="D7" s="23">
-        <f>D8*(1+$H$24)</f>
-        <v>127272.27067776</v>
-      </c>
-      <c r="E7" s="23">
-        <f>E8*(1+$H$24)</f>
-        <v>3743482.90292496</v>
-      </c>
-      <c r="F7" s="23">
-        <f t="shared" si="9"/>
-        <v>4434462.7602865156</v>
-      </c>
-      <c r="G7" s="23">
-        <f>G8*(1+$H$24)</f>
-        <v>369538.56335720961</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="23">
-        <f>F7-F8</f>
-        <v>284675.41208651941</v>
-      </c>
-      <c r="J7" s="25">
-        <f>I7/F8</f>
-        <v>6.8599999999999925E-2</v>
-      </c>
-      <c r="K7" s="32">
-        <f>N7*G7</f>
-        <v>10238727389.774464</v>
-      </c>
-      <c r="L7" s="32">
-        <f>K7-K8</f>
-        <v>711591497.47449493</v>
-      </c>
-      <c r="M7" s="26">
-        <f>L7/K8</f>
-        <v>7.4691020000000011E-2</v>
-      </c>
-      <c r="N7" s="24">
-        <f>(1+P7)*N8</f>
-        <v>27706.790048532315</v>
-      </c>
-      <c r="O7" s="24">
-        <f>N7-N8</f>
-        <v>157.03361169000345</v>
-      </c>
-      <c r="P7" s="25">
-        <f>$H$26</f>
-        <v>5.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23">
-        <f t="shared" ref="C8:D8" si="11">C10*(1+$H$24)</f>
-        <v>527519.73300000001</v>
-      </c>
-      <c r="D8" s="23">
-        <f t="shared" si="11"/>
-        <v>119101.88159999999</v>
-      </c>
-      <c r="E8" s="23">
-        <f>E10*(1+$H$24)</f>
-        <v>3503165.7335999999</v>
-      </c>
-      <c r="F8" s="23">
-        <f t="shared" si="9"/>
-        <v>4149787.3481999962</v>
-      </c>
-      <c r="G8" s="23">
-        <f>G10*(1+$H$24)</f>
-        <v>345815.61234999966</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="23">
-        <f>F8-F10</f>
-        <v>266400.34819999617</v>
-      </c>
-      <c r="J8" s="26">
-        <f>I8/F10</f>
-        <v>6.8599999999999009E-2</v>
-      </c>
-      <c r="K8" s="32">
-        <f>N8*G8</f>
-        <v>9527135892.2999687</v>
-      </c>
-      <c r="L8" s="32">
-        <f>K8-K10</f>
-        <v>662135892.29996872</v>
-      </c>
-      <c r="M8" s="26">
-        <f>L8/K10</f>
-        <v>7.4691019999996472E-2</v>
-      </c>
-      <c r="N8" s="24">
-        <f>(1+P8)*N10</f>
-        <v>27549.756436842312</v>
-      </c>
-      <c r="O8" s="24">
-        <f>N8-N10</f>
-        <v>156.14359320871154</v>
-      </c>
-      <c r="P8" s="25">
-        <f>$H$26</f>
-        <v>5.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="22">
-        <v>5</v>
-      </c>
-      <c r="C9" s="23">
-        <v>242846</v>
-      </c>
-      <c r="D9" s="23">
-        <v>47389</v>
-      </c>
-      <c r="E9" s="23">
-        <v>1465713</v>
-      </c>
-      <c r="F9" s="23">
-        <v>1755948</v>
-      </c>
-      <c r="G9" s="23">
-        <v>351189.6</v>
-      </c>
-      <c r="H9" s="23">
-        <v>358404</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="N9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="O9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="P9" s="27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="22">
-        <v>12</v>
-      </c>
-      <c r="C10" s="23">
-        <v>493655</v>
-      </c>
-      <c r="D10" s="23">
-        <v>111456</v>
-      </c>
-      <c r="E10" s="23">
-        <v>3278276</v>
-      </c>
-      <c r="F10" s="23">
-        <v>3883387</v>
-      </c>
-      <c r="G10" s="23">
-        <v>323615.58333333302</v>
-      </c>
-      <c r="H10" s="23">
-        <v>331687</v>
-      </c>
-      <c r="I10" s="23">
-        <v>358537</v>
-      </c>
-      <c r="J10" s="26">
-        <v>0.10171695249443199</v>
-      </c>
-      <c r="K10" s="32">
-        <v>8865000000</v>
-      </c>
-      <c r="L10" s="32">
-        <v>1251000000</v>
-      </c>
-      <c r="M10" s="26">
-        <v>0.164302600472813</v>
-      </c>
-      <c r="N10" s="24">
-        <v>27393.6128436336</v>
-      </c>
-      <c r="O10" s="24">
-        <v>1472.50981797299</v>
-      </c>
-      <c r="P10" s="26">
-        <v>5.6807374922096497E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="22">
-        <v>12</v>
-      </c>
-      <c r="C11" s="23">
-        <v>416312</v>
-      </c>
-      <c r="D11" s="23">
-        <v>91950</v>
-      </c>
-      <c r="E11" s="23">
-        <v>3016588</v>
-      </c>
-      <c r="F11" s="23">
-        <v>3524850</v>
-      </c>
-      <c r="G11" s="23">
-        <v>293737.5</v>
-      </c>
-      <c r="H11" s="23">
-        <v>299176</v>
-      </c>
-      <c r="I11" s="23">
-        <v>187501</v>
-      </c>
-      <c r="J11" s="26">
-        <v>5.6182616801539097E-2</v>
-      </c>
-      <c r="K11" s="32">
-        <v>7614000000</v>
-      </c>
-      <c r="L11" s="32">
-        <v>-83000000</v>
-      </c>
-      <c r="M11" s="26">
-        <v>-1.07834221125113E-2</v>
-      </c>
-      <c r="N11" s="24">
-        <v>25921.103025660599</v>
-      </c>
-      <c r="O11" s="24">
-        <v>-1754.7558671311799</v>
-      </c>
-      <c r="P11" s="26">
-        <v>-6.3403844987380095E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="22">
-        <v>12</v>
-      </c>
-      <c r="C12" s="23">
-        <v>356653</v>
-      </c>
-      <c r="D12" s="23">
-        <v>67089</v>
-      </c>
-      <c r="E12" s="23">
-        <v>2913607</v>
-      </c>
-      <c r="F12" s="23">
-        <v>3337349</v>
-      </c>
-      <c r="G12" s="23">
-        <v>278112.41666666599</v>
-      </c>
-      <c r="H12" s="23">
-        <v>280508</v>
-      </c>
-      <c r="I12" s="23">
-        <v>84655</v>
-      </c>
-      <c r="J12" s="26">
-        <v>2.60261186573345E-2</v>
-      </c>
-      <c r="K12" s="32">
-        <v>7697000000</v>
-      </c>
-      <c r="L12" s="32">
-        <v>482000000</v>
-      </c>
-      <c r="M12" s="26">
-        <v>6.68052668052668E-2</v>
-      </c>
-      <c r="N12" s="24">
-        <v>27675.858892791799</v>
-      </c>
-      <c r="O12" s="24">
-        <v>1057.9231140189199</v>
-      </c>
-      <c r="P12" s="26">
-        <v>3.9744746655471098E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="22">
-        <v>12</v>
-      </c>
-      <c r="C13" s="23">
-        <v>271565</v>
-      </c>
-      <c r="D13" s="23">
-        <v>65494</v>
-      </c>
-      <c r="E13" s="23">
-        <v>2915635</v>
-      </c>
-      <c r="F13" s="23">
-        <v>3252694</v>
-      </c>
-      <c r="G13" s="23">
-        <v>271057.83333333302</v>
-      </c>
-      <c r="H13" s="23">
-        <v>270784</v>
-      </c>
-      <c r="I13" s="23">
-        <v>61563</v>
-      </c>
-      <c r="J13" s="26">
-        <v>1.92919062238435E-2</v>
-      </c>
-      <c r="K13" s="32">
-        <v>7215000000</v>
-      </c>
-      <c r="L13" s="32">
-        <v>-550000000</v>
-      </c>
-      <c r="M13" s="26">
-        <v>-7.0830650354153202E-2</v>
-      </c>
-      <c r="N13" s="24">
-        <v>26617.935778772899</v>
-      </c>
-      <c r="O13" s="24">
-        <v>-2581.7429558199201</v>
-      </c>
-      <c r="P13" s="26">
-        <v>-8.8416827434520201E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="22">
-        <v>12</v>
-      </c>
-      <c r="C14" s="23">
-        <v>211114</v>
-      </c>
-      <c r="D14" s="23">
-        <v>68522</v>
-      </c>
-      <c r="E14" s="23">
-        <v>2911495</v>
-      </c>
-      <c r="F14" s="23">
-        <v>3191131</v>
-      </c>
-      <c r="G14" s="23">
-        <v>265927.58333333302</v>
-      </c>
-      <c r="H14" s="23">
-        <v>272758</v>
-      </c>
-      <c r="I14" s="23">
-        <v>391265</v>
-      </c>
-      <c r="J14" s="26">
-        <v>0.13974418775755601</v>
-      </c>
-      <c r="K14" s="32">
-        <v>7765000000</v>
-      </c>
-      <c r="L14" s="32">
-        <v>1480000000</v>
-      </c>
-      <c r="M14" s="26">
-        <v>0.235481304693715</v>
-      </c>
-      <c r="N14" s="24">
-        <v>29199.678734592799</v>
-      </c>
-      <c r="O14" s="24">
-        <v>2262.6753208580399</v>
-      </c>
-      <c r="P14" s="26">
-        <v>8.3998776185488302E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="22">
-        <v>12</v>
-      </c>
-      <c r="C15" s="23">
-        <v>146837</v>
-      </c>
-      <c r="D15" s="23">
-        <v>68314</v>
-      </c>
-      <c r="E15" s="23">
-        <v>2584715</v>
-      </c>
-      <c r="F15" s="23">
-        <v>2799866</v>
-      </c>
-      <c r="G15" s="23">
-        <v>233322.16666666599</v>
-      </c>
-      <c r="H15" s="23">
-        <v>240219</v>
-      </c>
-      <c r="I15" s="23">
-        <v>359451</v>
-      </c>
-      <c r="J15" s="26">
-        <v>0.14729093207507701</v>
-      </c>
-      <c r="K15" s="32">
-        <v>6285000000</v>
-      </c>
-      <c r="L15" s="32">
-        <v>473000000</v>
-      </c>
-      <c r="M15" s="26">
-        <v>8.1383344803853994E-2</v>
-      </c>
-      <c r="N15" s="24">
-        <v>26937.003413734801</v>
-      </c>
-      <c r="O15" s="24">
-        <v>-1641.7424143313201</v>
-      </c>
-      <c r="P15" s="26">
-        <v>-5.7446272282495797E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="22">
-        <v>12</v>
-      </c>
-      <c r="C16" s="23">
-        <v>102280</v>
-      </c>
-      <c r="D16" s="23">
-        <v>67591</v>
-      </c>
-      <c r="E16" s="23">
-        <v>2270544</v>
-      </c>
-      <c r="F16" s="23">
-        <v>2440415</v>
-      </c>
-      <c r="G16" s="23">
-        <v>203367.91666666599</v>
-      </c>
-      <c r="H16" s="23">
-        <v>210264</v>
-      </c>
-      <c r="I16" s="23">
-        <v>352109</v>
-      </c>
-      <c r="J16" s="26">
-        <v>0.168609868477129</v>
-      </c>
-      <c r="K16" s="32">
-        <v>5812000000</v>
-      </c>
-      <c r="L16" s="32">
-        <v>1200000000</v>
-      </c>
-      <c r="M16" s="26">
-        <v>0.26019080659150001</v>
-      </c>
-      <c r="N16" s="24">
-        <v>28578.745828066101</v>
-      </c>
-      <c r="O16" s="24">
-        <v>2076.8825953789601</v>
-      </c>
-      <c r="P16" s="26">
-        <v>7.8367418062038702E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="22">
-        <v>12</v>
-      </c>
-      <c r="C17" s="23">
-        <v>74966</v>
-      </c>
-      <c r="D17" s="23">
-        <v>66883</v>
-      </c>
-      <c r="E17" s="23">
-        <v>1946457</v>
-      </c>
-      <c r="F17" s="23">
-        <v>2088306</v>
-      </c>
-      <c r="G17" s="23">
-        <v>174025.5</v>
-      </c>
-      <c r="H17" s="23">
-        <v>181219</v>
-      </c>
-      <c r="I17" s="23">
-        <v>353466</v>
-      </c>
-      <c r="J17" s="26">
-        <v>0.20374559037144599</v>
-      </c>
-      <c r="K17" s="32">
-        <v>4612000000</v>
-      </c>
-      <c r="L17" s="32">
-        <v>819000000</v>
-      </c>
-      <c r="M17" s="26">
-        <v>0.21592407065647201</v>
-      </c>
-      <c r="N17" s="24">
-        <v>26501.863232687101</v>
-      </c>
-      <c r="O17" s="24">
-        <v>265.437971567982</v>
-      </c>
-      <c r="P17" s="26">
-        <v>1.01171546400166E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="22">
-        <v>12</v>
-      </c>
-      <c r="C18" s="23">
-        <v>71979</v>
-      </c>
-      <c r="D18" s="23">
-        <v>65736</v>
-      </c>
-      <c r="E18" s="23">
-        <v>1597125</v>
-      </c>
-      <c r="F18" s="23">
-        <v>1734840</v>
-      </c>
-      <c r="G18" s="23">
-        <v>144570</v>
-      </c>
-      <c r="H18" s="23">
-        <v>148887</v>
-      </c>
-      <c r="I18" s="23">
-        <v>121067</v>
-      </c>
-      <c r="J18" s="26">
-        <v>7.5021084130171903E-2</v>
-      </c>
-      <c r="K18" s="32">
-        <v>3793000000</v>
-      </c>
-      <c r="L18" s="32">
-        <v>322000000</v>
-      </c>
-      <c r="M18" s="26">
-        <v>9.2768654566407302E-2</v>
-      </c>
-      <c r="N18" s="24">
-        <v>26236.4252611191</v>
-      </c>
-      <c r="O18" s="24">
-        <v>426.10373510530098</v>
-      </c>
-      <c r="P18" s="26">
-        <v>1.6509044053396899E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
+        <v>(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = 2.</v>
+      </c>
+      <c r="H24" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="23">
-        <v>68552</v>
-      </c>
-      <c r="D19" s="23">
-        <v>67476</v>
-      </c>
-      <c r="E19" s="23">
-        <v>1477745</v>
-      </c>
-      <c r="F19" s="23">
-        <v>1613773</v>
-      </c>
-      <c r="G19" s="23">
-        <v>134481.08333333299</v>
-      </c>
-      <c r="H19" s="23">
-        <v>138251</v>
-      </c>
-      <c r="I19" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="K19" s="32">
-        <v>3471000000</v>
-      </c>
-      <c r="L19" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="M19" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="24">
-        <v>25810.321526013799</v>
-      </c>
-      <c r="O19" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="P19" s="69" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="28" t="s">
+    </row>
+    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>_xlfn.CONCAT("(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H27*100,2),"%")</f>
+        <v>(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = 0.19%</v>
+      </c>
+      <c r="H25" s="11">
+        <v>7.6799999999999993E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="11">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" t="str">
-        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
-        <v>(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = 5.</v>
-      </c>
-      <c r="H23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
-        <f>_xlfn.CONCAT("(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H26*100,2),"%")</f>
-        <v>(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = 0.57%</v>
-      </c>
-      <c r="H24" s="12">
-        <v>6.8599999999999994E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="H26" s="12">
-        <v>5.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:P19">
-    <sortCondition descending="1" ref="A9:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:P20">
+    <sortCondition descending="1" ref="A9:A20"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
@@ -4788,7 +4857,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4809,267 +4878,267 @@
   <sheetData>
     <row r="1" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P2" s="62" t="s">
+      <c r="P2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="64"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="66"/>
     </row>
     <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P3" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="67"/>
+      <c r="P3" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="69"/>
     </row>
     <row r="4" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P4" s="14"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="15"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="59" t="s">
+      <c r="P5" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="61"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="63"/>
     </row>
     <row r="6" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="17">
-        <f>AVERAGE(projection_data!E11)</f>
-        <v>0.10171695249443199</v>
-      </c>
-      <c r="R6" s="17"/>
-      <c r="S6" s="15"/>
+      <c r="Q6" s="16">
+        <f>AVERAGE(projection_data!E12)</f>
+        <v>0.11936297216746899</v>
+      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="17">
-        <f>AVERAGE(projection_data!E9:E11)</f>
-        <v>6.1308562651101899E-2</v>
-      </c>
-      <c r="R7" s="17"/>
-      <c r="S7" s="15"/>
+      <c r="Q7" s="16">
+        <f>AVERAGE(projection_data!E10:E12)</f>
+        <v>9.2582955812899867E-2</v>
+      </c>
+      <c r="R7" s="16"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="17">
-        <f>AVERAGE(projection_data!E7:E11)</f>
-        <v>6.8592356386941028E-2</v>
-      </c>
-      <c r="R8" s="17"/>
-      <c r="S8" s="15"/>
+      <c r="Q8" s="16">
+        <f>AVERAGE(projection_data!E7:E12)</f>
+        <v>7.6781796864895321E-2</v>
+      </c>
+      <c r="R8" s="16"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P9" s="14"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="15"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="14"/>
     </row>
     <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P10" s="59" t="s">
+      <c r="P10" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="63"/>
+    </row>
+    <row r="11" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="41">
+        <f>AVERAGE(projection_data!G12)</f>
+        <v>-1.9666405749800199E-2</v>
+      </c>
+      <c r="R11" s="41"/>
+      <c r="S11" s="14"/>
+    </row>
+    <row r="12" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="41">
+        <f>AVERAGE(projection_data!G10:G12)</f>
+        <v>-8.9492301706611006E-3</v>
+      </c>
+      <c r="R12" s="41"/>
+      <c r="S12" s="14"/>
+    </row>
+    <row r="13" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="41">
+        <f>AVERAGE(projection_data!G7:G12)</f>
+        <v>1.9194307122899501E-3</v>
+      </c>
+      <c r="R13" s="41"/>
+      <c r="S13" s="14"/>
+    </row>
+    <row r="14" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P14" s="13"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="14"/>
+    </row>
+    <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="59"/>
+      <c r="S15" s="60"/>
+    </row>
+    <row r="16" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="P16" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="14"/>
+    </row>
+    <row r="17" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P17" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="57"/>
+    </row>
+    <row r="18" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P18" s="55"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="57"/>
+    </row>
+    <row r="19" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="61"/>
-    </row>
-    <row r="11" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="42">
-        <f>AVERAGE(projection_data!G11)</f>
-        <v>5.6807374922096497E-2</v>
-      </c>
-      <c r="R11" s="42"/>
-      <c r="S11" s="15"/>
-    </row>
-    <row r="12" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q12" s="42">
-        <f>AVERAGE(projection_data!G9:G11)</f>
-        <v>1.1049425530062501E-2</v>
-      </c>
-      <c r="R12" s="42"/>
-      <c r="S12" s="15"/>
-    </row>
-    <row r="13" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q13" s="42">
-        <f>AVERAGE(projection_data!G7:G11)</f>
-        <v>5.7460450682311204E-3</v>
-      </c>
-      <c r="R13" s="42"/>
-      <c r="S13" s="15"/>
-    </row>
-    <row r="14" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P14" s="14"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="15"/>
-    </row>
-    <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="58"/>
-    </row>
-    <row r="16" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P16" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
-      <c r="S16" s="15"/>
-    </row>
-    <row r="17" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P17" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="55"/>
-    </row>
-    <row r="18" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P18" s="53"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="55"/>
-    </row>
-    <row r="19" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P19" s="16" t="s">
+      <c r="S19" s="14"/>
+    </row>
+    <row r="20" spans="16:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="P20" s="12">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="44">
+        <v>1.9E-3</v>
+      </c>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P21" s="4"/>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P22" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="16:19" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="S19" s="15"/>
-    </row>
-    <row r="20" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P20" s="13">
-        <v>6.8599999999999994E-2</v>
-      </c>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="45">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="S20" s="6"/>
-    </row>
-    <row r="21" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P21" s="5"/>
-      <c r="S21" s="6"/>
-    </row>
-    <row r="22" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P22" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="S22" s="6"/>
-    </row>
-    <row r="23" spans="16:19" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="R23" s="43" t="s">
+      <c r="R23" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="S23" s="39" t="s">
+      <c r="S23" s="38" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P24" s="8" t="str" cm="1">
-        <f t="array" ref="P24:P28">projection_data!B12:B16</f>
-        <v>FY25</v>
-      </c>
-      <c r="Q24" s="44" cm="1">
-        <f t="array" ref="Q24:Q28">projection_data!D12:D16</f>
-        <v>345815.61234999966</v>
-      </c>
-      <c r="R24" s="33" cm="1">
-        <f t="array" ref="R24:R28">projection_data!F12:F16</f>
-        <v>27549.756436842312</v>
-      </c>
-      <c r="S24" s="35" cm="1">
-        <f t="array" ref="S24:S28">projection_data!C12:C16</f>
-        <v>9527135892.2999687</v>
+      <c r="P24" s="7" t="str" cm="1">
+        <f t="array" ref="P24:P28">projection_data!B13:B17</f>
+        <v>FY26</v>
+      </c>
+      <c r="Q24" s="43" cm="1">
+        <f t="array" ref="Q24:Q28">projection_data!D13:D17</f>
+        <v>391718.304</v>
+      </c>
+      <c r="R24" s="32" cm="1">
+        <f t="array" ref="R24:R28">projection_data!F13:F17</f>
+        <v>26792.24586288413</v>
+      </c>
+      <c r="S24" s="34" cm="1">
+        <f t="array" ref="S24:S28">projection_data!C13:C17</f>
+        <v>10495013109.759989</v>
       </c>
     </row>
     <row r="25" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P25" s="8" t="str">
-        <v>FY26</v>
-      </c>
-      <c r="Q25" s="44">
-        <v>369538.56335720961</v>
-      </c>
-      <c r="R25" s="33">
-        <v>27706.790048532315</v>
-      </c>
-      <c r="S25" s="35">
-        <v>10238727389.774464</v>
+      <c r="P25" s="7" t="str">
+        <v>FY27</v>
+      </c>
+      <c r="Q25" s="43">
+        <v>421802.26974720001</v>
+      </c>
+      <c r="R25" s="32">
+        <v>26843.151130023609</v>
+      </c>
+      <c r="S25" s="34">
+        <v>11322502073.811075</v>
       </c>
     </row>
     <row r="26" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P26" s="8" t="str">
-        <v>FY27</v>
-      </c>
-      <c r="Q26" s="44">
-        <v>394888.9088035142</v>
-      </c>
-      <c r="R26" s="33">
-        <v>27864.718751808952</v>
-      </c>
-      <c r="S26" s="35">
-        <v>11003468382.018658</v>
+      <c r="P26" s="7" t="str">
+        <v>FY28</v>
+      </c>
+      <c r="Q26" s="43">
+        <v>454196.68406378495</v>
+      </c>
+      <c r="R26" s="32">
+        <v>26894.153117170656</v>
+      </c>
+      <c r="S26" s="34">
+        <v>12215235166.522617</v>
       </c>
     </row>
     <row r="27" spans="16:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="P27" s="8" t="str">
-        <v>FY28</v>
-      </c>
-      <c r="Q27" s="44">
-        <v>421978.28794743528</v>
-      </c>
-      <c r="R27" s="33">
-        <v>28023.547648694264</v>
-      </c>
-      <c r="S27" s="35">
-        <v>11825328659.00938</v>
+      <c r="P27" s="7" t="str">
+        <v>FY29</v>
+      </c>
+      <c r="Q27" s="43">
+        <v>489078.98939988361</v>
+      </c>
+      <c r="R27" s="32">
+        <v>26945.252008093281</v>
+      </c>
+      <c r="S27" s="34">
+        <v>13178356621.243446</v>
       </c>
     </row>
     <row r="28" spans="16:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P28" s="9" t="str">
-        <v>FY29</v>
-      </c>
-      <c r="Q28" s="10">
-        <v>450925.99850062933</v>
-      </c>
-      <c r="R28" s="34">
-        <v>28183.281870291823</v>
-      </c>
-      <c r="S28" s="36">
-        <v>12708574518.386024</v>
+      <c r="P28" s="8" t="str">
+        <v>FY30</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>526640.2557857947</v>
+      </c>
+      <c r="R28" s="33">
+        <v>26996.447986908657</v>
+      </c>
+      <c r="S28" s="35">
+        <v>14217416273.133478</v>
       </c>
     </row>
     <row r="29" spans="16:19" x14ac:dyDescent="0.2"/>
@@ -5110,10 +5179,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EC6393-3785-8B4D-BC33-531ADF13ED6E}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5127,26 +5196,26 @@
     <col min="7" max="7" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:7" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="46" t="s">
+      <c r="E1" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5155,22 +5224,22 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2">
         <v>3471000000</v>
       </c>
       <c r="D2" s="1">
-        <v>134481.08333333299</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="3">
-        <v>25810.321526013799</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>135152.91666666599</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="70">
+        <v>25682.0206741129</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -5178,22 +5247,22 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="3">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2">
         <v>3793000000</v>
       </c>
       <c r="D3" s="1">
-        <v>144570</v>
-      </c>
-      <c r="E3" s="18">
-        <v>7.5021084130171806E-2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>26236.4252611191</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1.6509044053396899E-2</v>
+        <v>144672</v>
+      </c>
+      <c r="E3" s="17">
+        <v>7.0431948996044602E-2</v>
+      </c>
+      <c r="F3" s="70">
+        <v>26217.927449679199</v>
+      </c>
+      <c r="G3" s="17">
+        <v>2.08670019531015E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -5201,22 +5270,22 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="3">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2">
         <v>4612000000</v>
       </c>
       <c r="D4" s="1">
-        <v>174025.5</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0.20374559037144599</v>
-      </c>
-      <c r="F4" s="3">
-        <v>26501.863232687101</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1.01171546400166E-2</v>
+        <v>175045.33333333299</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.20994617709946101</v>
+      </c>
+      <c r="F4" s="70">
+        <v>26347.4604673836</v>
+      </c>
+      <c r="G4" s="17">
+        <v>4.9406276660513403E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -5224,22 +5293,22 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2">
         <v>5812000000</v>
       </c>
       <c r="D5" s="1">
-        <v>203367.91666666599</v>
-      </c>
-      <c r="E5" s="18">
-        <v>0.168609868477129</v>
-      </c>
-      <c r="F5" s="3">
-        <v>28578.745828066101</v>
-      </c>
-      <c r="G5" s="2">
-        <v>7.8367418062038702E-2</v>
+        <v>204796.83333333299</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.16996454251850901</v>
+      </c>
+      <c r="F5" s="70">
+        <v>28379.345058232499</v>
+      </c>
+      <c r="G5" s="17">
+        <v>7.7118802146573004E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -5247,22 +5316,22 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2">
         <v>6285000000</v>
       </c>
       <c r="D6" s="1">
-        <v>233322.16666666599</v>
-      </c>
-      <c r="E6" s="18">
-        <v>0.14729093207507701</v>
-      </c>
-      <c r="F6" s="3">
-        <v>26937.003413734801</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-5.7446272282495797E-2</v>
+        <v>234696.41666666599</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.14599631667481799</v>
+      </c>
+      <c r="F6" s="70">
+        <v>26779.275496678802</v>
+      </c>
+      <c r="G6" s="17">
+        <v>-5.6381483021204402E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5270,22 +5339,22 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="3">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2">
         <v>7765000000</v>
       </c>
       <c r="D7" s="1">
-        <v>265927.58333333302</v>
-      </c>
-      <c r="E7" s="18">
-        <v>0.13974418775755601</v>
-      </c>
-      <c r="F7" s="3">
-        <v>29199.678734592799</v>
-      </c>
-      <c r="G7" s="2">
-        <v>8.3998776185488302E-2</v>
+        <v>267329.33333333302</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.13904309716417301</v>
+      </c>
+      <c r="F7" s="70">
+        <v>29046.569275350699</v>
+      </c>
+      <c r="G7" s="17">
+        <v>8.4665986536979806E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5293,22 +5362,22 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2">
         <v>7215000000</v>
       </c>
       <c r="D8" s="1">
-        <v>271057.83333333302</v>
-      </c>
-      <c r="E8" s="18">
-        <v>1.92919062238435E-2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>26617.935778772899</v>
-      </c>
-      <c r="G8" s="2">
-        <v>-8.8416827434520201E-2</v>
+        <v>274331.91666666599</v>
+      </c>
+      <c r="E8" s="17">
+        <v>2.61945939340739E-2</v>
+      </c>
+      <c r="F8" s="70">
+        <v>26300.257322106401</v>
+      </c>
+      <c r="G8" s="17">
+        <v>-9.4548582560999503E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -5316,22 +5385,22 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2">
         <v>7697000000</v>
       </c>
       <c r="D9" s="1">
-        <v>278112.41666666599</v>
-      </c>
-      <c r="E9" s="18">
-        <v>2.6026118657334601E-2</v>
-      </c>
-      <c r="F9" s="3">
-        <v>27675.858892791799</v>
-      </c>
-      <c r="G9" s="2">
-        <v>3.9744746655471098E-2</v>
+        <v>279188.75</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1.7704222652425501E-2</v>
+      </c>
+      <c r="F9" s="70">
+        <v>27569.1624393891</v>
+      </c>
+      <c r="G9" s="17">
+        <v>4.8246870809742701E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -5339,22 +5408,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2">
         <v>7614000000</v>
       </c>
       <c r="D10" s="1">
-        <v>293737.5</v>
-      </c>
-      <c r="E10" s="18">
-        <v>5.6182616801539097E-2</v>
-      </c>
-      <c r="F10" s="3">
-        <v>25921.103025660599</v>
-      </c>
-      <c r="G10" s="2">
-        <v>-6.3403844987380095E-2</v>
+        <v>294392.41666666599</v>
+      </c>
+      <c r="E10" s="17">
+        <v>5.4456587762460602E-2</v>
+      </c>
+      <c r="F10" s="70">
+        <v>25863.437945214198</v>
+      </c>
+      <c r="G10" s="17">
+        <v>-6.1870740466812603E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -5362,138 +5431,161 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="3">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
         <v>8865000000</v>
       </c>
       <c r="D11" s="1">
-        <v>323615.58333333302</v>
-      </c>
-      <c r="E11" s="18">
-        <v>0.10171695249443199</v>
-      </c>
-      <c r="F11" s="3">
-        <v>27393.6128436336</v>
-      </c>
-      <c r="G11" s="2">
-        <v>5.6807374922096497E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+        <v>324988.41666666599</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.10392930750877</v>
+      </c>
+      <c r="F11" s="70">
+        <v>27277.895289088501</v>
+      </c>
+      <c r="G11" s="17">
+        <v>5.4689455704629499E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2">
+        <v>9728000000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>363780</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.11936297216746899</v>
+      </c>
+      <c r="F12" s="70">
+        <v>26741.4371323327</v>
+      </c>
+      <c r="G12" s="17">
+        <v>-1.9666405749800199E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="29" t="str" cm="1">
-        <f t="array" ref="B12">CONCATENATE("FY",RIGHT(INDEX(Table1[],ROWS(Table1[]),2),2)+1)</f>
-        <v>FY25</v>
-      </c>
-      <c r="C12" s="30">
-        <f>D12*F12</f>
-        <v>9527135892.2999687</v>
-      </c>
-      <c r="D12" s="31" cm="1">
-        <f t="array" ref="D12">(1+Graph!$P$20)*INDEX(Table1[],ROWS(Table1[]),4)</f>
-        <v>345815.61234999966</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30" cm="1">
-        <f t="array" ref="F12">(1+Graph!$R$20)*INDEX(Table1[],ROWS(Table1[]),6)</f>
-        <v>27549.756436842312</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="B13" s="28" t="str" cm="1">
+        <f t="array" ref="B13">CONCATENATE("FY",RIGHT(INDEX(Table1[],ROWS(Table1[]),2),2)+1)</f>
+        <v>FY26</v>
+      </c>
+      <c r="C13" s="29">
+        <f>D13*F13</f>
+        <v>10495013109.759989</v>
+      </c>
+      <c r="D13" s="30" cm="1">
+        <f t="array" ref="D13">(1+Graph!$P$20)*INDEX(Table1[],ROWS(Table1[]),4)</f>
+        <v>391718.304</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29" cm="1">
+        <f t="array" ref="F13">(1+Graph!$R$20)*INDEX(Table1[],ROWS(Table1[]),6)</f>
+        <v>26792.24586288413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="29" t="str">
-        <f>CONCATENATE("FY",RIGHT(B12,2)+1)</f>
-        <v>FY26</v>
-      </c>
-      <c r="C13" s="30">
-        <f>D13*F13</f>
-        <v>10238727389.774464</v>
-      </c>
-      <c r="D13" s="31">
-        <f>(1+Graph!$P$20)*D12</f>
-        <v>369538.56335720961</v>
-      </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30">
-        <f>(1+Graph!$R$20)*F12</f>
-        <v>27706.790048532315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+      <c r="B14" s="28" t="str">
+        <f>CONCATENATE("FY",RIGHT(B13,2)+1)</f>
+        <v>FY27</v>
+      </c>
+      <c r="C14" s="29">
+        <f>D14*F14</f>
+        <v>11322502073.811075</v>
+      </c>
+      <c r="D14" s="30">
+        <f>(1+Graph!$P$20)*D13</f>
+        <v>421802.26974720001</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29">
+        <f>(1+Graph!$R$20)*F13</f>
+        <v>26843.151130023609</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="29" t="str">
-        <f t="shared" ref="B14:B16" si="0">CONCATENATE("FY",RIGHT(B13,2)+1)</f>
-        <v>FY27</v>
-      </c>
-      <c r="C14" s="30">
-        <f>D14*F14</f>
-        <v>11003468382.018658</v>
-      </c>
-      <c r="D14" s="31">
-        <f>(1+Graph!$P$20)*D13</f>
-        <v>394888.9088035142</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30">
-        <f>(1+Graph!$R$20)*F13</f>
-        <v>27864.718751808952</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="B15" s="28" t="str">
+        <f t="shared" ref="B15:B17" si="0">CONCATENATE("FY",RIGHT(B14,2)+1)</f>
+        <v>FY28</v>
+      </c>
+      <c r="C15" s="29">
+        <f>D15*F15</f>
+        <v>12215235166.522617</v>
+      </c>
+      <c r="D15" s="30">
+        <f>(1+Graph!$P$20)*D14</f>
+        <v>454196.68406378495</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29">
+        <f>(1+Graph!$R$20)*F14</f>
+        <v>26894.153117170656</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>FY28</v>
-      </c>
-      <c r="C15" s="30">
-        <f>D15*F15</f>
-        <v>11825328659.00938</v>
-      </c>
-      <c r="D15" s="31">
-        <f>(1+Graph!$P$20)*D14</f>
-        <v>421978.28794743528</v>
-      </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30">
-        <f>(1+Graph!$R$20)*F14</f>
-        <v>28023.547648694264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="29" t="str">
+      <c r="B16" s="28" t="str">
         <f t="shared" si="0"/>
         <v>FY29</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="29">
         <f>D16*F16</f>
-        <v>12708574518.386024</v>
-      </c>
-      <c r="D16" s="31">
+        <v>13178356621.243446</v>
+      </c>
+      <c r="D16" s="30">
         <f>(1+Graph!$P$20)*D15</f>
-        <v>450925.99850062933</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30">
+        <v>489078.98939988361</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29">
         <f>(1+Graph!$R$20)*F15</f>
-        <v>28183.281870291823</v>
+        <v>26945.252008093281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>FY30</v>
+      </c>
+      <c r="C17" s="29">
+        <f>D17*F17</f>
+        <v>14217416273.133478</v>
+      </c>
+      <c r="D17" s="30">
+        <f>(1+Graph!$P$20)*D16</f>
+        <v>526640.2557857947</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29">
+        <f>(1+Graph!$R$20)*F16</f>
+        <v>26996.447986908657</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G12">
-    <sortCondition ref="B2:B12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G13">
+    <sortCondition ref="B2:B13"/>
   </sortState>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 7/17/2025 at 8:19pm
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEA1472-4A52-E84A-B412-1C8F26433FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E20AAC-D522-6543-ACE7-DA9C85BACCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -128,12 +128,6 @@
     <t>Average Annual Per Capita Spending % Growth</t>
   </si>
   <si>
-    <t>FY26 (Forecast)</t>
-  </si>
-  <si>
-    <t>FY25 (Estimate)(1)(2)</t>
-  </si>
-  <si>
     <t>FY24</t>
   </si>
   <si>
@@ -183,12 +177,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>(1) Data sources: Full-year Enrollment 2025 Estimate Represents YTD annualized</t>
-  </si>
-  <si>
-    <t>FY26 Growth Assumptions</t>
   </si>
   <si>
     <t>Definitions</t>
@@ -523,6 +511,18 @@
   </si>
   <si>
     <t>FY25</t>
+  </si>
+  <si>
+    <t>FY30 (Forecast)</t>
+  </si>
+  <si>
+    <t>FY26 (Estimate)(1)(2)</t>
+  </si>
+  <si>
+    <t>FY27 Growth Assumptions</t>
+  </si>
+  <si>
+    <t>(1) Data sources: Full-year Enrollment 2026 Estimate Represents YTD annualized</t>
   </si>
 </sst>
 </file>
@@ -1215,6 +1215,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF7F7F7F"/>
+      <color rgb="FFB9CDE5"/>
       <color rgb="FFC7D8EA"/>
       <color rgb="FFF2DCDB"/>
       <color rgb="FFE4DFEC"/>
@@ -1356,7 +1358,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="C7D8EA"/>
+                <a:srgbClr val="B9CDE5">
+                  <a:alpha val="80000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1465,10 +1469,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
+                <a:srgbClr val="7F7F7F">
                   <a:alpha val="80000"/>
-                </a:schemeClr>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -3728,7 +3731,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="23" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -3748,7 +3751,7 @@
     </row>
     <row r="2" spans="1:16" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="57" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
@@ -3778,22 +3781,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>2</v>
@@ -3802,10 +3805,10 @@
         <v>21</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M3" s="19" t="s">
         <v>4</v>
@@ -3846,7 +3849,7 @@
         <v>526640.2557857947</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I4" s="22">
         <f>F4-F5</f>
@@ -3883,7 +3886,7 @@
     </row>
     <row r="5" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="22">
@@ -3907,7 +3910,7 @@
         <v>489078.98939988361</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I5" s="22">
         <f>F5-F6</f>
@@ -3944,7 +3947,7 @@
     </row>
     <row r="6" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="22">
@@ -3968,7 +3971,7 @@
         <v>454196.68406378495</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I6" s="22">
         <f t="shared" ref="I6" si="8">F6-F7</f>
@@ -4005,7 +4008,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="22">
@@ -4029,7 +4032,7 @@
         <v>421802.26974720001</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I7" s="22">
         <f>F7-F8</f>
@@ -4066,7 +4069,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22">
@@ -4090,7 +4093,7 @@
         <v>391718.304</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I8" s="22">
         <f>F8-F10</f>
@@ -4127,7 +4130,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="21">
         <v>3</v>
@@ -4151,33 +4154,33 @@
         <v>377313</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B10" s="21">
         <v>12</v>
@@ -4227,7 +4230,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="21">
         <v>12</v>
@@ -4277,7 +4280,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="21">
         <v>12</v>
@@ -4327,7 +4330,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="21">
         <v>12</v>
@@ -4377,7 +4380,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="21">
         <v>12</v>
@@ -4427,7 +4430,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="21">
         <v>12</v>
@@ -4477,7 +4480,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="21">
         <v>12</v>
@@ -4527,7 +4530,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="21">
         <v>12</v>
@@ -4577,7 +4580,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="21">
         <v>12</v>
@@ -4627,7 +4630,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="21">
         <v>12</v>
@@ -4677,7 +4680,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="21">
         <v>12</v>
@@ -4701,59 +4704,59 @@
         <v>139204</v>
       </c>
       <c r="I20" s="47" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J20" s="48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K20" s="31">
         <v>3471000000</v>
       </c>
       <c r="L20" s="49" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M20" s="48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N20" s="23">
         <v>25682.0206741129</v>
       </c>
       <c r="O20" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P20" s="48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
-        <v>(2) Full-year Enrollment 2025 Estimate Represents YTD annualized. Months in YTD = 3.</v>
+        <f>_xlfn.CONCAT("(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
+        <v>(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = 3.</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>_xlfn.CONCAT("(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H27*100,2),"%")</f>
-        <v>(3) FY25 full-year spending estimate is based an assumption of per capita spending growth = 0.19%</v>
+        <f>_xlfn.CONCAT("(3) FY26 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H27*100,2),"%")</f>
+        <v>(3) FY26 full-year spending estimate is based an assumption of per capita spending growth = 0.19%</v>
       </c>
       <c r="H25" s="11">
         <v>7.6799999999999993E-2</v>
@@ -4761,7 +4764,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
@@ -4771,67 +4774,67 @@
     </row>
     <row r="29" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -4857,7 +4860,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4887,7 +4890,7 @@
     </row>
     <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="P3" s="70" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="71"/>
       <c r="R3" s="71"/>
@@ -4948,7 +4951,7 @@
     </row>
     <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P10" s="64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q10" s="65"/>
       <c r="R10" s="65"/>
@@ -5011,7 +5014,7 @@
     </row>
     <row r="17" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P17" s="58" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q17" s="59"/>
       <c r="R17" s="59"/>
@@ -5029,7 +5032,7 @@
       </c>
       <c r="Q19" s="40"/>
       <c r="R19" s="39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S19" s="14"/>
     </row>
@@ -5049,7 +5052,7 @@
     </row>
     <row r="22" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P22" s="36" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="S22" s="5"/>
     </row>
@@ -5210,7 +5213,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>5</v>
@@ -5224,7 +5227,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2">
         <v>3471000000</v>
@@ -5233,13 +5236,13 @@
         <v>135152.91666666599</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F2" s="50">
         <v>25682.0206741129</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -5247,7 +5250,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2">
         <v>3793000000</v>
@@ -5270,7 +5273,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2">
         <v>4612000000</v>
@@ -5293,7 +5296,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2">
         <v>5812000000</v>
@@ -5316,7 +5319,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2">
         <v>6285000000</v>
@@ -5339,7 +5342,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>7765000000</v>
@@ -5362,7 +5365,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2">
         <v>7215000000</v>
@@ -5385,7 +5388,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2">
         <v>7697000000</v>
@@ -5408,7 +5411,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
         <v>7614000000</v>
@@ -5431,7 +5434,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2">
         <v>8865000000</v>
@@ -5454,7 +5457,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2">
         <v>9728000000</v>

</xml_diff>

<commit_message>
Update on 7/21/2025 at 2:29pm
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E20AAC-D522-6543-ACE7-DA9C85BACCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFCDEDA-A1CE-354A-ADA4-DFDE2C11F27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -519,10 +519,10 @@
     <t>FY26 (Estimate)(1)(2)</t>
   </si>
   <si>
-    <t>FY27 Growth Assumptions</t>
-  </si>
-  <si>
     <t>(1) Data sources: Full-year Enrollment 2026 Estimate Represents YTD annualized</t>
+  </si>
+  <si>
+    <t>FY27-FY30 Growth Assumptions</t>
   </si>
 </sst>
 </file>
@@ -3718,7 +3718,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3842,34 +3842,34 @@
       </c>
       <c r="F4" s="22">
         <f>G4*12</f>
-        <v>6319683.0694295364</v>
+        <v>5981829.4223834984</v>
       </c>
       <c r="G4" s="22">
         <f>G5*(1+$H$25)</f>
-        <v>526640.2557857947</v>
+        <v>498485.78519862483</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>63</v>
       </c>
       <c r="I4" s="22">
         <f>F4-F5</f>
-        <v>450735.19663093332</v>
+        <v>426638.65122497454</v>
       </c>
       <c r="J4" s="24">
         <f t="shared" ref="J4:J6" si="1">I4/F5</f>
-        <v>7.6800000000000104E-2</v>
+        <v>7.6799999999999979E-2</v>
       </c>
       <c r="K4" s="31">
         <f t="shared" ref="K4:K6" si="2">N4*G4</f>
-        <v>14217416273.133478</v>
+        <v>13457345572.327997</v>
       </c>
       <c r="L4" s="31">
         <f t="shared" ref="L4:L6" si="3">K4-K5</f>
-        <v>1039059651.8900318</v>
+        <v>983510965.5029583</v>
       </c>
       <c r="M4" s="25">
         <f t="shared" ref="M4:M6" si="4">L4/K5</f>
-        <v>7.8845920000000055E-2</v>
+        <v>7.8845919999999986E-2</v>
       </c>
       <c r="N4" s="23">
         <f t="shared" ref="N4:N6" si="5">(1+P4)*N5</f>
@@ -3903,34 +3903,34 @@
       </c>
       <c r="F5" s="22">
         <f t="shared" ref="F5:F8" si="7">G5*12</f>
-        <v>5868947.872798603</v>
+        <v>5555190.7711585239</v>
       </c>
       <c r="G5" s="22">
         <f>G6*(1+$H$25)</f>
-        <v>489078.98939988361</v>
+        <v>462932.56426321028</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>63</v>
       </c>
       <c r="I5" s="22">
         <f>F5-F6</f>
-        <v>418587.66403318383</v>
+        <v>396209.74296524376</v>
       </c>
       <c r="J5" s="24">
         <f t="shared" si="1"/>
-        <v>7.6799999999999938E-2</v>
+        <v>7.6799999999999966E-2</v>
       </c>
       <c r="K5" s="31">
         <f>N5*G5</f>
-        <v>13178356621.243446</v>
+        <v>12473834606.825039</v>
       </c>
       <c r="L5" s="31">
         <f t="shared" si="3"/>
-        <v>963121454.72082901</v>
+        <v>911632465.09099197</v>
       </c>
       <c r="M5" s="25">
         <f t="shared" si="4"/>
-        <v>7.884592E-2</v>
+        <v>7.8845920000000055E-2</v>
       </c>
       <c r="N5" s="23">
         <f t="shared" si="5"/>
@@ -3964,30 +3964,30 @@
       </c>
       <c r="F6" s="22">
         <f t="shared" si="7"/>
-        <v>5450360.2087654192</v>
+        <v>5158981.0281932801</v>
       </c>
       <c r="G6" s="22">
         <f>G7*(1+$H$25)</f>
-        <v>454196.68406378495</v>
+        <v>429915.08568277332</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>63</v>
       </c>
       <c r="I6" s="22">
         <f t="shared" ref="I6" si="8">F6-F7</f>
-        <v>388732.97179901879</v>
+        <v>367951.09859327972</v>
       </c>
       <c r="J6" s="24">
-        <f t="shared" si="1"/>
-        <v>7.6799999999999854E-2</v>
+        <f>I6/F7</f>
+        <v>7.6799999999999938E-2</v>
       </c>
       <c r="K6" s="31">
         <f t="shared" si="2"/>
-        <v>12215235166.522617</v>
+        <v>11562202141.734047</v>
       </c>
       <c r="L6" s="31">
         <f t="shared" si="3"/>
-        <v>892733092.71154213</v>
+        <v>845007102.67411613</v>
       </c>
       <c r="M6" s="25">
         <f t="shared" si="4"/>
@@ -4025,34 +4025,34 @@
       </c>
       <c r="F7" s="22">
         <f t="shared" si="7"/>
-        <v>5061627.2369664004</v>
+        <v>4791029.9296000004</v>
       </c>
       <c r="G7" s="22">
         <f>G8*(1+$H$25)</f>
-        <v>421802.26974720001</v>
+        <v>399252.49413333333</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>63</v>
       </c>
       <c r="I7" s="22">
         <f>F7-F8</f>
-        <v>361007.58896640036</v>
+        <v>257745.92960000038</v>
       </c>
       <c r="J7" s="24">
-        <f>I7/F8</f>
-        <v>7.6800000000000077E-2</v>
+        <f>H25</f>
+        <v>7.6799999999999993E-2</v>
       </c>
       <c r="K7" s="31">
         <f>N7*G7</f>
-        <v>11322502073.811075</v>
+        <v>10717195039.059931</v>
       </c>
       <c r="L7" s="31">
         <f>K7-K8</f>
-        <v>827488964.05108643</v>
+        <v>783250960.13165283</v>
       </c>
       <c r="M7" s="25">
         <f>L7/K8</f>
-        <v>7.8845919999999917E-2</v>
+        <v>7.8845920000000014E-2</v>
       </c>
       <c r="N7" s="23">
         <f>(1+P7)*N8</f>
@@ -4085,35 +4085,36 @@
         <v>3899499.8303999999</v>
       </c>
       <c r="F8" s="22">
-        <f t="shared" si="7"/>
-        <v>4700619.648</v>
+        <f>F9/(B9/12)</f>
+        <v>4533284</v>
       </c>
       <c r="G8" s="22">
-        <f>G10*(1+$H$25)</f>
-        <v>391718.304</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>63</v>
+        <f>((F8+F10)/2)/12</f>
+        <v>370776.83333333331</v>
+      </c>
+      <c r="H8" s="22">
+        <f>F8/12</f>
+        <v>377773.66666666669</v>
       </c>
       <c r="I8" s="22">
         <f>F8-F10</f>
-        <v>335259.64800000004</v>
-      </c>
-      <c r="J8" s="24">
-        <f>I8/F10</f>
-        <v>7.6800000000000007E-2</v>
+        <v>167924</v>
+      </c>
+      <c r="J8" s="48">
+        <f>(F8-F10)/F10</f>
+        <v>3.8467388714790988E-2</v>
       </c>
       <c r="K8" s="31">
         <f>N8*G8</f>
-        <v>10495013109.759989</v>
+        <v>9933944078.928278</v>
       </c>
       <c r="L8" s="31">
         <f>K8-K10</f>
-        <v>767013109.75998878</v>
+        <v>205944078.92827797</v>
       </c>
       <c r="M8" s="25">
         <f>L8/K10</f>
-        <v>7.8845919999998848E-2</v>
+        <v>2.1170238376673312E-2</v>
       </c>
       <c r="N8" s="23">
         <f>(1+P8)*N10</f>
@@ -4150,7 +4151,7 @@
       <c r="G9" s="22">
         <v>377773.66666666599</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="22">
         <v>377313</v>
       </c>
       <c r="I9" s="47" t="s">
@@ -4200,7 +4201,7 @@
       <c r="G10" s="22">
         <v>363780</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="22">
         <v>373961</v>
       </c>
       <c r="I10" s="22">
@@ -4250,7 +4251,7 @@
       <c r="G11" s="22">
         <v>324988.41666666599</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="22">
         <v>333060</v>
       </c>
       <c r="I11" s="22">
@@ -4300,7 +4301,7 @@
       <c r="G12" s="22">
         <v>294392.41666666599</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="22">
         <v>300026</v>
       </c>
       <c r="I12" s="22">
@@ -4350,7 +4351,7 @@
       <c r="G13" s="22">
         <v>279188.75</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="22">
         <v>281667</v>
       </c>
       <c r="I13" s="22">
@@ -4400,7 +4401,7 @@
       <c r="G14" s="22">
         <v>274331.91666666599</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="22">
         <v>272732</v>
       </c>
       <c r="I14" s="22">
@@ -4450,7 +4451,7 @@
       <c r="G15" s="22">
         <v>267329.33333333302</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="22">
         <v>274097</v>
       </c>
       <c r="I15" s="22">
@@ -4500,7 +4501,7 @@
       <c r="G16" s="22">
         <v>234696.41666666599</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="22">
         <v>242484</v>
       </c>
       <c r="I16" s="22">
@@ -4550,7 +4551,7 @@
       <c r="G17" s="22">
         <v>204796.83333333299</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="22">
         <v>211642</v>
       </c>
       <c r="I17" s="22">
@@ -4600,7 +4601,7 @@
       <c r="G18" s="22">
         <v>175045.33333333299</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="22">
         <v>182251</v>
       </c>
       <c r="I18" s="22">
@@ -4650,7 +4651,7 @@
       <c r="G19" s="22">
         <v>144672</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="22">
         <v>149436</v>
       </c>
       <c r="I19" s="22">
@@ -4700,7 +4701,7 @@
       <c r="G20" s="22">
         <v>135152.91666666599</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="22">
         <v>139204</v>
       </c>
       <c r="I20" s="47" t="s">
@@ -4733,12 +4734,12 @@
         <v>39</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Update on 8/29/2025 at 11:30am
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFCDEDA-A1CE-354A-ADA4-DFDE2C11F27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6BB189-5628-D84D-9128-2E680E9DB042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -524,6 +524,56 @@
   <si>
     <t>FY27-FY30 Growth Assumptions</t>
   </si>
+  <si>
+    <t>Enrollee Months Average Monthly % Growth</t>
+  </si>
+  <si>
+    <t>You can forecast projected enrollment and State spending by changing the inputs below:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enrollee Months Average Monthly % Growth:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For each row's respective fiscal year, this column calculates each month's enrollment delta percentage (i.e., </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[(that month's enrollment) - (previous month's enrollment)] / (previous month's enrollment))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and then reports the mean of those twelve percentages.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -539,7 +589,7 @@
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0,,_);[Red]\(&quot;$&quot;#,##0,,\)"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,6 +713,14 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1018,7 +1076,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1110,8 +1168,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1123,6 +1182,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="8" applyBorder="1" applyAlignment="1">
@@ -3715,65 +3777,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92772258-4AC4-6B47-AC5E-CDE7A2651A1C}">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" hidden="1" customWidth="1"/>
-    <col min="3" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="16" width="18" customWidth="1"/>
+    <col min="3" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="17" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:17" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-    </row>
-    <row r="2" spans="1:16" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="57" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+    </row>
+    <row r="2" spans="1:17" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="53" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="54" t="s">
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55" t="s">
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-    </row>
-    <row r="3" spans="1:16" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+    </row>
+    <row r="3" spans="1:17" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>19</v>
       </c>
@@ -3799,365 +3863,383 @@
         <v>47</v>
       </c>
       <c r="I3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="22">
-        <f t="shared" ref="C4:E7" si="0">C5*(1+$H$25)</f>
-        <v>907844.24037334672</v>
+        <f>C5*(1+K4)</f>
+        <v>873445.98163706099</v>
       </c>
       <c r="D4" s="22">
-        <f t="shared" si="0"/>
-        <v>169210.21776076485</v>
+        <f>D5*(1+K4)</f>
+        <v>162798.83506700632</v>
       </c>
       <c r="E4" s="22">
-        <f t="shared" si="0"/>
-        <v>5242628.6112954253</v>
+        <f>E5*(1+K4)</f>
+        <v>5043985.1795152854</v>
       </c>
       <c r="F4" s="22">
         <f>G4*12</f>
-        <v>5981829.4223834984</v>
+        <v>5983068.3203128288</v>
       </c>
       <c r="G4" s="22">
-        <f>G5*(1+$H$25)</f>
-        <v>498485.78519862483</v>
+        <f>G5*(1+K4)</f>
+        <v>498589.02669273573</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="22">
         <f>F4-F5</f>
-        <v>426638.65122497454</v>
-      </c>
-      <c r="J4" s="24">
-        <f t="shared" ref="J4:J6" si="1">I4/F5</f>
-        <v>7.6799999999999979E-2</v>
-      </c>
-      <c r="K4" s="31">
-        <f t="shared" ref="K4:K6" si="2">N4*G4</f>
-        <v>13457345572.327997</v>
+        <v>426727.01244430244</v>
+      </c>
+      <c r="K4" s="24">
+        <f>M25</f>
+        <v>7.6799999999999993E-2</v>
       </c>
       <c r="L4" s="31">
-        <f t="shared" ref="L4:L6" si="3">K4-K5</f>
-        <v>983510965.5029583</v>
-      </c>
-      <c r="M4" s="25">
-        <f t="shared" ref="M4:M6" si="4">L4/K5</f>
-        <v>7.8845919999999986E-2</v>
-      </c>
-      <c r="N4" s="23">
-        <f t="shared" ref="N4:N6" si="5">(1+P4)*N5</f>
+        <f>O4*G4</f>
+        <v>13460132725.953852</v>
+      </c>
+      <c r="M4" s="31">
+        <f>L4-L5</f>
+        <v>983714660.66251373</v>
+      </c>
+      <c r="N4" s="25">
+        <f>M4/L5</f>
+        <v>7.8845919999999847E-2</v>
+      </c>
+      <c r="O4" s="23">
+        <f>(1+Q4)*O5</f>
         <v>26996.447986908657</v>
       </c>
-      <c r="O4" s="23">
-        <f t="shared" ref="O4:O6" si="6">N4-N5</f>
+      <c r="P4" s="23">
+        <f>O4-O5</f>
         <v>51.195978815376293</v>
       </c>
-      <c r="P4" s="24">
-        <f>$H$27</f>
+      <c r="Q4" s="24">
+        <f>M26</f>
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="22">
-        <f t="shared" si="0"/>
-        <v>843094.57686974993</v>
+        <f>C6*(1+K5)</f>
+        <v>811149.68576993037</v>
       </c>
       <c r="D5" s="22">
-        <f t="shared" si="0"/>
-        <v>157141.73269016051</v>
+        <f>D6*(1+K5)</f>
+        <v>151187.6254336983</v>
       </c>
       <c r="E5" s="22">
-        <f t="shared" si="0"/>
-        <v>4868711.5632386934</v>
+        <f>E6*(1+K5)</f>
+        <v>4684235.8650773456</v>
       </c>
       <c r="F5" s="22">
-        <f t="shared" ref="F5:F8" si="7">G5*12</f>
-        <v>5555190.7711585239</v>
+        <f t="shared" ref="F5:F7" si="0">G5*12</f>
+        <v>5556341.3078685263</v>
       </c>
       <c r="G5" s="22">
-        <f>G6*(1+$H$25)</f>
-        <v>462932.56426321028</v>
+        <f>G6*(1+K5)</f>
+        <v>463028.44232237717</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="22">
         <f>F5-F6</f>
-        <v>396209.74296524376</v>
-      </c>
-      <c r="J5" s="24">
-        <f t="shared" si="1"/>
-        <v>7.6799999999999966E-2</v>
-      </c>
-      <c r="K5" s="31">
-        <f>N5*G5</f>
-        <v>12473834606.825039</v>
+        <v>396291.80204708595</v>
+      </c>
+      <c r="K5" s="24">
+        <f>L25</f>
+        <v>7.6799999999999993E-2</v>
       </c>
       <c r="L5" s="31">
-        <f t="shared" si="3"/>
-        <v>911632465.09099197</v>
-      </c>
-      <c r="M5" s="25">
-        <f t="shared" si="4"/>
-        <v>7.8845920000000055E-2</v>
-      </c>
-      <c r="N5" s="23">
-        <f t="shared" si="5"/>
+        <f>O5*G5</f>
+        <v>12476418065.291338</v>
+      </c>
+      <c r="M5" s="31">
+        <f t="shared" ref="M5:M6" si="1">L5-L6</f>
+        <v>911821273.47945595</v>
+      </c>
+      <c r="N5" s="25">
+        <f t="shared" ref="N5:N6" si="2">M5/L6</f>
+        <v>7.8845919999999972E-2</v>
+      </c>
+      <c r="O5" s="23">
+        <f t="shared" ref="O5:O6" si="3">(1+Q5)*O6</f>
         <v>26945.252008093281</v>
       </c>
-      <c r="O5" s="23">
-        <f t="shared" si="6"/>
+      <c r="P5" s="23">
+        <f t="shared" ref="P5:P6" si="4">O5-O6</f>
         <v>51.098890922625287</v>
       </c>
-      <c r="P5" s="24">
-        <f>$H$27</f>
+      <c r="Q5" s="24">
+        <f>L26</f>
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="22">
-        <f t="shared" si="0"/>
-        <v>782963.01715244236</v>
+        <f>C7*(1+K6)</f>
+        <v>753296.51353076741</v>
       </c>
       <c r="D6" s="22">
-        <f t="shared" si="0"/>
-        <v>145934.00138387864</v>
+        <f>D7*(1+K6)</f>
+        <v>140404.55556621312</v>
       </c>
       <c r="E6" s="22">
-        <f t="shared" si="0"/>
-        <v>4521463.1902290983</v>
+        <f>E7*(1+K6)</f>
+        <v>4350144.7484002095</v>
       </c>
       <c r="F6" s="22">
-        <f t="shared" si="7"/>
-        <v>5158981.0281932801</v>
+        <f>G6*12</f>
+        <v>5160049.5058214404</v>
       </c>
       <c r="G6" s="22">
-        <f>G7*(1+$H$25)</f>
-        <v>429915.08568277332</v>
+        <f>G7*(1+K6)</f>
+        <v>430004.12548511999</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="22">
-        <f t="shared" ref="I6" si="8">F6-F7</f>
-        <v>367951.09859327972</v>
-      </c>
-      <c r="J6" s="24">
-        <f>I6/F7</f>
-        <v>7.6799999999999938E-2</v>
-      </c>
-      <c r="K6" s="31">
+      <c r="I6" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="22">
+        <f>F6-F7</f>
+        <v>368027.30502144061</v>
+      </c>
+      <c r="K6" s="24">
+        <f>K25</f>
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="L6" s="31">
+        <f t="shared" ref="L6" si="5">O6*G6</f>
+        <v>11564596791.811882</v>
+      </c>
+      <c r="M6" s="31">
+        <f t="shared" si="1"/>
+        <v>845182112.26998711</v>
+      </c>
+      <c r="N6" s="25">
         <f t="shared" si="2"/>
-        <v>11562202141.734047</v>
-      </c>
-      <c r="L6" s="31">
+        <v>7.8845920000000111E-2</v>
+      </c>
+      <c r="O6" s="23">
         <f t="shared" si="3"/>
-        <v>845007102.67411613</v>
-      </c>
-      <c r="M6" s="25">
+        <v>26894.153117170656</v>
+      </c>
+      <c r="P6" s="23">
         <f t="shared" si="4"/>
-        <v>7.884592E-2</v>
-      </c>
-      <c r="N6" s="23">
-        <f t="shared" si="5"/>
-        <v>26894.153117170656</v>
-      </c>
-      <c r="O6" s="23">
-        <f t="shared" si="6"/>
         <v>51.001987147046748</v>
       </c>
-      <c r="P6" s="24">
-        <f>$H$27</f>
+      <c r="Q6" s="24">
+        <f>K26</f>
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="22">
+        <f>C8*(1+K7)</f>
+        <v>699569.57051520003</v>
+      </c>
+      <c r="D7" s="22">
+        <f>D8*(1+K7)</f>
+        <v>130390.5605184</v>
+      </c>
+      <c r="E7" s="22">
+        <f>E8*(1+K7)</f>
+        <v>4039881.8242943999</v>
+      </c>
+      <c r="F7" s="22">
         <f t="shared" si="0"/>
-        <v>727120.18680576002</v>
-      </c>
-      <c r="D7" s="22">
-        <f t="shared" si="0"/>
-        <v>135525.63278592</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="0"/>
-        <v>4198981.4173747199</v>
-      </c>
-      <c r="F7" s="22">
-        <f t="shared" si="7"/>
-        <v>4791029.9296000004</v>
+        <v>4792022.2007999998</v>
       </c>
       <c r="G7" s="22">
-        <f>G8*(1+$H$25)</f>
-        <v>399252.49413333333</v>
+        <f>G8*(1+K7)</f>
+        <v>399335.18339999998</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="22">
         <f>F7-F8</f>
-        <v>257745.92960000038</v>
-      </c>
-      <c r="J7" s="24">
-        <f>H25</f>
+        <v>256895.20079999976</v>
+      </c>
+      <c r="K7" s="24">
+        <f>J25</f>
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="K7" s="31">
-        <f>N7*G7</f>
-        <v>10717195039.059931</v>
-      </c>
       <c r="L7" s="31">
-        <f>K7-K8</f>
-        <v>783250960.13165283</v>
-      </c>
-      <c r="M7" s="25">
-        <f>L7/K8</f>
-        <v>7.8845920000000014E-2</v>
-      </c>
-      <c r="N7" s="23">
-        <f>(1+P7)*N8</f>
+        <f>O7*G7</f>
+        <v>10719414679.541895</v>
+      </c>
+      <c r="M7" s="31">
+        <f>L7-L8</f>
+        <v>783413179.40006256</v>
+      </c>
+      <c r="N7" s="25">
+        <f>M7/L8</f>
+        <v>7.8845919999999972E-2</v>
+      </c>
+      <c r="O7" s="23">
+        <f>(1+Q7)*O8</f>
         <v>26843.151130023609</v>
       </c>
-      <c r="O7" s="23">
-        <f>N7-N8</f>
+      <c r="P7" s="23">
+        <f>O7-O8</f>
         <v>50.905267139478383</v>
       </c>
-      <c r="P7" s="24">
-        <f>$H$27</f>
+      <c r="Q7" s="24">
+        <f>J26</f>
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>71</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22">
-        <f>C10*(1+$H$25)</f>
-        <v>675260.20319999999</v>
+        <f>C10*(1+K8)</f>
+        <v>649674.56400000001</v>
       </c>
       <c r="D8" s="22">
-        <f t="shared" ref="D8" si="9">D10*(1+$H$25)</f>
-        <v>125859.61439999999</v>
+        <f>D10*(1+K8)</f>
+        <v>121090.788</v>
       </c>
       <c r="E8" s="22">
-        <f>E10*(1+$H$25)</f>
-        <v>3899499.8303999999</v>
+        <f>E10*(1+K8)</f>
+        <v>3751747.608</v>
       </c>
       <c r="F8" s="22">
         <f>F9/(B9/12)</f>
-        <v>4533284</v>
+        <v>4535127</v>
       </c>
       <c r="G8" s="22">
         <f>((F8+F10)/2)/12</f>
-        <v>370776.83333333331</v>
+        <v>370853.625</v>
       </c>
       <c r="H8" s="22">
         <f>F8/12</f>
-        <v>377773.66666666669</v>
-      </c>
-      <c r="I8" s="22">
+        <v>377927.25</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="22">
         <f>F8-F10</f>
-        <v>167924</v>
-      </c>
-      <c r="J8" s="48">
-        <f>(F8-F10)/F10</f>
-        <v>3.8467388714790988E-2</v>
-      </c>
-      <c r="K8" s="31">
-        <f>N8*G8</f>
-        <v>9933944078.928278</v>
+        <v>169767</v>
+      </c>
+      <c r="K8" s="24">
+        <f>I25</f>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="L8" s="31">
-        <f>K8-K10</f>
-        <v>205944078.92827797</v>
-      </c>
-      <c r="M8" s="25">
-        <f>L8/K10</f>
-        <v>2.1170238376673312E-2</v>
-      </c>
-      <c r="N8" s="23">
-        <f>(1+P8)*N10</f>
+        <f>O8*G8</f>
+        <v>9936001500.1418324</v>
+      </c>
+      <c r="M8" s="31">
+        <f>L8-L10</f>
+        <v>208001500.14183235</v>
+      </c>
+      <c r="N8" s="25">
+        <f>M8/L10</f>
+        <v>2.1381733156027174E-2</v>
+      </c>
+      <c r="O8" s="23">
+        <f>(1+Q8)*O10</f>
         <v>26792.24586288413</v>
       </c>
-      <c r="O8" s="23">
-        <f>N8-N10</f>
+      <c r="P8" s="23">
+        <f>O8-O10</f>
         <v>50.808730551430926</v>
       </c>
-      <c r="P8" s="24">
-        <f>$H$27</f>
+      <c r="Q8" s="24">
+        <f>I26</f>
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="22">
-        <v>189988</v>
+        <v>257469</v>
       </c>
       <c r="D9" s="22">
-        <v>29261</v>
+        <v>38916</v>
       </c>
       <c r="E9" s="22">
-        <v>914072</v>
+        <v>1215324</v>
       </c>
       <c r="F9" s="22">
-        <v>1133321</v>
+        <v>1511709</v>
       </c>
       <c r="G9" s="22">
-        <v>377773.66666666599</v>
+        <v>377927.25</v>
       </c>
       <c r="H9" s="22">
-        <v>377313</v>
-      </c>
-      <c r="I9" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="26" t="s">
+        <v>378388</v>
+      </c>
+      <c r="I9" s="53">
+        <v>2.9577466746810001E-3</v>
+      </c>
+      <c r="J9" s="47" t="s">
         <v>63</v>
       </c>
       <c r="K9" s="26" t="s">
@@ -4178,8 +4260,11 @@
       <c r="P9" s="26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>69</v>
       </c>
@@ -4204,32 +4289,35 @@
       <c r="H10" s="22">
         <v>373961</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="53">
+        <v>1.06536426565819E-2</v>
+      </c>
+      <c r="J10" s="22">
         <v>465499</v>
       </c>
-      <c r="J10" s="48">
+      <c r="K10" s="48">
         <v>0.11936297216746899</v>
       </c>
-      <c r="K10" s="31">
+      <c r="L10" s="31">
         <v>9728000000</v>
       </c>
-      <c r="L10" s="31">
+      <c r="M10" s="31">
         <v>863000000</v>
       </c>
-      <c r="M10" s="25">
+      <c r="N10" s="25">
         <v>9.7349125775521697E-2</v>
       </c>
-      <c r="N10" s="23">
+      <c r="O10" s="23">
         <v>26741.4371323327</v>
       </c>
-      <c r="O10" s="23">
+      <c r="P10" s="23">
         <v>-536.45815675577899</v>
       </c>
-      <c r="P10" s="25">
+      <c r="Q10" s="25">
         <v>-1.9666405749800199E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>23</v>
       </c>
@@ -4254,32 +4342,35 @@
       <c r="H11" s="22">
         <v>333060</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="53">
+        <v>9.6832089430078806E-3</v>
+      </c>
+      <c r="J11" s="22">
         <v>367152</v>
       </c>
-      <c r="J11" s="48">
+      <c r="K11" s="48">
         <v>0.10392930750877</v>
       </c>
-      <c r="K11" s="31">
+      <c r="L11" s="31">
         <v>8865000000</v>
       </c>
-      <c r="L11" s="31">
+      <c r="M11" s="31">
         <v>1251000000</v>
       </c>
-      <c r="M11" s="25">
+      <c r="N11" s="25">
         <v>0.164302600472813</v>
       </c>
-      <c r="N11" s="23">
+      <c r="O11" s="23">
         <v>27277.895289088501</v>
       </c>
-      <c r="O11" s="23">
+      <c r="P11" s="23">
         <v>1414.45734387423</v>
       </c>
-      <c r="P11" s="25">
+      <c r="Q11" s="25">
         <v>5.4689455704629499E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>24</v>
       </c>
@@ -4304,32 +4395,35 @@
       <c r="H12" s="22">
         <v>300026</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="53">
+        <v>5.7563574810133604E-3</v>
+      </c>
+      <c r="J12" s="22">
         <v>182444</v>
       </c>
-      <c r="J12" s="48">
+      <c r="K12" s="48">
         <v>5.4456587762460498E-2</v>
       </c>
-      <c r="K12" s="31">
+      <c r="L12" s="31">
         <v>7614000000</v>
       </c>
-      <c r="L12" s="31">
+      <c r="M12" s="31">
         <v>-83000000</v>
       </c>
-      <c r="M12" s="25">
+      <c r="N12" s="25">
         <v>-1.07834221125113E-2</v>
       </c>
-      <c r="N12" s="23">
+      <c r="O12" s="23">
         <v>25863.437945214198</v>
       </c>
-      <c r="O12" s="23">
+      <c r="P12" s="23">
         <v>-1705.7244941748399</v>
       </c>
-      <c r="P12" s="25">
+      <c r="Q12" s="25">
         <v>-6.1870740466812603E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
@@ -4354,32 +4448,35 @@
       <c r="H13" s="22">
         <v>281667</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="53">
+        <v>2.7813959491820102E-3</v>
+      </c>
+      <c r="J13" s="22">
         <v>58282</v>
       </c>
-      <c r="J13" s="48">
+      <c r="K13" s="48">
         <v>1.7704222652425598E-2</v>
       </c>
-      <c r="K13" s="31">
+      <c r="L13" s="31">
         <v>7697000000</v>
       </c>
-      <c r="L13" s="31">
+      <c r="M13" s="31">
         <v>482000000</v>
       </c>
-      <c r="M13" s="25">
+      <c r="N13" s="25">
         <v>6.68052668052668E-2</v>
       </c>
-      <c r="N13" s="23">
+      <c r="O13" s="23">
         <v>27569.1624393891</v>
       </c>
-      <c r="O13" s="23">
+      <c r="P13" s="23">
         <v>1268.9051172826601</v>
       </c>
-      <c r="P13" s="25">
+      <c r="Q13" s="25">
         <v>4.8246870809742701E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>26</v>
       </c>
@@ -4404,32 +4501,35 @@
       <c r="H14" s="22">
         <v>272732</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="53">
+        <v>-2.4915131332300402E-4</v>
+      </c>
+      <c r="J14" s="22">
         <v>84031</v>
       </c>
-      <c r="J14" s="48">
+      <c r="K14" s="48">
         <v>2.61945939340738E-2</v>
       </c>
-      <c r="K14" s="31">
+      <c r="L14" s="31">
         <v>7215000000</v>
       </c>
-      <c r="L14" s="31">
+      <c r="M14" s="31">
         <v>-550000000</v>
       </c>
-      <c r="M14" s="25">
+      <c r="N14" s="25">
         <v>-7.0830650354153202E-2</v>
       </c>
-      <c r="N14" s="23">
+      <c r="O14" s="23">
         <v>26300.257322106401</v>
       </c>
-      <c r="O14" s="23">
+      <c r="P14" s="23">
         <v>-2746.3119532442902</v>
       </c>
-      <c r="P14" s="25">
+      <c r="Q14" s="25">
         <v>-9.4548582560999503E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>27</v>
       </c>
@@ -4454,32 +4554,35 @@
       <c r="H15" s="22">
         <v>274097</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="53">
+        <v>1.15463267044202E-2</v>
+      </c>
+      <c r="J15" s="22">
         <v>391595</v>
       </c>
-      <c r="J15" s="48">
+      <c r="K15" s="48">
         <v>0.13904309716417301</v>
       </c>
-      <c r="K15" s="31">
+      <c r="L15" s="31">
         <v>7765000000</v>
       </c>
-      <c r="L15" s="31">
+      <c r="M15" s="31">
         <v>1480000000</v>
       </c>
-      <c r="M15" s="25">
+      <c r="N15" s="25">
         <v>0.235481304693715</v>
       </c>
-      <c r="N15" s="23">
+      <c r="O15" s="23">
         <v>29046.569275350699</v>
       </c>
-      <c r="O15" s="23">
+      <c r="P15" s="23">
         <v>2267.2937786718799</v>
       </c>
-      <c r="P15" s="25">
+      <c r="Q15" s="25">
         <v>8.4665986536979806E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>28</v>
       </c>
@@ -4504,32 +4607,35 @@
       <c r="H16" s="22">
         <v>242484</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="53">
+        <v>1.2904331091802701E-2</v>
+      </c>
+      <c r="J16" s="22">
         <v>358795</v>
       </c>
-      <c r="J16" s="48">
+      <c r="K16" s="48">
         <v>0.14599631667481799</v>
       </c>
-      <c r="K16" s="31">
+      <c r="L16" s="31">
         <v>6285000000</v>
       </c>
-      <c r="L16" s="31">
+      <c r="M16" s="31">
         <v>473000000</v>
       </c>
-      <c r="M16" s="25">
+      <c r="N16" s="25">
         <v>8.1383344803853994E-2</v>
       </c>
-      <c r="N16" s="23">
+      <c r="O16" s="23">
         <v>26779.275496678802</v>
       </c>
-      <c r="O16" s="23">
+      <c r="P16" s="23">
         <v>-1600.0695615536299</v>
       </c>
-      <c r="P16" s="25">
+      <c r="Q16" s="25">
         <v>-5.6381483021204402E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>29</v>
       </c>
@@ -4554,32 +4660,35 @@
       <c r="H17" s="22">
         <v>211642</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="53">
+        <v>1.43963315484748E-2</v>
+      </c>
+      <c r="J17" s="22">
         <v>357018</v>
       </c>
-      <c r="J17" s="48">
+      <c r="K17" s="48">
         <v>0.16996454251850901</v>
       </c>
-      <c r="K17" s="31">
+      <c r="L17" s="31">
         <v>5812000000</v>
       </c>
-      <c r="L17" s="31">
+      <c r="M17" s="31">
         <v>1200000000</v>
       </c>
-      <c r="M17" s="25">
+      <c r="N17" s="25">
         <v>0.26019080659150001</v>
       </c>
-      <c r="N17" s="23">
+      <c r="O17" s="23">
         <v>28379.345058232499</v>
       </c>
-      <c r="O17" s="23">
+      <c r="P17" s="23">
         <v>2031.8845908488099</v>
       </c>
-      <c r="P17" s="25">
+      <c r="Q17" s="25">
         <v>7.7118802146573004E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>30</v>
       </c>
@@ -4604,32 +4713,35 @@
       <c r="H18" s="22">
         <v>182251</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="53">
+        <v>1.9703822998225699E-2</v>
+      </c>
+      <c r="J18" s="22">
         <v>364480</v>
       </c>
-      <c r="J18" s="48">
+      <c r="K18" s="48">
         <v>0.20994617709946101</v>
       </c>
-      <c r="K18" s="31">
+      <c r="L18" s="31">
         <v>4612000000</v>
       </c>
-      <c r="L18" s="31">
+      <c r="M18" s="31">
         <v>819000000</v>
       </c>
-      <c r="M18" s="25">
+      <c r="N18" s="25">
         <v>0.21592407065647201</v>
       </c>
-      <c r="N18" s="23">
+      <c r="O18" s="23">
         <v>26347.4604673836</v>
       </c>
-      <c r="O18" s="23">
+      <c r="P18" s="23">
         <v>129.533017704412</v>
       </c>
-      <c r="P18" s="25">
+      <c r="Q18" s="25">
         <v>4.9406276660513403E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>31</v>
       </c>
@@ -4654,32 +4766,35 @@
       <c r="H19" s="22">
         <v>149436</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="53">
+        <v>7.2741559352159204E-3</v>
+      </c>
+      <c r="J19" s="22">
         <v>114229</v>
       </c>
-      <c r="J19" s="48">
+      <c r="K19" s="48">
         <v>7.0431948996044602E-2</v>
       </c>
-      <c r="K19" s="31">
+      <c r="L19" s="31">
         <v>3793000000</v>
       </c>
-      <c r="L19" s="49">
+      <c r="M19" s="49">
         <v>322000000</v>
       </c>
-      <c r="M19" s="25">
+      <c r="N19" s="25">
         <v>9.2768654566407302E-2</v>
       </c>
-      <c r="N19" s="23">
+      <c r="O19" s="23">
         <v>26217.927449679199</v>
       </c>
-      <c r="O19" s="23">
+      <c r="P19" s="23">
         <v>535.90677556630897</v>
       </c>
-      <c r="P19" s="25">
+      <c r="Q19" s="25">
         <v>2.08670019531015E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>32</v>
       </c>
@@ -4704,91 +4819,139 @@
       <c r="H20" s="22">
         <v>139204</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="53">
+        <v>1.09662297978985E-2</v>
+      </c>
+      <c r="J20" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="48" t="s">
+      <c r="K20" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="31">
+      <c r="L20" s="31">
         <v>3471000000</v>
       </c>
-      <c r="L20" s="49" t="s">
+      <c r="M20" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="M20" s="48" t="s">
+      <c r="N20" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="N20" s="23">
+      <c r="O20" s="23">
         <v>25682.0206741129</v>
       </c>
-      <c r="O20" s="26" t="s">
+      <c r="P20" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="P20" s="48" t="s">
+      <c r="Q20" s="48" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="I22" s="27" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>_xlfn.CONCAT("(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
-        <v>(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = 3.</v>
-      </c>
-      <c r="H24" t="s">
+        <v>(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = 4.</v>
+      </c>
+      <c r="I24" s="54" t="str">
+        <f>LEFT(A8,4)</f>
+        <v>FY26</v>
+      </c>
+      <c r="J24" s="54" t="str">
+        <f>LEFT(A7,4)</f>
+        <v>FY27</v>
+      </c>
+      <c r="K24" s="54" t="str">
+        <f>LEFT(A6,4)</f>
+        <v>FY28</v>
+      </c>
+      <c r="L24" s="54" t="str">
+        <f>LEFT(A5,4)</f>
+        <v>FY29</v>
+      </c>
+      <c r="M24" s="54" t="str">
+        <f>LEFT(A4,4)</f>
+        <v>FY30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>_xlfn.CONCAT("(3) FY26 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(J26*100,2),"%")</f>
+        <v>(3) FY26 full-year spending estimate is based an assumption of per capita spending growth = 0.19%</v>
+      </c>
+      <c r="H25" s="54" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="str">
-        <f>_xlfn.CONCAT("(3) FY26 full-year spending estimate is based an assumption of per capita spending growth = ",ROUND(H27*100,2),"%")</f>
-        <v>(3) FY26 full-year spending estimate is based an assumption of per capita spending growth = 0.19%</v>
-      </c>
-      <c r="H25" s="11">
+      <c r="I25" s="11">
+        <f>0.003*12</f>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="J25" s="11">
         <v>7.6799999999999993E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H26" t="s">
+      <c r="K25" s="11">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="L25" s="11">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="M25" s="11">
+        <v>7.6799999999999993E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="H26" s="54" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="H27" s="11">
+      <c r="I26" s="11">
         <v>1.9E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="11">
+        <v>1.9E-3</v>
+      </c>
+      <c r="K26" s="11">
+        <v>1.9E-3</v>
+      </c>
+      <c r="L26" s="11">
+        <v>1.9E-3</v>
+      </c>
+      <c r="M26" s="11">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -4800,54 +4963,59 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:P20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:Q20">
     <sortCondition descending="1" ref="A9:A20"/>
   </sortState>
   <mergeCells count="5">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -4861,7 +5029,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4882,20 +5050,20 @@
   <sheetData>
     <row r="1" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P2" s="67" t="s">
+      <c r="P2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="69"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="71"/>
     </row>
     <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P3" s="70" t="s">
+      <c r="P3" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="72"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="74"/>
     </row>
     <row r="4" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P4" s="13"/>
@@ -4904,12 +5072,12 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="64" t="s">
+      <c r="P5" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="66"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="68"/>
     </row>
     <row r="6" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P6" s="6" t="s">
@@ -4951,12 +5119,12 @@
       <c r="S9" s="14"/>
     </row>
     <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P10" s="64" t="s">
+      <c r="P10" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="66"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="67"/>
+      <c r="S10" s="68"/>
     </row>
     <row r="11" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P11" s="6" t="s">
@@ -4998,12 +5166,12 @@
       <c r="S14" s="14"/>
     </row>
     <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="61" t="s">
+      <c r="P15" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="Q15" s="62"/>
-      <c r="R15" s="62"/>
-      <c r="S15" s="63"/>
+      <c r="Q15" s="64"/>
+      <c r="R15" s="64"/>
+      <c r="S15" s="65"/>
     </row>
     <row r="16" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="P16" s="36" t="s">
@@ -5014,18 +5182,18 @@
       <c r="S16" s="14"/>
     </row>
     <row r="17" spans="16:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P17" s="58" t="s">
+      <c r="P17" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="59"/>
-      <c r="S17" s="60"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="61"/>
+      <c r="S17" s="62"/>
     </row>
     <row r="18" spans="16:19" x14ac:dyDescent="0.2">
-      <c r="P18" s="58"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="62"/>
     </row>
     <row r="19" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P19" s="15" t="s">

</xml_diff>

<commit_message>
Update on 12/10/2025 at 8:58pm
</commit_message>
<xml_diff>
--- a/mltc_enrollment_vs_spending.xlsx
+++ b/mltc_enrollment_vs_spending.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6BB189-5628-D84D-9128-2E680E9DB042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D409B22C-498D-9945-A8C4-488AB2DAD481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1225,6 +1225,25 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
@@ -1253,25 +1272,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3475,16 +3475,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:G12" xr:uid="{8D7DA177-DADE-4043-9ADA-6081AE770CD2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5930A738-8B59-6A4E-919B-090BCB11A0AA}" name="Data  Type"/>
     <tableColumn id="2" xr3:uid="{BC5DD464-CE62-C145-9541-0E916FE9BF25}" name="Fiscal Year"/>
-    <tableColumn id="3" xr3:uid="{1858EE94-CA04-2649-B52D-6343C025BC1C}" name="State Spending" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{2A994CA5-E802-1241-A0A7-341CFD69AFD6}" name="Average Annual Enrollment" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{410693AE-0DD9-F340-BB48-7F49D2049665}" name="Average Annual Enrollment Change %" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{4B0D0AC8-F08E-7544-9AF6-BC3DA742F6F2}" name="Average Annual Spending per Enrollee" dataDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{F8434FAD-6E36-6344-9152-D139B9351C1D}" name="Average Annual Spending per Enrollee Annual Change %" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1858EE94-CA04-2649-B52D-6343C025BC1C}" name="State Spending" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{2A994CA5-E802-1241-A0A7-341CFD69AFD6}" name="Average Annual Enrollment" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{410693AE-0DD9-F340-BB48-7F49D2049665}" name="Average Annual Enrollment Change %" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{4B0D0AC8-F08E-7544-9AF6-BC3DA742F6F2}" name="Average Annual Spending per Enrollee" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{F8434FAD-6E36-6344-9152-D139B9351C1D}" name="Average Annual Spending per Enrollee Annual Change %" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3779,14 +3779,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92772258-4AC4-6B47-AC5E-CDE7A2651A1C}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="11" width="14.6640625" customWidth="1"/>
     <col min="12" max="17" width="18" customWidth="1"/>
   </cols>
@@ -3909,11 +3909,11 @@
       </c>
       <c r="F4" s="22">
         <f>G4*12</f>
-        <v>5983068.3203128288</v>
+        <v>5983828.0227792207</v>
       </c>
       <c r="G4" s="22">
         <f>G5*(1+K4)</f>
-        <v>498589.02669273573</v>
+        <v>498652.33523160173</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>63</v>
@@ -3923,7 +3923,7 @@
       </c>
       <c r="J4" s="22">
         <f>F4-F5</f>
-        <v>426727.01244430244</v>
+        <v>426781.19627548661</v>
       </c>
       <c r="K4" s="24">
         <f>M25</f>
@@ -3931,15 +3931,15 @@
       </c>
       <c r="L4" s="31">
         <f>O4*G4</f>
-        <v>13460132725.953852</v>
+        <v>13461841831.630476</v>
       </c>
       <c r="M4" s="31">
         <f>L4-L5</f>
-        <v>983714660.66251373</v>
+        <v>983839568.22063065</v>
       </c>
       <c r="N4" s="25">
         <f>M4/L5</f>
-        <v>7.8845919999999847E-2</v>
+        <v>7.8845919999999931E-2</v>
       </c>
       <c r="O4" s="23">
         <f>(1+Q4)*O5</f>
@@ -3973,11 +3973,11 @@
       </c>
       <c r="F5" s="22">
         <f t="shared" ref="F5:F7" si="0">G5*12</f>
-        <v>5556341.3078685263</v>
+        <v>5557046.8265037341</v>
       </c>
       <c r="G5" s="22">
         <f>G6*(1+K5)</f>
-        <v>463028.44232237717</v>
+        <v>463087.23554197786</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>63</v>
@@ -3987,7 +3987,7 @@
       </c>
       <c r="J5" s="22">
         <f>F5-F6</f>
-        <v>396291.80204708595</v>
+        <v>396342.12135539204</v>
       </c>
       <c r="K5" s="24">
         <f>L25</f>
@@ -3995,15 +3995,15 @@
       </c>
       <c r="L5" s="31">
         <f>O5*G5</f>
-        <v>12476418065.291338</v>
+        <v>12478002263.409845</v>
       </c>
       <c r="M5" s="31">
         <f t="shared" ref="M5:M6" si="1">L5-L6</f>
-        <v>911821273.47945595</v>
+        <v>911937052.34630013</v>
       </c>
       <c r="N5" s="25">
         <f t="shared" ref="N5:N6" si="2">M5/L6</f>
-        <v>7.8845919999999972E-2</v>
+        <v>7.8845920000000069E-2</v>
       </c>
       <c r="O5" s="23">
         <f t="shared" ref="O5:O6" si="3">(1+Q5)*O6</f>
@@ -4037,11 +4037,11 @@
       </c>
       <c r="F6" s="22">
         <f>G6*12</f>
-        <v>5160049.5058214404</v>
+        <v>5160704.7051483421</v>
       </c>
       <c r="G6" s="22">
         <f>G7*(1+K6)</f>
-        <v>430004.12548511999</v>
+        <v>430058.72542902851</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>63</v>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="J6" s="22">
         <f>F6-F7</f>
-        <v>368027.30502144061</v>
+        <v>368074.035434057</v>
       </c>
       <c r="K6" s="24">
         <f>K25</f>
@@ -4059,15 +4059,15 @@
       </c>
       <c r="L6" s="31">
         <f t="shared" ref="L6" si="5">O6*G6</f>
-        <v>11564596791.811882</v>
+        <v>11566065211.063545</v>
       </c>
       <c r="M6" s="31">
         <f t="shared" si="1"/>
-        <v>845182112.26998711</v>
+        <v>845289429.60297585</v>
       </c>
       <c r="N6" s="25">
         <f t="shared" si="2"/>
-        <v>7.8845920000000111E-2</v>
+        <v>7.8845919999999847E-2</v>
       </c>
       <c r="O6" s="23">
         <f t="shared" si="3"/>
@@ -4101,11 +4101,11 @@
       </c>
       <c r="F7" s="22">
         <f t="shared" si="0"/>
-        <v>4792022.2007999998</v>
+        <v>4792630.6697142851</v>
       </c>
       <c r="G7" s="22">
         <f>G8*(1+K7)</f>
-        <v>399335.18339999998</v>
+        <v>399385.88914285711</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>63</v>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="J7" s="22">
         <f>F7-F8</f>
-        <v>256895.20079999976</v>
+        <v>256373.52685714234</v>
       </c>
       <c r="K7" s="24">
         <f>J25</f>
@@ -4123,15 +4123,15 @@
       </c>
       <c r="L7" s="31">
         <f>O7*G7</f>
-        <v>10719414679.541895</v>
+        <v>10720775781.460569</v>
       </c>
       <c r="M7" s="31">
         <f>L7-L8</f>
-        <v>783413179.40006256</v>
+        <v>783512653.59837341</v>
       </c>
       <c r="N7" s="25">
         <f>M7/L8</f>
-        <v>7.8845919999999972E-2</v>
+        <v>7.8845920000000097E-2</v>
       </c>
       <c r="O7" s="23">
         <f>(1+Q7)*O8</f>
@@ -4165,22 +4165,22 @@
       </c>
       <c r="F8" s="22">
         <f>F9/(B9/12)</f>
-        <v>4535127</v>
+        <v>4536257.1428571427</v>
       </c>
       <c r="G8" s="22">
         <f>((F8+F10)/2)/12</f>
-        <v>370853.625</v>
+        <v>370900.71428571426</v>
       </c>
       <c r="H8" s="22">
         <f>F8/12</f>
-        <v>377927.25</v>
+        <v>378021.42857142858</v>
       </c>
       <c r="I8" s="26" t="s">
         <v>63</v>
       </c>
       <c r="J8" s="22">
         <f>F8-F10</f>
-        <v>169767</v>
+        <v>170897.14285714272</v>
       </c>
       <c r="K8" s="24">
         <f>I25</f>
@@ -4188,15 +4188,15 @@
       </c>
       <c r="L8" s="31">
         <f>O8*G8</f>
-        <v>9936001500.1418324</v>
+        <v>9937263127.862196</v>
       </c>
       <c r="M8" s="31">
         <f>L8-L10</f>
-        <v>208001500.14183235</v>
+        <v>209263127.86219597</v>
       </c>
       <c r="N8" s="25">
         <f>M8/L10</f>
-        <v>2.1381733156027174E-2</v>
+        <v>2.1511423505571132E-2</v>
       </c>
       <c r="O8" s="23">
         <f>(1+Q8)*O10</f>
@@ -4216,28 +4216,28 @@
         <v>68</v>
       </c>
       <c r="B9" s="21">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="22">
-        <v>257469</v>
+        <v>469889</v>
       </c>
       <c r="D9" s="22">
-        <v>38916</v>
+        <v>67873</v>
       </c>
       <c r="E9" s="22">
-        <v>1215324</v>
+        <v>2108388</v>
       </c>
       <c r="F9" s="22">
-        <v>1511709</v>
+        <v>2646150</v>
       </c>
       <c r="G9" s="22">
-        <v>377927.25</v>
+        <v>378021.428571428</v>
       </c>
       <c r="H9" s="22">
-        <v>378388</v>
+        <v>377032</v>
       </c>
       <c r="I9" s="53">
-        <v>2.9577466746810001E-3</v>
+        <v>1.1790586541767299E-3</v>
       </c>
       <c r="J9" s="47" t="s">
         <v>63</v>
@@ -4868,7 +4868,7 @@
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>_xlfn.CONCAT("(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = ",B9,".")</f>
-        <v>(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = 4.</v>
+        <v>(2) Full-year Enrollment 2026 Estimate Represents YTD annualized. Months in YTD = 7.</v>
       </c>
       <c r="I24" s="54" t="str">
         <f>LEFT(A8,4)</f>
@@ -5353,8 +5353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EC6393-3785-8B4D-BC33-531ADF13ED6E}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>